<commit_message>
worked to compute SHARED, OFFSET constraints - needs testing
</commit_message>
<xml_diff>
--- a/data/Times_to_Transfer_Stations.xlsx
+++ b/data/Times_to_Transfer_Stations.xlsx
@@ -4,13 +4,17 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25725"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="6240" yWindow="0" windowWidth="25360" windowHeight="15660" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="2560" yWindow="0" windowWidth="25600" windowHeight="15860" tabRatio="564" firstSheet="3" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Station_Time_Calculations" sheetId="1" r:id="rId1"/>
     <sheet name="Attempt_2" sheetId="2" r:id="rId2"/>
     <sheet name="Times_to_Stations" sheetId="3" r:id="rId3"/>
-    <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
+    <sheet name="Times_Transpose" sheetId="4" r:id="rId4"/>
+    <sheet name="Shared_Lines_Calc" sheetId="5" r:id="rId5"/>
+    <sheet name="Shared_Lines" sheetId="6" r:id="rId6"/>
+    <sheet name="Shared_Lines_Offset" sheetId="7" r:id="rId7"/>
+    <sheet name="shared_test_sat_morn" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -22,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="674" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="905" uniqueCount="109">
   <si>
     <t>-</t>
   </si>
@@ -277,6 +281,78 @@
   </si>
   <si>
     <t>*above values copied to "Times_to_Stations" tab</t>
+  </si>
+  <si>
+    <t>Shared Lines</t>
+  </si>
+  <si>
+    <t>Line 1</t>
+  </si>
+  <si>
+    <t>Line 2</t>
+  </si>
+  <si>
+    <t>Line 1 time_to</t>
+  </si>
+  <si>
+    <t>Line 2 time_to</t>
+  </si>
+  <si>
+    <t>Line_Dir_1</t>
+  </si>
+  <si>
+    <t>Line_Dir_2</t>
+  </si>
+  <si>
+    <t>Offset</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Blue_pos </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Blue_neg </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Green_pos </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Green_neg </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Orange_pos </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Orange_neg </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Red_pos </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Red_neg </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Silver_pos </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Silver_neg </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yellow_pos </t>
+  </si>
+  <si>
+    <t>Yellow_neg :=</t>
+  </si>
+  <si>
+    <t xml:space="preserve">param OFFSET: </t>
+  </si>
+  <si>
+    <t>Start</t>
+  </si>
+  <si>
+    <t>Shared Only</t>
+  </si>
+  <si>
+    <t>Violated Shared</t>
   </si>
 </sst>
 </file>
@@ -337,8 +413,60 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="85">
+  <cellStyleXfs count="137">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -429,7 +557,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="85">
+  <cellStyles count="137">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -472,6 +600,32 @@
     <cellStyle name="Followed Hyperlink" xfId="80" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="82" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="84" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="86" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="88" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="90" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="92" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="94" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="96" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="98" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="100" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="102" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="104" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="106" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="108" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="110" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="112" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="114" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="116" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="118" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="120" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="122" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="124" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="126" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="128" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="130" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="132" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="134" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="136" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -514,6 +668,32 @@
     <cellStyle name="Hyperlink" xfId="79" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="81" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="83" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="85" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="87" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="89" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="91" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="93" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="95" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="97" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="99" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="101" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="103" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="105" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="107" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="109" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="111" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="113" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="115" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="117" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="119" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="121" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="123" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="125" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="127" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="129" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="131" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="133" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="135" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -3659,35 +3839,35 @@
         <v>23</v>
       </c>
       <c r="F65" t="str">
-        <f>F53</f>
+        <f t="shared" ref="F65:M65" si="8">F53</f>
         <v>-</v>
       </c>
       <c r="G65" t="str">
-        <f>G53</f>
+        <f t="shared" si="8"/>
         <v>-</v>
       </c>
       <c r="H65" t="str">
-        <f>H53</f>
+        <f t="shared" si="8"/>
         <v>-</v>
       </c>
       <c r="I65" t="str">
-        <f>I53</f>
+        <f t="shared" si="8"/>
         <v>-</v>
       </c>
       <c r="J65">
-        <f>J53</f>
+        <f t="shared" si="8"/>
         <v>36</v>
       </c>
       <c r="K65">
-        <f>K53</f>
+        <f t="shared" si="8"/>
         <v>35</v>
       </c>
       <c r="L65" t="str">
-        <f>L53</f>
+        <f t="shared" si="8"/>
         <v>-</v>
       </c>
       <c r="M65" t="str">
-        <f>M53</f>
+        <f t="shared" si="8"/>
         <v>-</v>
       </c>
     </row>
@@ -3712,7 +3892,7 @@
   <dimension ref="A1:M10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -4142,8 +4322,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -4561,6 +4741,3960 @@
         <v>16</v>
       </c>
       <c r="J13" t="s">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M23"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D13" sqref="D13:H23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:13">
+      <c r="A1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H1" t="s">
+        <v>19</v>
+      </c>
+      <c r="I1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J1" t="s">
+        <v>17</v>
+      </c>
+      <c r="K1" t="s">
+        <v>16</v>
+      </c>
+      <c r="L1" t="s">
+        <v>15</v>
+      </c>
+      <c r="M1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13">
+      <c r="A2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>34</v>
+      </c>
+      <c r="D2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>31</v>
+      </c>
+      <c r="F2">
+        <v>29</v>
+      </c>
+      <c r="G2">
+        <v>39</v>
+      </c>
+      <c r="H2" t="s">
+        <v>0</v>
+      </c>
+      <c r="I2">
+        <v>27</v>
+      </c>
+      <c r="J2" t="s">
+        <v>0</v>
+      </c>
+      <c r="K2">
+        <v>23</v>
+      </c>
+      <c r="L2">
+        <v>28</v>
+      </c>
+      <c r="M2">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13">
+      <c r="A3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>3</v>
+      </c>
+      <c r="E3">
+        <v>11</v>
+      </c>
+      <c r="F3" t="s">
+        <v>0</v>
+      </c>
+      <c r="G3" t="s">
+        <v>0</v>
+      </c>
+      <c r="H3" t="s">
+        <v>0</v>
+      </c>
+      <c r="I3" t="s">
+        <v>0</v>
+      </c>
+      <c r="J3">
+        <v>48</v>
+      </c>
+      <c r="K3">
+        <v>37</v>
+      </c>
+      <c r="L3" t="s">
+        <v>0</v>
+      </c>
+      <c r="M3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13">
+      <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4">
+        <v>22</v>
+      </c>
+      <c r="C4">
+        <v>36</v>
+      </c>
+      <c r="D4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E4" t="s">
+        <v>0</v>
+      </c>
+      <c r="F4" t="s">
+        <v>0</v>
+      </c>
+      <c r="G4" t="s">
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <v>25</v>
+      </c>
+      <c r="I4">
+        <v>25</v>
+      </c>
+      <c r="J4">
+        <v>40</v>
+      </c>
+      <c r="K4" t="s">
+        <v>0</v>
+      </c>
+      <c r="L4" t="s">
+        <v>0</v>
+      </c>
+      <c r="M4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13">
+      <c r="A5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5">
+        <v>19</v>
+      </c>
+      <c r="C5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>22</v>
+      </c>
+      <c r="E5">
+        <v>36</v>
+      </c>
+      <c r="F5">
+        <v>34</v>
+      </c>
+      <c r="G5">
+        <v>44</v>
+      </c>
+      <c r="H5">
+        <v>28</v>
+      </c>
+      <c r="I5" t="s">
+        <v>0</v>
+      </c>
+      <c r="J5">
+        <v>31</v>
+      </c>
+      <c r="K5">
+        <v>18</v>
+      </c>
+      <c r="L5">
+        <v>23</v>
+      </c>
+      <c r="M5">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13">
+      <c r="A6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6">
+        <v>35</v>
+      </c>
+      <c r="C6">
+        <v>22</v>
+      </c>
+      <c r="D6" t="s">
+        <v>0</v>
+      </c>
+      <c r="E6" t="s">
+        <v>0</v>
+      </c>
+      <c r="F6" t="s">
+        <v>0</v>
+      </c>
+      <c r="G6" t="s">
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <v>12</v>
+      </c>
+      <c r="I6">
+        <v>14</v>
+      </c>
+      <c r="J6">
+        <v>10</v>
+      </c>
+      <c r="K6" t="s">
+        <v>0</v>
+      </c>
+      <c r="L6" t="s">
+        <v>0</v>
+      </c>
+      <c r="M6" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13">
+      <c r="A7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" t="s">
+        <v>0</v>
+      </c>
+      <c r="C7" t="s">
+        <v>0</v>
+      </c>
+      <c r="D7" t="s">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>24</v>
+      </c>
+      <c r="F7">
+        <v>22</v>
+      </c>
+      <c r="G7">
+        <v>32</v>
+      </c>
+      <c r="H7" t="s">
+        <v>0</v>
+      </c>
+      <c r="I7" t="s">
+        <v>0</v>
+      </c>
+      <c r="J7" t="s">
+        <v>0</v>
+      </c>
+      <c r="K7">
+        <v>30</v>
+      </c>
+      <c r="L7">
+        <v>35</v>
+      </c>
+      <c r="M7">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13">
+      <c r="A8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>0</v>
+      </c>
+      <c r="C8" t="s">
+        <v>0</v>
+      </c>
+      <c r="D8" t="s">
+        <v>0</v>
+      </c>
+      <c r="E8" t="s">
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <v>10</v>
+      </c>
+      <c r="G8">
+        <v>22</v>
+      </c>
+      <c r="H8" t="s">
+        <v>0</v>
+      </c>
+      <c r="I8" t="s">
+        <v>0</v>
+      </c>
+      <c r="J8" t="s">
+        <v>0</v>
+      </c>
+      <c r="K8" t="s">
+        <v>0</v>
+      </c>
+      <c r="L8">
+        <v>46</v>
+      </c>
+      <c r="M8">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13">
+      <c r="A9" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9" t="s">
+        <v>0</v>
+      </c>
+      <c r="C9" t="s">
+        <v>0</v>
+      </c>
+      <c r="D9" t="s">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>45</v>
+      </c>
+      <c r="F9">
+        <v>30</v>
+      </c>
+      <c r="G9">
+        <v>53</v>
+      </c>
+      <c r="H9" t="s">
+        <v>0</v>
+      </c>
+      <c r="I9" t="s">
+        <v>0</v>
+      </c>
+      <c r="J9" t="s">
+        <v>0</v>
+      </c>
+      <c r="K9">
+        <v>9</v>
+      </c>
+      <c r="L9">
+        <v>14</v>
+      </c>
+      <c r="M9">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13">
+      <c r="A10" t="s">
+        <v>3</v>
+      </c>
+      <c r="B10" t="s">
+        <v>0</v>
+      </c>
+      <c r="C10" t="s">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>15</v>
+      </c>
+      <c r="E10">
+        <v>23</v>
+      </c>
+      <c r="F10" t="s">
+        <v>0</v>
+      </c>
+      <c r="G10" t="s">
+        <v>0</v>
+      </c>
+      <c r="H10" t="s">
+        <v>0</v>
+      </c>
+      <c r="I10" t="s">
+        <v>0</v>
+      </c>
+      <c r="J10">
+        <v>36</v>
+      </c>
+      <c r="K10">
+        <v>35</v>
+      </c>
+      <c r="L10" t="s">
+        <v>0</v>
+      </c>
+      <c r="M10" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13">
+      <c r="A12" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13">
+      <c r="A13" t="s">
+        <v>86</v>
+      </c>
+      <c r="B13" t="s">
+        <v>87</v>
+      </c>
+      <c r="C13" t="s">
+        <v>40</v>
+      </c>
+      <c r="D13" t="s">
+        <v>90</v>
+      </c>
+      <c r="E13" t="s">
+        <v>91</v>
+      </c>
+      <c r="F13" t="s">
+        <v>88</v>
+      </c>
+      <c r="G13" t="s">
+        <v>89</v>
+      </c>
+      <c r="H13" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13">
+      <c r="A14" t="s">
+        <v>46</v>
+      </c>
+      <c r="B14" t="s">
+        <v>47</v>
+      </c>
+      <c r="C14" t="s">
+        <v>3</v>
+      </c>
+      <c r="D14" t="str">
+        <f>CONCATENATE(A14,"_pos")</f>
+        <v>Blue_pos</v>
+      </c>
+      <c r="E14" t="str">
+        <f>CONCATENATE(B14,"_pos")</f>
+        <v>Yellow_pos</v>
+      </c>
+      <c r="F14">
+        <v>23</v>
+      </c>
+      <c r="G14">
+        <v>15</v>
+      </c>
+      <c r="H14">
+        <f>F14-G14</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13">
+      <c r="A15" t="s">
+        <v>46</v>
+      </c>
+      <c r="B15" t="s">
+        <v>44</v>
+      </c>
+      <c r="C15" t="s">
+        <v>7</v>
+      </c>
+      <c r="D15" t="str">
+        <f t="shared" ref="D15:D18" si="0">CONCATENATE(A15,"_pos")</f>
+        <v>Blue_pos</v>
+      </c>
+      <c r="E15" t="str">
+        <f t="shared" ref="E15:E18" si="1">CONCATENATE(B15,"_pos")</f>
+        <v>Orange_pos</v>
+      </c>
+      <c r="F15">
+        <v>24</v>
+      </c>
+      <c r="G15">
+        <v>22</v>
+      </c>
+      <c r="H15">
+        <f t="shared" ref="H15:H23" si="2">F15-G15</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13">
+      <c r="A16" t="s">
+        <v>46</v>
+      </c>
+      <c r="B16" t="s">
+        <v>42</v>
+      </c>
+      <c r="C16" t="s">
+        <v>7</v>
+      </c>
+      <c r="D16" t="str">
+        <f t="shared" si="0"/>
+        <v>Blue_pos</v>
+      </c>
+      <c r="E16" t="str">
+        <f t="shared" si="1"/>
+        <v>Silver_pos</v>
+      </c>
+      <c r="F16">
+        <v>24</v>
+      </c>
+      <c r="G16">
+        <v>32</v>
+      </c>
+      <c r="H16">
+        <f t="shared" si="2"/>
+        <v>-8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8">
+      <c r="A17" t="s">
+        <v>50</v>
+      </c>
+      <c r="B17" t="s">
+        <v>47</v>
+      </c>
+      <c r="C17" t="s">
+        <v>9</v>
+      </c>
+      <c r="D17" t="str">
+        <f t="shared" si="0"/>
+        <v>Green_pos</v>
+      </c>
+      <c r="E17" t="str">
+        <f t="shared" si="1"/>
+        <v>Yellow_pos</v>
+      </c>
+      <c r="F17">
+        <v>19</v>
+      </c>
+      <c r="G17">
+        <v>22</v>
+      </c>
+      <c r="H17">
+        <f t="shared" si="2"/>
+        <v>-3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8">
+      <c r="A18" t="s">
+        <v>44</v>
+      </c>
+      <c r="B18" t="s">
+        <v>42</v>
+      </c>
+      <c r="C18" t="s">
+        <v>7</v>
+      </c>
+      <c r="D18" t="str">
+        <f t="shared" si="0"/>
+        <v>Orange_pos</v>
+      </c>
+      <c r="E18" t="str">
+        <f t="shared" si="1"/>
+        <v>Silver_pos</v>
+      </c>
+      <c r="F18">
+        <v>22</v>
+      </c>
+      <c r="G18">
+        <v>32</v>
+      </c>
+      <c r="H18">
+        <f t="shared" si="2"/>
+        <v>-10</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8">
+      <c r="C19" t="s">
+        <v>3</v>
+      </c>
+      <c r="D19" t="str">
+        <f>CONCATENATE(A14,"_neg")</f>
+        <v>Blue_neg</v>
+      </c>
+      <c r="E19" t="str">
+        <f>CONCATENATE(B14,"_neg")</f>
+        <v>Yellow_neg</v>
+      </c>
+      <c r="F19">
+        <v>35</v>
+      </c>
+      <c r="G19">
+        <v>36</v>
+      </c>
+      <c r="H19">
+        <f t="shared" si="2"/>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8">
+      <c r="C20" t="s">
+        <v>7</v>
+      </c>
+      <c r="D20" t="str">
+        <f t="shared" ref="D20:E20" si="3">CONCATENATE(A15,"_neg")</f>
+        <v>Blue_neg</v>
+      </c>
+      <c r="E20" t="str">
+        <f t="shared" si="3"/>
+        <v>Orange_neg</v>
+      </c>
+      <c r="F20">
+        <v>30</v>
+      </c>
+      <c r="G20">
+        <v>35</v>
+      </c>
+      <c r="H20">
+        <f t="shared" si="2"/>
+        <v>-5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8">
+      <c r="C21" t="s">
+        <v>7</v>
+      </c>
+      <c r="D21" t="str">
+        <f t="shared" ref="D21:E21" si="4">CONCATENATE(A16,"_neg")</f>
+        <v>Blue_neg</v>
+      </c>
+      <c r="E21" t="str">
+        <f t="shared" si="4"/>
+        <v>Silver_neg</v>
+      </c>
+      <c r="F21">
+        <v>30</v>
+      </c>
+      <c r="G21">
+        <v>37</v>
+      </c>
+      <c r="H21">
+        <f t="shared" si="2"/>
+        <v>-7</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8">
+      <c r="C22" t="s">
+        <v>9</v>
+      </c>
+      <c r="D22" t="str">
+        <f t="shared" ref="D22:E22" si="5">CONCATENATE(A17,"_neg")</f>
+        <v>Green_neg</v>
+      </c>
+      <c r="E22" t="str">
+        <f t="shared" si="5"/>
+        <v>Yellow_neg</v>
+      </c>
+      <c r="F22">
+        <v>28</v>
+      </c>
+      <c r="G22">
+        <v>31</v>
+      </c>
+      <c r="H22">
+        <f t="shared" si="2"/>
+        <v>-3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8">
+      <c r="C23" t="s">
+        <v>7</v>
+      </c>
+      <c r="D23" t="str">
+        <f t="shared" ref="D23:E23" si="6">CONCATENATE(A18,"_neg")</f>
+        <v>Orange_neg</v>
+      </c>
+      <c r="E23" t="str">
+        <f t="shared" si="6"/>
+        <v>Silver_neg</v>
+      </c>
+      <c r="F23">
+        <v>35</v>
+      </c>
+      <c r="G23">
+        <v>37</v>
+      </c>
+      <c r="H23">
+        <f t="shared" si="2"/>
+        <v>-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G21" sqref="G21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:13">
+      <c r="B1" t="s">
+        <v>93</v>
+      </c>
+      <c r="C1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D1" t="s">
+        <v>95</v>
+      </c>
+      <c r="E1" t="s">
+        <v>96</v>
+      </c>
+      <c r="F1" t="s">
+        <v>97</v>
+      </c>
+      <c r="G1" t="s">
+        <v>98</v>
+      </c>
+      <c r="H1" t="s">
+        <v>99</v>
+      </c>
+      <c r="I1" t="s">
+        <v>100</v>
+      </c>
+      <c r="J1" t="s">
+        <v>101</v>
+      </c>
+      <c r="K1" t="s">
+        <v>102</v>
+      </c>
+      <c r="L1" t="s">
+        <v>103</v>
+      </c>
+      <c r="M1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13">
+      <c r="A2" t="s">
+        <v>93</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+      <c r="I2">
+        <v>0</v>
+      </c>
+      <c r="J2">
+        <v>1</v>
+      </c>
+      <c r="K2">
+        <v>0</v>
+      </c>
+      <c r="L2">
+        <v>1</v>
+      </c>
+      <c r="M2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13">
+      <c r="A3" t="s">
+        <v>94</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>1</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="I3">
+        <v>0</v>
+      </c>
+      <c r="J3">
+        <v>0</v>
+      </c>
+      <c r="K3">
+        <v>1</v>
+      </c>
+      <c r="L3">
+        <v>0</v>
+      </c>
+      <c r="M3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13">
+      <c r="A4" t="s">
+        <v>95</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4">
+        <v>0</v>
+      </c>
+      <c r="J4">
+        <v>0</v>
+      </c>
+      <c r="K4">
+        <v>0</v>
+      </c>
+      <c r="L4">
+        <v>1</v>
+      </c>
+      <c r="M4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13">
+      <c r="A5" t="s">
+        <v>96</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <v>0</v>
+      </c>
+      <c r="J5">
+        <v>0</v>
+      </c>
+      <c r="K5">
+        <v>0</v>
+      </c>
+      <c r="L5">
+        <v>0</v>
+      </c>
+      <c r="M5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13">
+      <c r="A6" t="s">
+        <v>97</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6">
+        <v>0</v>
+      </c>
+      <c r="J6">
+        <v>1</v>
+      </c>
+      <c r="K6">
+        <v>0</v>
+      </c>
+      <c r="L6">
+        <v>0</v>
+      </c>
+      <c r="M6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13">
+      <c r="A7" t="s">
+        <v>98</v>
+      </c>
+      <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="I7">
+        <v>0</v>
+      </c>
+      <c r="J7">
+        <v>0</v>
+      </c>
+      <c r="K7">
+        <v>1</v>
+      </c>
+      <c r="L7">
+        <v>0</v>
+      </c>
+      <c r="M7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13">
+      <c r="A8" t="s">
+        <v>99</v>
+      </c>
+      <c r="B8">
+        <v>0</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="I8">
+        <v>0</v>
+      </c>
+      <c r="J8">
+        <v>0</v>
+      </c>
+      <c r="K8">
+        <v>0</v>
+      </c>
+      <c r="L8">
+        <v>0</v>
+      </c>
+      <c r="M8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13">
+      <c r="A9" t="s">
+        <v>100</v>
+      </c>
+      <c r="B9">
+        <v>0</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
+      <c r="I9">
+        <v>0</v>
+      </c>
+      <c r="J9">
+        <v>0</v>
+      </c>
+      <c r="K9">
+        <v>0</v>
+      </c>
+      <c r="L9">
+        <v>0</v>
+      </c>
+      <c r="M9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13">
+      <c r="A10" t="s">
+        <v>101</v>
+      </c>
+      <c r="B10">
+        <v>0</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
+      <c r="I10">
+        <v>0</v>
+      </c>
+      <c r="J10">
+        <v>0</v>
+      </c>
+      <c r="K10">
+        <v>0</v>
+      </c>
+      <c r="L10">
+        <v>0</v>
+      </c>
+      <c r="M10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13">
+      <c r="A11" t="s">
+        <v>102</v>
+      </c>
+      <c r="B11">
+        <v>0</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+      <c r="I11">
+        <v>0</v>
+      </c>
+      <c r="J11">
+        <v>0</v>
+      </c>
+      <c r="K11">
+        <v>0</v>
+      </c>
+      <c r="L11">
+        <v>0</v>
+      </c>
+      <c r="M11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13">
+      <c r="A12" t="s">
+        <v>103</v>
+      </c>
+      <c r="B12">
+        <v>0</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
+      <c r="G12">
+        <v>0</v>
+      </c>
+      <c r="H12">
+        <v>0</v>
+      </c>
+      <c r="I12">
+        <v>0</v>
+      </c>
+      <c r="J12">
+        <v>0</v>
+      </c>
+      <c r="K12">
+        <v>0</v>
+      </c>
+      <c r="L12">
+        <v>0</v>
+      </c>
+      <c r="M12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13">
+      <c r="A13" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13">
+        <v>0</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
+      <c r="F13">
+        <v>0</v>
+      </c>
+      <c r="G13">
+        <v>0</v>
+      </c>
+      <c r="H13">
+        <v>0</v>
+      </c>
+      <c r="I13">
+        <v>0</v>
+      </c>
+      <c r="J13">
+        <v>0</v>
+      </c>
+      <c r="K13">
+        <v>0</v>
+      </c>
+      <c r="L13">
+        <v>0</v>
+      </c>
+      <c r="M13">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H23" sqref="H23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:13">
+      <c r="A1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B1" t="s">
+        <v>93</v>
+      </c>
+      <c r="C1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D1" t="s">
+        <v>95</v>
+      </c>
+      <c r="E1" t="s">
+        <v>96</v>
+      </c>
+      <c r="F1" t="s">
+        <v>97</v>
+      </c>
+      <c r="G1" t="s">
+        <v>98</v>
+      </c>
+      <c r="H1" t="s">
+        <v>99</v>
+      </c>
+      <c r="I1" t="s">
+        <v>100</v>
+      </c>
+      <c r="J1" t="s">
+        <v>101</v>
+      </c>
+      <c r="K1" t="s">
+        <v>102</v>
+      </c>
+      <c r="L1" t="s">
+        <v>103</v>
+      </c>
+      <c r="M1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13">
+      <c r="A2" t="s">
+        <v>93</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>2</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+      <c r="I2">
+        <v>0</v>
+      </c>
+      <c r="J2">
+        <v>-8</v>
+      </c>
+      <c r="K2">
+        <v>0</v>
+      </c>
+      <c r="L2">
+        <v>8</v>
+      </c>
+      <c r="M2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13">
+      <c r="A3" t="s">
+        <v>94</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>-5</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="I3">
+        <v>0</v>
+      </c>
+      <c r="J3">
+        <v>0</v>
+      </c>
+      <c r="K3">
+        <v>-7</v>
+      </c>
+      <c r="L3">
+        <v>0</v>
+      </c>
+      <c r="M3">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13">
+      <c r="A4" t="s">
+        <v>95</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4">
+        <v>0</v>
+      </c>
+      <c r="J4">
+        <v>0</v>
+      </c>
+      <c r="K4">
+        <v>0</v>
+      </c>
+      <c r="L4">
+        <v>-3</v>
+      </c>
+      <c r="M4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13">
+      <c r="A5" t="s">
+        <v>96</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <v>0</v>
+      </c>
+      <c r="J5">
+        <v>0</v>
+      </c>
+      <c r="K5">
+        <v>0</v>
+      </c>
+      <c r="L5">
+        <v>0</v>
+      </c>
+      <c r="M5">
+        <v>-3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13">
+      <c r="A6" t="s">
+        <v>97</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6">
+        <v>0</v>
+      </c>
+      <c r="J6">
+        <v>-10</v>
+      </c>
+      <c r="K6">
+        <v>0</v>
+      </c>
+      <c r="L6">
+        <v>0</v>
+      </c>
+      <c r="M6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13">
+      <c r="A7" t="s">
+        <v>98</v>
+      </c>
+      <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="I7">
+        <v>0</v>
+      </c>
+      <c r="J7">
+        <v>0</v>
+      </c>
+      <c r="K7">
+        <v>-2</v>
+      </c>
+      <c r="L7">
+        <v>0</v>
+      </c>
+      <c r="M7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13">
+      <c r="A8" t="s">
+        <v>99</v>
+      </c>
+      <c r="B8">
+        <v>0</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="I8">
+        <v>0</v>
+      </c>
+      <c r="J8">
+        <v>0</v>
+      </c>
+      <c r="K8">
+        <v>0</v>
+      </c>
+      <c r="L8">
+        <v>0</v>
+      </c>
+      <c r="M8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13">
+      <c r="A9" t="s">
+        <v>100</v>
+      </c>
+      <c r="B9">
+        <v>0</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
+      <c r="I9">
+        <v>0</v>
+      </c>
+      <c r="J9">
+        <v>0</v>
+      </c>
+      <c r="K9">
+        <v>0</v>
+      </c>
+      <c r="L9">
+        <v>0</v>
+      </c>
+      <c r="M9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13">
+      <c r="A10" t="s">
+        <v>101</v>
+      </c>
+      <c r="B10">
+        <v>0</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
+      <c r="I10">
+        <v>0</v>
+      </c>
+      <c r="J10">
+        <v>0</v>
+      </c>
+      <c r="K10">
+        <v>0</v>
+      </c>
+      <c r="L10">
+        <v>0</v>
+      </c>
+      <c r="M10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13">
+      <c r="A11" t="s">
+        <v>102</v>
+      </c>
+      <c r="B11">
+        <v>0</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+      <c r="I11">
+        <v>0</v>
+      </c>
+      <c r="J11">
+        <v>0</v>
+      </c>
+      <c r="K11">
+        <v>0</v>
+      </c>
+      <c r="L11">
+        <v>0</v>
+      </c>
+      <c r="M11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13">
+      <c r="A12" t="s">
+        <v>103</v>
+      </c>
+      <c r="B12">
+        <v>0</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
+      <c r="G12">
+        <v>0</v>
+      </c>
+      <c r="H12">
+        <v>0</v>
+      </c>
+      <c r="I12">
+        <v>0</v>
+      </c>
+      <c r="J12">
+        <v>0</v>
+      </c>
+      <c r="K12">
+        <v>0</v>
+      </c>
+      <c r="L12">
+        <v>0</v>
+      </c>
+      <c r="M12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13">
+      <c r="A13" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13">
+        <v>0</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
+      <c r="F13">
+        <v>0</v>
+      </c>
+      <c r="G13">
+        <v>0</v>
+      </c>
+      <c r="H13">
+        <v>0</v>
+      </c>
+      <c r="I13">
+        <v>0</v>
+      </c>
+      <c r="J13">
+        <v>0</v>
+      </c>
+      <c r="K13">
+        <v>0</v>
+      </c>
+      <c r="L13">
+        <v>0</v>
+      </c>
+      <c r="M13">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:N42"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O16" sqref="O16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:14">
+      <c r="C1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14">
+      <c r="A2" s="1"/>
+      <c r="B2" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="C2" s="1">
+        <v>4</v>
+      </c>
+      <c r="D2" s="1">
+        <v>11</v>
+      </c>
+      <c r="E2" s="1">
+        <v>5</v>
+      </c>
+      <c r="F2" s="1">
+        <v>5</v>
+      </c>
+      <c r="G2" s="1">
+        <v>6</v>
+      </c>
+      <c r="H2" s="1">
+        <v>9</v>
+      </c>
+      <c r="I2" s="1">
+        <v>2</v>
+      </c>
+      <c r="J2" s="1">
+        <v>9</v>
+      </c>
+      <c r="K2" s="1">
+        <v>8</v>
+      </c>
+      <c r="L2" s="1">
+        <v>7</v>
+      </c>
+      <c r="M2" s="1">
+        <v>11</v>
+      </c>
+      <c r="N2" s="1">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14">
+      <c r="A3" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" s="1">
+        <v>4</v>
+      </c>
+      <c r="C3">
+        <f>$B3-C$2</f>
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <f t="shared" ref="D3:N14" si="0">$B3-D$2</f>
+        <v>-7</v>
+      </c>
+      <c r="E3">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+      <c r="F3">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+      <c r="G3">
+        <f t="shared" si="0"/>
+        <v>-2</v>
+      </c>
+      <c r="H3">
+        <f t="shared" si="0"/>
+        <v>-5</v>
+      </c>
+      <c r="I3">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="J3">
+        <f t="shared" si="0"/>
+        <v>-5</v>
+      </c>
+      <c r="K3">
+        <f t="shared" si="0"/>
+        <v>-4</v>
+      </c>
+      <c r="L3">
+        <f t="shared" si="0"/>
+        <v>-3</v>
+      </c>
+      <c r="M3">
+        <f t="shared" si="0"/>
+        <v>-7</v>
+      </c>
+      <c r="N3">
+        <f t="shared" si="0"/>
+        <v>-5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14">
+      <c r="A4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="1">
+        <v>11</v>
+      </c>
+      <c r="C4">
+        <f t="shared" ref="C4:C14" si="1">$B4-C$2</f>
+        <v>7</v>
+      </c>
+      <c r="D4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="F4">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="G4">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="H4">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="I4">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="J4">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="K4">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="L4">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="M4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N4">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14">
+      <c r="A5" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B5" s="1">
+        <v>5</v>
+      </c>
+      <c r="C5">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <f t="shared" si="0"/>
+        <v>-6</v>
+      </c>
+      <c r="E5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+      <c r="H5">
+        <f t="shared" si="0"/>
+        <v>-4</v>
+      </c>
+      <c r="I5">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="J5">
+        <f t="shared" si="0"/>
+        <v>-4</v>
+      </c>
+      <c r="K5">
+        <f t="shared" si="0"/>
+        <v>-3</v>
+      </c>
+      <c r="L5">
+        <f t="shared" si="0"/>
+        <v>-2</v>
+      </c>
+      <c r="M5">
+        <f t="shared" si="0"/>
+        <v>-6</v>
+      </c>
+      <c r="N5">
+        <f t="shared" si="0"/>
+        <v>-4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14">
+      <c r="A6" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B6" s="1">
+        <v>5</v>
+      </c>
+      <c r="C6">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <f t="shared" si="0"/>
+        <v>-6</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+      <c r="H6">
+        <f t="shared" si="0"/>
+        <v>-4</v>
+      </c>
+      <c r="I6">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="J6">
+        <f t="shared" si="0"/>
+        <v>-4</v>
+      </c>
+      <c r="K6">
+        <f t="shared" si="0"/>
+        <v>-3</v>
+      </c>
+      <c r="L6">
+        <f t="shared" si="0"/>
+        <v>-2</v>
+      </c>
+      <c r="M6">
+        <f t="shared" si="0"/>
+        <v>-6</v>
+      </c>
+      <c r="N6">
+        <f t="shared" si="0"/>
+        <v>-4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14">
+      <c r="A7" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B7" s="1">
+        <v>6</v>
+      </c>
+      <c r="C7">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="D7">
+        <f t="shared" si="0"/>
+        <v>-5</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="F7">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="G7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H7">
+        <f t="shared" si="0"/>
+        <v>-3</v>
+      </c>
+      <c r="I7">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="J7">
+        <f t="shared" si="0"/>
+        <v>-3</v>
+      </c>
+      <c r="K7">
+        <f t="shared" si="0"/>
+        <v>-2</v>
+      </c>
+      <c r="L7">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+      <c r="M7">
+        <f t="shared" si="0"/>
+        <v>-5</v>
+      </c>
+      <c r="N7">
+        <f t="shared" si="0"/>
+        <v>-3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14">
+      <c r="A8" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="B8" s="1">
+        <v>9</v>
+      </c>
+      <c r="C8">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="D8">
+        <f t="shared" si="0"/>
+        <v>-2</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="F8">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="G8">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="H8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I8">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="J8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K8">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="L8">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="M8">
+        <f t="shared" si="0"/>
+        <v>-2</v>
+      </c>
+      <c r="N8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14">
+      <c r="A9" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B9" s="1">
+        <v>2</v>
+      </c>
+      <c r="C9">
+        <f t="shared" si="1"/>
+        <v>-2</v>
+      </c>
+      <c r="D9">
+        <f t="shared" si="0"/>
+        <v>-9</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="0"/>
+        <v>-3</v>
+      </c>
+      <c r="F9">
+        <f t="shared" si="0"/>
+        <v>-3</v>
+      </c>
+      <c r="G9">
+        <f t="shared" si="0"/>
+        <v>-4</v>
+      </c>
+      <c r="H9">
+        <f t="shared" si="0"/>
+        <v>-7</v>
+      </c>
+      <c r="I9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J9">
+        <f t="shared" si="0"/>
+        <v>-7</v>
+      </c>
+      <c r="K9">
+        <f t="shared" si="0"/>
+        <v>-6</v>
+      </c>
+      <c r="L9">
+        <f t="shared" si="0"/>
+        <v>-5</v>
+      </c>
+      <c r="M9">
+        <f t="shared" si="0"/>
+        <v>-9</v>
+      </c>
+      <c r="N9">
+        <f t="shared" si="0"/>
+        <v>-7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14">
+      <c r="A10" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B10" s="1">
+        <v>9</v>
+      </c>
+      <c r="C10">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="D10">
+        <f t="shared" si="0"/>
+        <v>-2</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="F10">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="G10">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="H10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I10">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="J10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K10">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="L10">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="M10">
+        <f t="shared" si="0"/>
+        <v>-2</v>
+      </c>
+      <c r="N10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14">
+      <c r="A11" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="B11" s="1">
+        <v>8</v>
+      </c>
+      <c r="C11">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="D11">
+        <f t="shared" si="0"/>
+        <v>-3</v>
+      </c>
+      <c r="E11">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="F11">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="G11">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="H11">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+      <c r="I11">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="J11">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+      <c r="K11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L11">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="M11">
+        <f t="shared" si="0"/>
+        <v>-3</v>
+      </c>
+      <c r="N11">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14">
+      <c r="A12" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="B12" s="1">
+        <v>7</v>
+      </c>
+      <c r="C12">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="D12">
+        <f t="shared" si="0"/>
+        <v>-4</v>
+      </c>
+      <c r="E12">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="F12">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="G12">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="H12">
+        <f t="shared" si="0"/>
+        <v>-2</v>
+      </c>
+      <c r="I12">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="J12">
+        <f t="shared" si="0"/>
+        <v>-2</v>
+      </c>
+      <c r="K12">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+      <c r="L12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M12">
+        <f t="shared" si="0"/>
+        <v>-4</v>
+      </c>
+      <c r="N12">
+        <f t="shared" si="0"/>
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14">
+      <c r="A13" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="B13" s="1">
+        <v>11</v>
+      </c>
+      <c r="C13">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="D13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E13">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="F13">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="G13">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="H13">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="I13">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="J13">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="K13">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="L13">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="M13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N13">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14">
+      <c r="A14" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B14" s="1">
+        <v>9</v>
+      </c>
+      <c r="C14">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="D14">
+        <f t="shared" si="0"/>
+        <v>-2</v>
+      </c>
+      <c r="E14">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="F14">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="G14">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="H14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I14">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="J14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K14">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="L14">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="M14">
+        <f t="shared" si="0"/>
+        <v>-2</v>
+      </c>
+      <c r="N14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14">
+      <c r="B16" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="J16" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="K16" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="L16" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="M16" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="N16" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="17" spans="2:14">
+      <c r="B17" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C17">
+        <f>C3*Shared_Lines!B2</f>
+        <v>0</v>
+      </c>
+      <c r="D17">
+        <f>D3*Shared_Lines!C2</f>
+        <v>0</v>
+      </c>
+      <c r="E17">
+        <f>E3*Shared_Lines!D2</f>
+        <v>0</v>
+      </c>
+      <c r="F17">
+        <f>F3*Shared_Lines!E2</f>
+        <v>0</v>
+      </c>
+      <c r="G17">
+        <f>G3*Shared_Lines!F2</f>
+        <v>-2</v>
+      </c>
+      <c r="H17">
+        <f>H3*Shared_Lines!G2</f>
+        <v>0</v>
+      </c>
+      <c r="I17">
+        <f>I3*Shared_Lines!H2</f>
+        <v>0</v>
+      </c>
+      <c r="J17">
+        <f>J3*Shared_Lines!I2</f>
+        <v>0</v>
+      </c>
+      <c r="K17">
+        <f>K3*Shared_Lines!J2</f>
+        <v>-4</v>
+      </c>
+      <c r="L17">
+        <f>L3*Shared_Lines!K2</f>
+        <v>0</v>
+      </c>
+      <c r="M17">
+        <f>M3*Shared_Lines!L2</f>
+        <v>-7</v>
+      </c>
+      <c r="N17">
+        <f>N3*Shared_Lines!M2</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="2:14">
+      <c r="B18" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C18">
+        <f>C4*Shared_Lines!B3</f>
+        <v>0</v>
+      </c>
+      <c r="D18">
+        <f>D4*Shared_Lines!C3</f>
+        <v>0</v>
+      </c>
+      <c r="E18">
+        <f>E4*Shared_Lines!D3</f>
+        <v>0</v>
+      </c>
+      <c r="F18">
+        <f>F4*Shared_Lines!E3</f>
+        <v>0</v>
+      </c>
+      <c r="G18">
+        <f>G4*Shared_Lines!F3</f>
+        <v>0</v>
+      </c>
+      <c r="H18">
+        <f>H4*Shared_Lines!G3</f>
+        <v>2</v>
+      </c>
+      <c r="I18">
+        <f>I4*Shared_Lines!H3</f>
+        <v>0</v>
+      </c>
+      <c r="J18">
+        <f>J4*Shared_Lines!I3</f>
+        <v>0</v>
+      </c>
+      <c r="K18">
+        <f>K4*Shared_Lines!J3</f>
+        <v>0</v>
+      </c>
+      <c r="L18">
+        <f>L4*Shared_Lines!K3</f>
+        <v>4</v>
+      </c>
+      <c r="M18">
+        <f>M4*Shared_Lines!L3</f>
+        <v>0</v>
+      </c>
+      <c r="N18">
+        <f>N4*Shared_Lines!M3</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="2:14">
+      <c r="B19" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="C19">
+        <f>C5*Shared_Lines!B4</f>
+        <v>0</v>
+      </c>
+      <c r="D19">
+        <f>D5*Shared_Lines!C4</f>
+        <v>0</v>
+      </c>
+      <c r="E19">
+        <f>E5*Shared_Lines!D4</f>
+        <v>0</v>
+      </c>
+      <c r="F19">
+        <f>F5*Shared_Lines!E4</f>
+        <v>0</v>
+      </c>
+      <c r="G19">
+        <f>G5*Shared_Lines!F4</f>
+        <v>0</v>
+      </c>
+      <c r="H19">
+        <f>H5*Shared_Lines!G4</f>
+        <v>0</v>
+      </c>
+      <c r="I19">
+        <f>I5*Shared_Lines!H4</f>
+        <v>0</v>
+      </c>
+      <c r="J19">
+        <f>J5*Shared_Lines!I4</f>
+        <v>0</v>
+      </c>
+      <c r="K19">
+        <f>K5*Shared_Lines!J4</f>
+        <v>0</v>
+      </c>
+      <c r="L19">
+        <f>L5*Shared_Lines!K4</f>
+        <v>0</v>
+      </c>
+      <c r="M19">
+        <f>M5*Shared_Lines!L4</f>
+        <v>-6</v>
+      </c>
+      <c r="N19">
+        <f>N5*Shared_Lines!M4</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="2:14">
+      <c r="B20" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="C20">
+        <f>C6*Shared_Lines!B5</f>
+        <v>0</v>
+      </c>
+      <c r="D20">
+        <f>D6*Shared_Lines!C5</f>
+        <v>0</v>
+      </c>
+      <c r="E20">
+        <f>E6*Shared_Lines!D5</f>
+        <v>0</v>
+      </c>
+      <c r="F20">
+        <f>F6*Shared_Lines!E5</f>
+        <v>0</v>
+      </c>
+      <c r="G20">
+        <f>G6*Shared_Lines!F5</f>
+        <v>0</v>
+      </c>
+      <c r="H20">
+        <f>H6*Shared_Lines!G5</f>
+        <v>0</v>
+      </c>
+      <c r="I20">
+        <f>I6*Shared_Lines!H5</f>
+        <v>0</v>
+      </c>
+      <c r="J20">
+        <f>J6*Shared_Lines!I5</f>
+        <v>0</v>
+      </c>
+      <c r="K20">
+        <f>K6*Shared_Lines!J5</f>
+        <v>0</v>
+      </c>
+      <c r="L20">
+        <f>L6*Shared_Lines!K5</f>
+        <v>0</v>
+      </c>
+      <c r="M20">
+        <f>M6*Shared_Lines!L5</f>
+        <v>0</v>
+      </c>
+      <c r="N20">
+        <f>N6*Shared_Lines!M5</f>
+        <v>-4</v>
+      </c>
+    </row>
+    <row r="21" spans="2:14">
+      <c r="B21" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="C21">
+        <f>C7*Shared_Lines!B6</f>
+        <v>0</v>
+      </c>
+      <c r="D21">
+        <f>D7*Shared_Lines!C6</f>
+        <v>0</v>
+      </c>
+      <c r="E21">
+        <f>E7*Shared_Lines!D6</f>
+        <v>0</v>
+      </c>
+      <c r="F21">
+        <f>F7*Shared_Lines!E6</f>
+        <v>0</v>
+      </c>
+      <c r="G21">
+        <f>G7*Shared_Lines!F6</f>
+        <v>0</v>
+      </c>
+      <c r="H21">
+        <f>H7*Shared_Lines!G6</f>
+        <v>0</v>
+      </c>
+      <c r="I21">
+        <f>I7*Shared_Lines!H6</f>
+        <v>0</v>
+      </c>
+      <c r="J21">
+        <f>J7*Shared_Lines!I6</f>
+        <v>0</v>
+      </c>
+      <c r="K21">
+        <f>K7*Shared_Lines!J6</f>
+        <v>-2</v>
+      </c>
+      <c r="L21">
+        <f>L7*Shared_Lines!K6</f>
+        <v>0</v>
+      </c>
+      <c r="M21">
+        <f>M7*Shared_Lines!L6</f>
+        <v>0</v>
+      </c>
+      <c r="N21">
+        <f>N7*Shared_Lines!M6</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="2:14">
+      <c r="B22" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="C22">
+        <f>C8*Shared_Lines!B7</f>
+        <v>0</v>
+      </c>
+      <c r="D22">
+        <f>D8*Shared_Lines!C7</f>
+        <v>0</v>
+      </c>
+      <c r="E22">
+        <f>E8*Shared_Lines!D7</f>
+        <v>0</v>
+      </c>
+      <c r="F22">
+        <f>F8*Shared_Lines!E7</f>
+        <v>0</v>
+      </c>
+      <c r="G22">
+        <f>G8*Shared_Lines!F7</f>
+        <v>0</v>
+      </c>
+      <c r="H22">
+        <f>H8*Shared_Lines!G7</f>
+        <v>0</v>
+      </c>
+      <c r="I22">
+        <f>I8*Shared_Lines!H7</f>
+        <v>0</v>
+      </c>
+      <c r="J22">
+        <f>J8*Shared_Lines!I7</f>
+        <v>0</v>
+      </c>
+      <c r="K22">
+        <f>K8*Shared_Lines!J7</f>
+        <v>0</v>
+      </c>
+      <c r="L22">
+        <f>L8*Shared_Lines!K7</f>
+        <v>2</v>
+      </c>
+      <c r="M22">
+        <f>M8*Shared_Lines!L7</f>
+        <v>0</v>
+      </c>
+      <c r="N22">
+        <f>N8*Shared_Lines!M7</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="2:14">
+      <c r="B23" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="C23">
+        <f>C9*Shared_Lines!B8</f>
+        <v>0</v>
+      </c>
+      <c r="D23">
+        <f>D9*Shared_Lines!C8</f>
+        <v>0</v>
+      </c>
+      <c r="E23">
+        <f>E9*Shared_Lines!D8</f>
+        <v>0</v>
+      </c>
+      <c r="F23">
+        <f>F9*Shared_Lines!E8</f>
+        <v>0</v>
+      </c>
+      <c r="G23">
+        <f>G9*Shared_Lines!F8</f>
+        <v>0</v>
+      </c>
+      <c r="H23">
+        <f>H9*Shared_Lines!G8</f>
+        <v>0</v>
+      </c>
+      <c r="I23">
+        <f>I9*Shared_Lines!H8</f>
+        <v>0</v>
+      </c>
+      <c r="J23">
+        <f>J9*Shared_Lines!I8</f>
+        <v>0</v>
+      </c>
+      <c r="K23">
+        <f>K9*Shared_Lines!J8</f>
+        <v>0</v>
+      </c>
+      <c r="L23">
+        <f>L9*Shared_Lines!K8</f>
+        <v>0</v>
+      </c>
+      <c r="M23">
+        <f>M9*Shared_Lines!L8</f>
+        <v>0</v>
+      </c>
+      <c r="N23">
+        <f>N9*Shared_Lines!M8</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="2:14">
+      <c r="B24" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="C24">
+        <f>C10*Shared_Lines!B9</f>
+        <v>0</v>
+      </c>
+      <c r="D24">
+        <f>D10*Shared_Lines!C9</f>
+        <v>0</v>
+      </c>
+      <c r="E24">
+        <f>E10*Shared_Lines!D9</f>
+        <v>0</v>
+      </c>
+      <c r="F24">
+        <f>F10*Shared_Lines!E9</f>
+        <v>0</v>
+      </c>
+      <c r="G24">
+        <f>G10*Shared_Lines!F9</f>
+        <v>0</v>
+      </c>
+      <c r="H24">
+        <f>H10*Shared_Lines!G9</f>
+        <v>0</v>
+      </c>
+      <c r="I24">
+        <f>I10*Shared_Lines!H9</f>
+        <v>0</v>
+      </c>
+      <c r="J24">
+        <f>J10*Shared_Lines!I9</f>
+        <v>0</v>
+      </c>
+      <c r="K24">
+        <f>K10*Shared_Lines!J9</f>
+        <v>0</v>
+      </c>
+      <c r="L24">
+        <f>L10*Shared_Lines!K9</f>
+        <v>0</v>
+      </c>
+      <c r="M24">
+        <f>M10*Shared_Lines!L9</f>
+        <v>0</v>
+      </c>
+      <c r="N24">
+        <f>N10*Shared_Lines!M9</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="2:14">
+      <c r="B25" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="C25">
+        <f>C11*Shared_Lines!B10</f>
+        <v>0</v>
+      </c>
+      <c r="D25">
+        <f>D11*Shared_Lines!C10</f>
+        <v>0</v>
+      </c>
+      <c r="E25">
+        <f>E11*Shared_Lines!D10</f>
+        <v>0</v>
+      </c>
+      <c r="F25">
+        <f>F11*Shared_Lines!E10</f>
+        <v>0</v>
+      </c>
+      <c r="G25">
+        <f>G11*Shared_Lines!F10</f>
+        <v>0</v>
+      </c>
+      <c r="H25">
+        <f>H11*Shared_Lines!G10</f>
+        <v>0</v>
+      </c>
+      <c r="I25">
+        <f>I11*Shared_Lines!H10</f>
+        <v>0</v>
+      </c>
+      <c r="J25">
+        <f>J11*Shared_Lines!I10</f>
+        <v>0</v>
+      </c>
+      <c r="K25">
+        <f>K11*Shared_Lines!J10</f>
+        <v>0</v>
+      </c>
+      <c r="L25">
+        <f>L11*Shared_Lines!K10</f>
+        <v>0</v>
+      </c>
+      <c r="M25">
+        <f>M11*Shared_Lines!L10</f>
+        <v>0</v>
+      </c>
+      <c r="N25">
+        <f>N11*Shared_Lines!M10</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="2:14">
+      <c r="B26" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C26">
+        <f>C12*Shared_Lines!B11</f>
+        <v>0</v>
+      </c>
+      <c r="D26">
+        <f>D12*Shared_Lines!C11</f>
+        <v>0</v>
+      </c>
+      <c r="E26">
+        <f>E12*Shared_Lines!D11</f>
+        <v>0</v>
+      </c>
+      <c r="F26">
+        <f>F12*Shared_Lines!E11</f>
+        <v>0</v>
+      </c>
+      <c r="G26">
+        <f>G12*Shared_Lines!F11</f>
+        <v>0</v>
+      </c>
+      <c r="H26">
+        <f>H12*Shared_Lines!G11</f>
+        <v>0</v>
+      </c>
+      <c r="I26">
+        <f>I12*Shared_Lines!H11</f>
+        <v>0</v>
+      </c>
+      <c r="J26">
+        <f>J12*Shared_Lines!I11</f>
+        <v>0</v>
+      </c>
+      <c r="K26">
+        <f>K12*Shared_Lines!J11</f>
+        <v>0</v>
+      </c>
+      <c r="L26">
+        <f>L12*Shared_Lines!K11</f>
+        <v>0</v>
+      </c>
+      <c r="M26">
+        <f>M12*Shared_Lines!L11</f>
+        <v>0</v>
+      </c>
+      <c r="N26">
+        <f>N12*Shared_Lines!M11</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="2:14">
+      <c r="B27" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="C27">
+        <f>C13*Shared_Lines!B12</f>
+        <v>0</v>
+      </c>
+      <c r="D27">
+        <f>D13*Shared_Lines!C12</f>
+        <v>0</v>
+      </c>
+      <c r="E27">
+        <f>E13*Shared_Lines!D12</f>
+        <v>0</v>
+      </c>
+      <c r="F27">
+        <f>F13*Shared_Lines!E12</f>
+        <v>0</v>
+      </c>
+      <c r="G27">
+        <f>G13*Shared_Lines!F12</f>
+        <v>0</v>
+      </c>
+      <c r="H27">
+        <f>H13*Shared_Lines!G12</f>
+        <v>0</v>
+      </c>
+      <c r="I27">
+        <f>I13*Shared_Lines!H12</f>
+        <v>0</v>
+      </c>
+      <c r="J27">
+        <f>J13*Shared_Lines!I12</f>
+        <v>0</v>
+      </c>
+      <c r="K27">
+        <f>K13*Shared_Lines!J12</f>
+        <v>0</v>
+      </c>
+      <c r="L27">
+        <f>L13*Shared_Lines!K12</f>
+        <v>0</v>
+      </c>
+      <c r="M27">
+        <f>M13*Shared_Lines!L12</f>
+        <v>0</v>
+      </c>
+      <c r="N27">
+        <f>N13*Shared_Lines!M12</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="2:14">
+      <c r="B28" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C28">
+        <f>C14*Shared_Lines!B13</f>
+        <v>0</v>
+      </c>
+      <c r="D28">
+        <f>D14*Shared_Lines!C13</f>
+        <v>0</v>
+      </c>
+      <c r="E28">
+        <f>E14*Shared_Lines!D13</f>
+        <v>0</v>
+      </c>
+      <c r="F28">
+        <f>F14*Shared_Lines!E13</f>
+        <v>0</v>
+      </c>
+      <c r="G28">
+        <f>G14*Shared_Lines!F13</f>
+        <v>0</v>
+      </c>
+      <c r="H28">
+        <f>H14*Shared_Lines!G13</f>
+        <v>0</v>
+      </c>
+      <c r="I28">
+        <f>I14*Shared_Lines!H13</f>
+        <v>0</v>
+      </c>
+      <c r="J28">
+        <f>J14*Shared_Lines!I13</f>
+        <v>0</v>
+      </c>
+      <c r="K28">
+        <f>K14*Shared_Lines!J13</f>
+        <v>0</v>
+      </c>
+      <c r="L28">
+        <f>L14*Shared_Lines!K13</f>
+        <v>0</v>
+      </c>
+      <c r="M28">
+        <f>M14*Shared_Lines!L13</f>
+        <v>0</v>
+      </c>
+      <c r="N28">
+        <f>N14*Shared_Lines!M13</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="2:14">
+      <c r="B30" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="G30" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="H30" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="I30" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="J30" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="K30" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="L30" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="M30" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="N30" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="31" spans="2:14">
+      <c r="B31" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C31" t="b">
+        <f>AND(C17=Shared_Lines_Offset!B2,C17&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="D31" t="b">
+        <f>AND(D17=Shared_Lines_Offset!C2,D17&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="E31" t="b">
+        <f>AND(E17=Shared_Lines_Offset!D2,E17&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="F31" t="b">
+        <f>AND(F17=Shared_Lines_Offset!E2,F17&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="G31" t="b">
+        <f>AND(G17=Shared_Lines_Offset!F2,G17&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="H31" t="b">
+        <f>AND(H17=Shared_Lines_Offset!G2,H17&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="I31" t="b">
+        <f>AND(I17=Shared_Lines_Offset!H2,I17&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="J31" t="b">
+        <f>AND(J17=Shared_Lines_Offset!I2,J17&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="K31" t="b">
+        <f>AND(K17=Shared_Lines_Offset!J2,K17&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="L31" t="b">
+        <f>AND(L17=Shared_Lines_Offset!K2,L17&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="M31" t="b">
+        <f>AND(M17=Shared_Lines_Offset!L2,M17&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="N31" t="b">
+        <f>AND(N17=Shared_Lines_Offset!M2,N17&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="2:14">
+      <c r="B32" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C32" t="b">
+        <f>AND(C18=Shared_Lines_Offset!B3,C18&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="D32" t="b">
+        <f>AND(D18=Shared_Lines_Offset!C3,D18&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="E32" t="b">
+        <f>AND(E18=Shared_Lines_Offset!D3,E18&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="F32" t="b">
+        <f>AND(F18=Shared_Lines_Offset!E3,F18&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="G32" t="b">
+        <f>AND(G18=Shared_Lines_Offset!F3,G18&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="H32" t="b">
+        <f>AND(H18=Shared_Lines_Offset!G3,H18&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="I32" t="b">
+        <f>AND(I18=Shared_Lines_Offset!H3,I18&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="J32" t="b">
+        <f>AND(J18=Shared_Lines_Offset!I3,J18&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="K32" t="b">
+        <f>AND(K18=Shared_Lines_Offset!J3,K18&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="L32" t="b">
+        <f>AND(L18=Shared_Lines_Offset!K3,L18&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="M32" t="b">
+        <f>AND(M18=Shared_Lines_Offset!L3,M18&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="N32" t="b">
+        <f>AND(N18=Shared_Lines_Offset!M3,N18&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="2:14">
+      <c r="B33" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="C33" t="b">
+        <f>AND(C19=Shared_Lines_Offset!B4,C19&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="D33" t="b">
+        <f>AND(D19=Shared_Lines_Offset!C4,D19&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="E33" t="b">
+        <f>AND(E19=Shared_Lines_Offset!D4,E19&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="F33" t="b">
+        <f>AND(F19=Shared_Lines_Offset!E4,F19&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="G33" t="b">
+        <f>AND(G19=Shared_Lines_Offset!F4,G19&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="H33" t="b">
+        <f>AND(H19=Shared_Lines_Offset!G4,H19&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="I33" t="b">
+        <f>AND(I19=Shared_Lines_Offset!H4,I19&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="J33" t="b">
+        <f>AND(J19=Shared_Lines_Offset!I4,J19&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="K33" t="b">
+        <f>AND(K19=Shared_Lines_Offset!J4,K19&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="L33" t="b">
+        <f>AND(L19=Shared_Lines_Offset!K4,L19&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="M33" t="b">
+        <f>AND(M19=Shared_Lines_Offset!L4,M19&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="N33" t="b">
+        <f>AND(N19=Shared_Lines_Offset!M4,N19&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="2:14">
+      <c r="B34" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="C34" t="b">
+        <f>AND(C20=Shared_Lines_Offset!B5,C20&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="D34" t="b">
+        <f>AND(D20=Shared_Lines_Offset!C5,D20&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="E34" t="b">
+        <f>AND(E20=Shared_Lines_Offset!D5,E20&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="F34" t="b">
+        <f>AND(F20=Shared_Lines_Offset!E5,F20&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="G34" t="b">
+        <f>AND(G20=Shared_Lines_Offset!F5,G20&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="H34" t="b">
+        <f>AND(H20=Shared_Lines_Offset!G5,H20&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="I34" t="b">
+        <f>AND(I20=Shared_Lines_Offset!H5,I20&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="J34" t="b">
+        <f>AND(J20=Shared_Lines_Offset!I5,J20&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="K34" t="b">
+        <f>AND(K20=Shared_Lines_Offset!J5,K20&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="L34" t="b">
+        <f>AND(L20=Shared_Lines_Offset!K5,L20&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="M34" t="b">
+        <f>AND(M20=Shared_Lines_Offset!L5,M20&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="N34" t="b">
+        <f>AND(N20=Shared_Lines_Offset!M5,N20&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="2:14">
+      <c r="B35" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="C35" t="b">
+        <f>AND(C21=Shared_Lines_Offset!B6,C21&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="D35" t="b">
+        <f>AND(D21=Shared_Lines_Offset!C6,D21&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="E35" t="b">
+        <f>AND(E21=Shared_Lines_Offset!D6,E21&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="F35" t="b">
+        <f>AND(F21=Shared_Lines_Offset!E6,F21&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="G35" t="b">
+        <f>AND(G21=Shared_Lines_Offset!F6,G21&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="H35" t="b">
+        <f>AND(H21=Shared_Lines_Offset!G6,H21&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="I35" t="b">
+        <f>AND(I21=Shared_Lines_Offset!H6,I21&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="J35" t="b">
+        <f>AND(J21=Shared_Lines_Offset!I6,J21&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="K35" t="b">
+        <f>AND(K21=Shared_Lines_Offset!J6,K21&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="L35" t="b">
+        <f>AND(L21=Shared_Lines_Offset!K6,L21&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="M35" t="b">
+        <f>AND(M21=Shared_Lines_Offset!L6,M21&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="N35" t="b">
+        <f>AND(N21=Shared_Lines_Offset!M6,N21&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="2:14">
+      <c r="B36" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="C36" t="b">
+        <f>AND(C22=Shared_Lines_Offset!B7,C22&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="D36" t="b">
+        <f>AND(D22=Shared_Lines_Offset!C7,D22&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="E36" t="b">
+        <f>AND(E22=Shared_Lines_Offset!D7,E22&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="F36" t="b">
+        <f>AND(F22=Shared_Lines_Offset!E7,F22&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="G36" t="b">
+        <f>AND(G22=Shared_Lines_Offset!F7,G22&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="H36" t="b">
+        <f>AND(H22=Shared_Lines_Offset!G7,H22&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="I36" t="b">
+        <f>AND(I22=Shared_Lines_Offset!H7,I22&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="J36" t="b">
+        <f>AND(J22=Shared_Lines_Offset!I7,J22&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="K36" t="b">
+        <f>AND(K22=Shared_Lines_Offset!J7,K22&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="L36" t="b">
+        <f>AND(L22=Shared_Lines_Offset!K7,L22&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="M36" t="b">
+        <f>AND(M22=Shared_Lines_Offset!L7,M22&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="N36" t="b">
+        <f>AND(N22=Shared_Lines_Offset!M7,N22&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="2:14">
+      <c r="B37" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="C37" t="b">
+        <f>AND(C23=Shared_Lines_Offset!B8,C23&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="D37" t="b">
+        <f>AND(D23=Shared_Lines_Offset!C8,D23&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="E37" t="b">
+        <f>AND(E23=Shared_Lines_Offset!D8,E23&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="F37" t="b">
+        <f>AND(F23=Shared_Lines_Offset!E8,F23&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="G37" t="b">
+        <f>AND(G23=Shared_Lines_Offset!F8,G23&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="H37" t="b">
+        <f>AND(H23=Shared_Lines_Offset!G8,H23&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="I37" t="b">
+        <f>AND(I23=Shared_Lines_Offset!H8,I23&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="J37" t="b">
+        <f>AND(J23=Shared_Lines_Offset!I8,J23&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="K37" t="b">
+        <f>AND(K23=Shared_Lines_Offset!J8,K23&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="L37" t="b">
+        <f>AND(L23=Shared_Lines_Offset!K8,L23&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="M37" t="b">
+        <f>AND(M23=Shared_Lines_Offset!L8,M23&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="N37" t="b">
+        <f>AND(N23=Shared_Lines_Offset!M8,N23&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="2:14">
+      <c r="B38" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="C38" t="b">
+        <f>AND(C24=Shared_Lines_Offset!B9,C24&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="D38" t="b">
+        <f>AND(D24=Shared_Lines_Offset!C9,D24&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="E38" t="b">
+        <f>AND(E24=Shared_Lines_Offset!D9,E24&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="F38" t="b">
+        <f>AND(F24=Shared_Lines_Offset!E9,F24&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="G38" t="b">
+        <f>AND(G24=Shared_Lines_Offset!F9,G24&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="H38" t="b">
+        <f>AND(H24=Shared_Lines_Offset!G9,H24&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="I38" t="b">
+        <f>AND(I24=Shared_Lines_Offset!H9,I24&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="J38" t="b">
+        <f>AND(J24=Shared_Lines_Offset!I9,J24&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="K38" t="b">
+        <f>AND(K24=Shared_Lines_Offset!J9,K24&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="L38" t="b">
+        <f>AND(L24=Shared_Lines_Offset!K9,L24&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="M38" t="b">
+        <f>AND(M24=Shared_Lines_Offset!L9,M24&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="N38" t="b">
+        <f>AND(N24=Shared_Lines_Offset!M9,N24&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="2:14">
+      <c r="B39" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="C39" t="b">
+        <f>AND(C25=Shared_Lines_Offset!B10,C25&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="D39" t="b">
+        <f>AND(D25=Shared_Lines_Offset!C10,D25&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="E39" t="b">
+        <f>AND(E25=Shared_Lines_Offset!D10,E25&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="F39" t="b">
+        <f>AND(F25=Shared_Lines_Offset!E10,F25&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="G39" t="b">
+        <f>AND(G25=Shared_Lines_Offset!F10,G25&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="H39" t="b">
+        <f>AND(H25=Shared_Lines_Offset!G10,H25&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="I39" t="b">
+        <f>AND(I25=Shared_Lines_Offset!H10,I25&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="J39" t="b">
+        <f>AND(J25=Shared_Lines_Offset!I10,J25&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="K39" t="b">
+        <f>AND(K25=Shared_Lines_Offset!J10,K25&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="L39" t="b">
+        <f>AND(L25=Shared_Lines_Offset!K10,L25&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="M39" t="b">
+        <f>AND(M25=Shared_Lines_Offset!L10,M25&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="N39" t="b">
+        <f>AND(N25=Shared_Lines_Offset!M10,N25&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="2:14">
+      <c r="B40" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C40" t="b">
+        <f>AND(C26=Shared_Lines_Offset!B11,C26&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="D40" t="b">
+        <f>AND(D26=Shared_Lines_Offset!C11,D26&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="E40" t="b">
+        <f>AND(E26=Shared_Lines_Offset!D11,E26&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="F40" t="b">
+        <f>AND(F26=Shared_Lines_Offset!E11,F26&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="G40" t="b">
+        <f>AND(G26=Shared_Lines_Offset!F11,G26&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="H40" t="b">
+        <f>AND(H26=Shared_Lines_Offset!G11,H26&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="I40" t="b">
+        <f>AND(I26=Shared_Lines_Offset!H11,I26&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="J40" t="b">
+        <f>AND(J26=Shared_Lines_Offset!I11,J26&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="K40" t="b">
+        <f>AND(K26=Shared_Lines_Offset!J11,K26&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="L40" t="b">
+        <f>AND(L26=Shared_Lines_Offset!K11,L26&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="M40" t="b">
+        <f>AND(M26=Shared_Lines_Offset!L11,M26&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="N40" t="b">
+        <f>AND(N26=Shared_Lines_Offset!M11,N26&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="2:14">
+      <c r="B41" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="C41" t="b">
+        <f>AND(C27=Shared_Lines_Offset!B12,C27&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="D41" t="b">
+        <f>AND(D27=Shared_Lines_Offset!C12,D27&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="E41" t="b">
+        <f>AND(E27=Shared_Lines_Offset!D12,E27&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="F41" t="b">
+        <f>AND(F27=Shared_Lines_Offset!E12,F27&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="G41" t="b">
+        <f>AND(G27=Shared_Lines_Offset!F12,G27&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="H41" t="b">
+        <f>AND(H27=Shared_Lines_Offset!G12,H27&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="I41" t="b">
+        <f>AND(I27=Shared_Lines_Offset!H12,I27&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="J41" t="b">
+        <f>AND(J27=Shared_Lines_Offset!I12,J27&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="K41" t="b">
+        <f>AND(K27=Shared_Lines_Offset!J12,K27&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="L41" t="b">
+        <f>AND(L27=Shared_Lines_Offset!K12,L27&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="M41" t="b">
+        <f>AND(M27=Shared_Lines_Offset!L12,M27&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="N41" t="b">
+        <f>AND(N27=Shared_Lines_Offset!M12,N27&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="2:14">
+      <c r="B42" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C42" t="b">
+        <f>AND(C28=Shared_Lines_Offset!B13,C28&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="D42" t="b">
+        <f>AND(D28=Shared_Lines_Offset!C13,D28&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="E42" t="b">
+        <f>AND(E28=Shared_Lines_Offset!D13,E28&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="F42" t="b">
+        <f>AND(F28=Shared_Lines_Offset!E13,F28&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="G42" t="b">
+        <f>AND(G28=Shared_Lines_Offset!F13,G28&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="H42" t="b">
+        <f>AND(H28=Shared_Lines_Offset!G13,H28&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="I42" t="b">
+        <f>AND(I28=Shared_Lines_Offset!H13,I28&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="J42" t="b">
+        <f>AND(J28=Shared_Lines_Offset!I13,J28&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="K42" t="b">
+        <f>AND(K28=Shared_Lines_Offset!J13,K28&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="L42" t="b">
+        <f>AND(L28=Shared_Lines_Offset!K13,L28&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="M42" t="b">
+        <f>AND(M28=Shared_Lines_Offset!L13,M28&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="N42" t="b">
+        <f>AND(N28=Shared_Lines_Offset!M13,N28&lt;&gt;0)</f>
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
tested and fixed OFFSET
</commit_message>
<xml_diff>
--- a/data/Times_to_Transfer_Stations.xlsx
+++ b/data/Times_to_Transfer_Stations.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25725"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="2560" yWindow="0" windowWidth="25600" windowHeight="15860" tabRatio="564" firstSheet="3" activeTab="7"/>
+    <workbookView xWindow="8760" yWindow="0" windowWidth="25600" windowHeight="15860" tabRatio="564" firstSheet="5" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="Station_Time_Calculations" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,8 @@
     <sheet name="Shared_Lines_Calc" sheetId="5" r:id="rId5"/>
     <sheet name="Shared_Lines" sheetId="6" r:id="rId6"/>
     <sheet name="Shared_Lines_Offset" sheetId="7" r:id="rId7"/>
-    <sheet name="shared_test_sat_morn" sheetId="8" r:id="rId8"/>
+    <sheet name="shared_test_sat_morn_orig" sheetId="8" r:id="rId8"/>
+    <sheet name="shared_test_sat_morn_abs1" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="905" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="986" uniqueCount="113">
   <si>
     <t>-</t>
   </si>
@@ -353,6 +354,18 @@
   </si>
   <si>
     <t>Violated Shared</t>
+  </si>
+  <si>
+    <t>start</t>
+  </si>
+  <si>
+    <t>to rosslyn</t>
+  </si>
+  <si>
+    <t>arrive rosslyn</t>
+  </si>
+  <si>
+    <t>*shared lines constraint violated for Orange_neg, Silver_neg</t>
   </si>
 </sst>
 </file>
@@ -396,12 +409,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -413,7 +432,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="137">
+  <cellStyleXfs count="149">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -551,13 +570,27 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="137">
+  <cellStyles count="149">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -626,6 +659,12 @@
     <cellStyle name="Followed Hyperlink" xfId="132" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="134" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="136" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="138" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="140" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="142" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="144" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="146" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="148" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -694,6 +733,12 @@
     <cellStyle name="Hyperlink" xfId="131" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="133" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="135" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="137" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="139" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="141" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="143" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="145" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="147" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -4323,7 +4368,7 @@
   <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -6033,7 +6078,7 @@
   <dimension ref="A1:M13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H23" sqref="H23"/>
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -6584,10 +6629,2180 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:T45"/>
+  <sheetViews>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="D45" sqref="D45"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:20">
+      <c r="C1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20">
+      <c r="A2" s="1"/>
+      <c r="B2" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="C2" s="1">
+        <v>4</v>
+      </c>
+      <c r="D2" s="1">
+        <v>11</v>
+      </c>
+      <c r="E2" s="1">
+        <v>5</v>
+      </c>
+      <c r="F2" s="1">
+        <v>5</v>
+      </c>
+      <c r="G2" s="1">
+        <v>6</v>
+      </c>
+      <c r="H2" s="1">
+        <v>9</v>
+      </c>
+      <c r="I2" s="1">
+        <v>2</v>
+      </c>
+      <c r="J2" s="1">
+        <v>9</v>
+      </c>
+      <c r="K2" s="1">
+        <v>8</v>
+      </c>
+      <c r="L2" s="1">
+        <v>7</v>
+      </c>
+      <c r="M2" s="1">
+        <v>11</v>
+      </c>
+      <c r="N2" s="1">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20">
+      <c r="A3" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" s="1">
+        <v>4</v>
+      </c>
+      <c r="C3">
+        <f>$B3-C$2</f>
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <f t="shared" ref="D3:N14" si="0">$B3-D$2</f>
+        <v>-7</v>
+      </c>
+      <c r="E3">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+      <c r="F3">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+      <c r="G3">
+        <f t="shared" si="0"/>
+        <v>-2</v>
+      </c>
+      <c r="H3">
+        <f t="shared" si="0"/>
+        <v>-5</v>
+      </c>
+      <c r="I3">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="J3">
+        <f t="shared" si="0"/>
+        <v>-5</v>
+      </c>
+      <c r="K3">
+        <f t="shared" si="0"/>
+        <v>-4</v>
+      </c>
+      <c r="L3">
+        <f t="shared" si="0"/>
+        <v>-3</v>
+      </c>
+      <c r="M3">
+        <f t="shared" si="0"/>
+        <v>-7</v>
+      </c>
+      <c r="N3">
+        <f t="shared" si="0"/>
+        <v>-5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20">
+      <c r="A4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="1">
+        <v>11</v>
+      </c>
+      <c r="C4">
+        <f t="shared" ref="C4:C14" si="1">$B4-C$2</f>
+        <v>7</v>
+      </c>
+      <c r="D4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="F4">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="G4">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="H4">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="I4">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="J4">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="K4">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="L4">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="M4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N4">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20">
+      <c r="A5" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B5" s="1">
+        <v>5</v>
+      </c>
+      <c r="C5">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <f t="shared" si="0"/>
+        <v>-6</v>
+      </c>
+      <c r="E5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+      <c r="H5">
+        <f t="shared" si="0"/>
+        <v>-4</v>
+      </c>
+      <c r="I5">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="J5">
+        <f t="shared" si="0"/>
+        <v>-4</v>
+      </c>
+      <c r="K5">
+        <f t="shared" si="0"/>
+        <v>-3</v>
+      </c>
+      <c r="L5">
+        <f t="shared" si="0"/>
+        <v>-2</v>
+      </c>
+      <c r="M5">
+        <f t="shared" si="0"/>
+        <v>-6</v>
+      </c>
+      <c r="N5">
+        <f t="shared" si="0"/>
+        <v>-4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20">
+      <c r="A6" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B6" s="1">
+        <v>5</v>
+      </c>
+      <c r="C6">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <f t="shared" si="0"/>
+        <v>-6</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+      <c r="H6">
+        <f t="shared" si="0"/>
+        <v>-4</v>
+      </c>
+      <c r="I6">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="J6">
+        <f t="shared" si="0"/>
+        <v>-4</v>
+      </c>
+      <c r="K6">
+        <f t="shared" si="0"/>
+        <v>-3</v>
+      </c>
+      <c r="L6">
+        <f t="shared" si="0"/>
+        <v>-2</v>
+      </c>
+      <c r="M6">
+        <f t="shared" si="0"/>
+        <v>-6</v>
+      </c>
+      <c r="N6">
+        <f t="shared" si="0"/>
+        <v>-4</v>
+      </c>
+      <c r="R6" t="s">
+        <v>109</v>
+      </c>
+      <c r="S6" t="s">
+        <v>110</v>
+      </c>
+      <c r="T6" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20">
+      <c r="A7" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B7" s="1">
+        <v>6</v>
+      </c>
+      <c r="C7">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="D7">
+        <f t="shared" si="0"/>
+        <v>-5</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="F7">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="G7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H7">
+        <f t="shared" si="0"/>
+        <v>-3</v>
+      </c>
+      <c r="I7">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="J7">
+        <f t="shared" si="0"/>
+        <v>-3</v>
+      </c>
+      <c r="K7">
+        <f t="shared" si="0"/>
+        <v>-2</v>
+      </c>
+      <c r="L7">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+      <c r="M7">
+        <f t="shared" si="0"/>
+        <v>-5</v>
+      </c>
+      <c r="N7">
+        <f t="shared" si="0"/>
+        <v>-3</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>15</v>
+      </c>
+      <c r="R7">
+        <v>9</v>
+      </c>
+      <c r="S7">
+        <v>35</v>
+      </c>
+      <c r="T7">
+        <f>R7+S7</f>
+        <v>44</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20">
+      <c r="A8" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="B8" s="1">
+        <v>9</v>
+      </c>
+      <c r="C8">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="D8">
+        <f t="shared" si="0"/>
+        <v>-2</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="F8">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="G8">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="H8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I8">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="J8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K8">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="L8">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="M8">
+        <f t="shared" si="0"/>
+        <v>-2</v>
+      </c>
+      <c r="N8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>14</v>
+      </c>
+      <c r="R8">
+        <v>7</v>
+      </c>
+      <c r="S8">
+        <v>37</v>
+      </c>
+      <c r="T8">
+        <f>R8+S8</f>
+        <v>44</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20">
+      <c r="A9" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B9" s="1">
+        <v>2</v>
+      </c>
+      <c r="C9">
+        <f t="shared" si="1"/>
+        <v>-2</v>
+      </c>
+      <c r="D9">
+        <f t="shared" si="0"/>
+        <v>-9</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="0"/>
+        <v>-3</v>
+      </c>
+      <c r="F9">
+        <f t="shared" si="0"/>
+        <v>-3</v>
+      </c>
+      <c r="G9">
+        <f t="shared" si="0"/>
+        <v>-4</v>
+      </c>
+      <c r="H9">
+        <f t="shared" si="0"/>
+        <v>-7</v>
+      </c>
+      <c r="I9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J9">
+        <f t="shared" si="0"/>
+        <v>-7</v>
+      </c>
+      <c r="K9">
+        <f t="shared" si="0"/>
+        <v>-6</v>
+      </c>
+      <c r="L9">
+        <f t="shared" si="0"/>
+        <v>-5</v>
+      </c>
+      <c r="M9">
+        <f t="shared" si="0"/>
+        <v>-9</v>
+      </c>
+      <c r="N9">
+        <f t="shared" si="0"/>
+        <v>-7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20">
+      <c r="A10" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B10" s="1">
+        <v>9</v>
+      </c>
+      <c r="C10">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="D10">
+        <f t="shared" si="0"/>
+        <v>-2</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="F10">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="G10">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="H10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I10">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="J10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K10">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="L10">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="M10">
+        <f t="shared" si="0"/>
+        <v>-2</v>
+      </c>
+      <c r="N10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20">
+      <c r="A11" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="B11" s="1">
+        <v>8</v>
+      </c>
+      <c r="C11">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="D11">
+        <f t="shared" si="0"/>
+        <v>-3</v>
+      </c>
+      <c r="E11">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="F11">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="G11">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="H11">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+      <c r="I11">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="J11">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+      <c r="K11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L11">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="M11">
+        <f t="shared" si="0"/>
+        <v>-3</v>
+      </c>
+      <c r="N11">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20">
+      <c r="A12" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="B12" s="1">
+        <v>7</v>
+      </c>
+      <c r="C12">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="D12">
+        <f t="shared" si="0"/>
+        <v>-4</v>
+      </c>
+      <c r="E12">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="F12">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="G12">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="H12">
+        <f t="shared" si="0"/>
+        <v>-2</v>
+      </c>
+      <c r="I12">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="J12">
+        <f t="shared" si="0"/>
+        <v>-2</v>
+      </c>
+      <c r="K12">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+      <c r="L12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M12">
+        <f t="shared" si="0"/>
+        <v>-4</v>
+      </c>
+      <c r="N12">
+        <f t="shared" si="0"/>
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20">
+      <c r="A13" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="B13" s="1">
+        <v>11</v>
+      </c>
+      <c r="C13">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="D13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E13">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="F13">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="G13">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="H13">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="I13">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="J13">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="K13">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="L13">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="M13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N13">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20">
+      <c r="A14" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B14" s="1">
+        <v>9</v>
+      </c>
+      <c r="C14">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="D14">
+        <f t="shared" si="0"/>
+        <v>-2</v>
+      </c>
+      <c r="E14">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="F14">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="G14">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="H14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I14">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="J14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K14">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="L14">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="M14">
+        <f t="shared" si="0"/>
+        <v>-2</v>
+      </c>
+      <c r="N14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20">
+      <c r="B16" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="J16" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="K16" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="L16" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="M16" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="N16" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="17" spans="2:14">
+      <c r="B17" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C17">
+        <f>C3*Shared_Lines!B2</f>
+        <v>0</v>
+      </c>
+      <c r="D17">
+        <f>D3*Shared_Lines!C2</f>
+        <v>0</v>
+      </c>
+      <c r="E17">
+        <f>E3*Shared_Lines!D2</f>
+        <v>0</v>
+      </c>
+      <c r="F17">
+        <f>F3*Shared_Lines!E2</f>
+        <v>0</v>
+      </c>
+      <c r="G17">
+        <f>G3*Shared_Lines!F2</f>
+        <v>-2</v>
+      </c>
+      <c r="H17">
+        <f>H3*Shared_Lines!G2</f>
+        <v>0</v>
+      </c>
+      <c r="I17">
+        <f>I3*Shared_Lines!H2</f>
+        <v>0</v>
+      </c>
+      <c r="J17">
+        <f>J3*Shared_Lines!I2</f>
+        <v>0</v>
+      </c>
+      <c r="K17">
+        <f>K3*Shared_Lines!J2</f>
+        <v>-4</v>
+      </c>
+      <c r="L17">
+        <f>L3*Shared_Lines!K2</f>
+        <v>0</v>
+      </c>
+      <c r="M17">
+        <f>M3*Shared_Lines!L2</f>
+        <v>-7</v>
+      </c>
+      <c r="N17">
+        <f>N3*Shared_Lines!M2</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="2:14">
+      <c r="B18" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C18">
+        <f>C4*Shared_Lines!B3</f>
+        <v>0</v>
+      </c>
+      <c r="D18">
+        <f>D4*Shared_Lines!C3</f>
+        <v>0</v>
+      </c>
+      <c r="E18">
+        <f>E4*Shared_Lines!D3</f>
+        <v>0</v>
+      </c>
+      <c r="F18">
+        <f>F4*Shared_Lines!E3</f>
+        <v>0</v>
+      </c>
+      <c r="G18">
+        <f>G4*Shared_Lines!F3</f>
+        <v>0</v>
+      </c>
+      <c r="H18">
+        <f>H4*Shared_Lines!G3</f>
+        <v>2</v>
+      </c>
+      <c r="I18">
+        <f>I4*Shared_Lines!H3</f>
+        <v>0</v>
+      </c>
+      <c r="J18">
+        <f>J4*Shared_Lines!I3</f>
+        <v>0</v>
+      </c>
+      <c r="K18">
+        <f>K4*Shared_Lines!J3</f>
+        <v>0</v>
+      </c>
+      <c r="L18">
+        <f>L4*Shared_Lines!K3</f>
+        <v>4</v>
+      </c>
+      <c r="M18">
+        <f>M4*Shared_Lines!L3</f>
+        <v>0</v>
+      </c>
+      <c r="N18">
+        <f>N4*Shared_Lines!M3</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="2:14">
+      <c r="B19" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="C19">
+        <f>C5*Shared_Lines!B4</f>
+        <v>0</v>
+      </c>
+      <c r="D19">
+        <f>D5*Shared_Lines!C4</f>
+        <v>0</v>
+      </c>
+      <c r="E19">
+        <f>E5*Shared_Lines!D4</f>
+        <v>0</v>
+      </c>
+      <c r="F19">
+        <f>F5*Shared_Lines!E4</f>
+        <v>0</v>
+      </c>
+      <c r="G19">
+        <f>G5*Shared_Lines!F4</f>
+        <v>0</v>
+      </c>
+      <c r="H19">
+        <f>H5*Shared_Lines!G4</f>
+        <v>0</v>
+      </c>
+      <c r="I19">
+        <f>I5*Shared_Lines!H4</f>
+        <v>0</v>
+      </c>
+      <c r="J19">
+        <f>J5*Shared_Lines!I4</f>
+        <v>0</v>
+      </c>
+      <c r="K19">
+        <f>K5*Shared_Lines!J4</f>
+        <v>0</v>
+      </c>
+      <c r="L19">
+        <f>L5*Shared_Lines!K4</f>
+        <v>0</v>
+      </c>
+      <c r="M19">
+        <f>M5*Shared_Lines!L4</f>
+        <v>-6</v>
+      </c>
+      <c r="N19">
+        <f>N5*Shared_Lines!M4</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="2:14">
+      <c r="B20" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="C20">
+        <f>C6*Shared_Lines!B5</f>
+        <v>0</v>
+      </c>
+      <c r="D20">
+        <f>D6*Shared_Lines!C5</f>
+        <v>0</v>
+      </c>
+      <c r="E20">
+        <f>E6*Shared_Lines!D5</f>
+        <v>0</v>
+      </c>
+      <c r="F20">
+        <f>F6*Shared_Lines!E5</f>
+        <v>0</v>
+      </c>
+      <c r="G20">
+        <f>G6*Shared_Lines!F5</f>
+        <v>0</v>
+      </c>
+      <c r="H20">
+        <f>H6*Shared_Lines!G5</f>
+        <v>0</v>
+      </c>
+      <c r="I20">
+        <f>I6*Shared_Lines!H5</f>
+        <v>0</v>
+      </c>
+      <c r="J20">
+        <f>J6*Shared_Lines!I5</f>
+        <v>0</v>
+      </c>
+      <c r="K20">
+        <f>K6*Shared_Lines!J5</f>
+        <v>0</v>
+      </c>
+      <c r="L20">
+        <f>L6*Shared_Lines!K5</f>
+        <v>0</v>
+      </c>
+      <c r="M20">
+        <f>M6*Shared_Lines!L5</f>
+        <v>0</v>
+      </c>
+      <c r="N20">
+        <f>N6*Shared_Lines!M5</f>
+        <v>-4</v>
+      </c>
+    </row>
+    <row r="21" spans="2:14">
+      <c r="B21" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="C21">
+        <f>C7*Shared_Lines!B6</f>
+        <v>0</v>
+      </c>
+      <c r="D21">
+        <f>D7*Shared_Lines!C6</f>
+        <v>0</v>
+      </c>
+      <c r="E21">
+        <f>E7*Shared_Lines!D6</f>
+        <v>0</v>
+      </c>
+      <c r="F21">
+        <f>F7*Shared_Lines!E6</f>
+        <v>0</v>
+      </c>
+      <c r="G21">
+        <f>G7*Shared_Lines!F6</f>
+        <v>0</v>
+      </c>
+      <c r="H21">
+        <f>H7*Shared_Lines!G6</f>
+        <v>0</v>
+      </c>
+      <c r="I21">
+        <f>I7*Shared_Lines!H6</f>
+        <v>0</v>
+      </c>
+      <c r="J21">
+        <f>J7*Shared_Lines!I6</f>
+        <v>0</v>
+      </c>
+      <c r="K21">
+        <f>K7*Shared_Lines!J6</f>
+        <v>-2</v>
+      </c>
+      <c r="L21">
+        <f>L7*Shared_Lines!K6</f>
+        <v>0</v>
+      </c>
+      <c r="M21">
+        <f>M7*Shared_Lines!L6</f>
+        <v>0</v>
+      </c>
+      <c r="N21">
+        <f>N7*Shared_Lines!M6</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="2:14">
+      <c r="B22" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="C22">
+        <f>C8*Shared_Lines!B7</f>
+        <v>0</v>
+      </c>
+      <c r="D22">
+        <f>D8*Shared_Lines!C7</f>
+        <v>0</v>
+      </c>
+      <c r="E22">
+        <f>E8*Shared_Lines!D7</f>
+        <v>0</v>
+      </c>
+      <c r="F22">
+        <f>F8*Shared_Lines!E7</f>
+        <v>0</v>
+      </c>
+      <c r="G22">
+        <f>G8*Shared_Lines!F7</f>
+        <v>0</v>
+      </c>
+      <c r="H22">
+        <f>H8*Shared_Lines!G7</f>
+        <v>0</v>
+      </c>
+      <c r="I22">
+        <f>I8*Shared_Lines!H7</f>
+        <v>0</v>
+      </c>
+      <c r="J22">
+        <f>J8*Shared_Lines!I7</f>
+        <v>0</v>
+      </c>
+      <c r="K22">
+        <f>K8*Shared_Lines!J7</f>
+        <v>0</v>
+      </c>
+      <c r="L22">
+        <f>L8*Shared_Lines!K7</f>
+        <v>2</v>
+      </c>
+      <c r="M22">
+        <f>M8*Shared_Lines!L7</f>
+        <v>0</v>
+      </c>
+      <c r="N22">
+        <f>N8*Shared_Lines!M7</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="2:14">
+      <c r="B23" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="C23">
+        <f>C9*Shared_Lines!B8</f>
+        <v>0</v>
+      </c>
+      <c r="D23">
+        <f>D9*Shared_Lines!C8</f>
+        <v>0</v>
+      </c>
+      <c r="E23">
+        <f>E9*Shared_Lines!D8</f>
+        <v>0</v>
+      </c>
+      <c r="F23">
+        <f>F9*Shared_Lines!E8</f>
+        <v>0</v>
+      </c>
+      <c r="G23">
+        <f>G9*Shared_Lines!F8</f>
+        <v>0</v>
+      </c>
+      <c r="H23">
+        <f>H9*Shared_Lines!G8</f>
+        <v>0</v>
+      </c>
+      <c r="I23">
+        <f>I9*Shared_Lines!H8</f>
+        <v>0</v>
+      </c>
+      <c r="J23">
+        <f>J9*Shared_Lines!I8</f>
+        <v>0</v>
+      </c>
+      <c r="K23">
+        <f>K9*Shared_Lines!J8</f>
+        <v>0</v>
+      </c>
+      <c r="L23">
+        <f>L9*Shared_Lines!K8</f>
+        <v>0</v>
+      </c>
+      <c r="M23">
+        <f>M9*Shared_Lines!L8</f>
+        <v>0</v>
+      </c>
+      <c r="N23">
+        <f>N9*Shared_Lines!M8</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="2:14">
+      <c r="B24" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="C24">
+        <f>C10*Shared_Lines!B9</f>
+        <v>0</v>
+      </c>
+      <c r="D24">
+        <f>D10*Shared_Lines!C9</f>
+        <v>0</v>
+      </c>
+      <c r="E24">
+        <f>E10*Shared_Lines!D9</f>
+        <v>0</v>
+      </c>
+      <c r="F24">
+        <f>F10*Shared_Lines!E9</f>
+        <v>0</v>
+      </c>
+      <c r="G24">
+        <f>G10*Shared_Lines!F9</f>
+        <v>0</v>
+      </c>
+      <c r="H24">
+        <f>H10*Shared_Lines!G9</f>
+        <v>0</v>
+      </c>
+      <c r="I24">
+        <f>I10*Shared_Lines!H9</f>
+        <v>0</v>
+      </c>
+      <c r="J24">
+        <f>J10*Shared_Lines!I9</f>
+        <v>0</v>
+      </c>
+      <c r="K24">
+        <f>K10*Shared_Lines!J9</f>
+        <v>0</v>
+      </c>
+      <c r="L24">
+        <f>L10*Shared_Lines!K9</f>
+        <v>0</v>
+      </c>
+      <c r="M24">
+        <f>M10*Shared_Lines!L9</f>
+        <v>0</v>
+      </c>
+      <c r="N24">
+        <f>N10*Shared_Lines!M9</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="2:14">
+      <c r="B25" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="C25">
+        <f>C11*Shared_Lines!B10</f>
+        <v>0</v>
+      </c>
+      <c r="D25">
+        <f>D11*Shared_Lines!C10</f>
+        <v>0</v>
+      </c>
+      <c r="E25">
+        <f>E11*Shared_Lines!D10</f>
+        <v>0</v>
+      </c>
+      <c r="F25">
+        <f>F11*Shared_Lines!E10</f>
+        <v>0</v>
+      </c>
+      <c r="G25">
+        <f>G11*Shared_Lines!F10</f>
+        <v>0</v>
+      </c>
+      <c r="H25">
+        <f>H11*Shared_Lines!G10</f>
+        <v>0</v>
+      </c>
+      <c r="I25">
+        <f>I11*Shared_Lines!H10</f>
+        <v>0</v>
+      </c>
+      <c r="J25">
+        <f>J11*Shared_Lines!I10</f>
+        <v>0</v>
+      </c>
+      <c r="K25">
+        <f>K11*Shared_Lines!J10</f>
+        <v>0</v>
+      </c>
+      <c r="L25">
+        <f>L11*Shared_Lines!K10</f>
+        <v>0</v>
+      </c>
+      <c r="M25">
+        <f>M11*Shared_Lines!L10</f>
+        <v>0</v>
+      </c>
+      <c r="N25">
+        <f>N11*Shared_Lines!M10</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="2:14">
+      <c r="B26" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C26">
+        <f>C12*Shared_Lines!B11</f>
+        <v>0</v>
+      </c>
+      <c r="D26">
+        <f>D12*Shared_Lines!C11</f>
+        <v>0</v>
+      </c>
+      <c r="E26">
+        <f>E12*Shared_Lines!D11</f>
+        <v>0</v>
+      </c>
+      <c r="F26">
+        <f>F12*Shared_Lines!E11</f>
+        <v>0</v>
+      </c>
+      <c r="G26">
+        <f>G12*Shared_Lines!F11</f>
+        <v>0</v>
+      </c>
+      <c r="H26">
+        <f>H12*Shared_Lines!G11</f>
+        <v>0</v>
+      </c>
+      <c r="I26">
+        <f>I12*Shared_Lines!H11</f>
+        <v>0</v>
+      </c>
+      <c r="J26">
+        <f>J12*Shared_Lines!I11</f>
+        <v>0</v>
+      </c>
+      <c r="K26">
+        <f>K12*Shared_Lines!J11</f>
+        <v>0</v>
+      </c>
+      <c r="L26">
+        <f>L12*Shared_Lines!K11</f>
+        <v>0</v>
+      </c>
+      <c r="M26">
+        <f>M12*Shared_Lines!L11</f>
+        <v>0</v>
+      </c>
+      <c r="N26">
+        <f>N12*Shared_Lines!M11</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="2:14">
+      <c r="B27" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="C27">
+        <f>C13*Shared_Lines!B12</f>
+        <v>0</v>
+      </c>
+      <c r="D27">
+        <f>D13*Shared_Lines!C12</f>
+        <v>0</v>
+      </c>
+      <c r="E27">
+        <f>E13*Shared_Lines!D12</f>
+        <v>0</v>
+      </c>
+      <c r="F27">
+        <f>F13*Shared_Lines!E12</f>
+        <v>0</v>
+      </c>
+      <c r="G27">
+        <f>G13*Shared_Lines!F12</f>
+        <v>0</v>
+      </c>
+      <c r="H27">
+        <f>H13*Shared_Lines!G12</f>
+        <v>0</v>
+      </c>
+      <c r="I27">
+        <f>I13*Shared_Lines!H12</f>
+        <v>0</v>
+      </c>
+      <c r="J27">
+        <f>J13*Shared_Lines!I12</f>
+        <v>0</v>
+      </c>
+      <c r="K27">
+        <f>K13*Shared_Lines!J12</f>
+        <v>0</v>
+      </c>
+      <c r="L27">
+        <f>L13*Shared_Lines!K12</f>
+        <v>0</v>
+      </c>
+      <c r="M27">
+        <f>M13*Shared_Lines!L12</f>
+        <v>0</v>
+      </c>
+      <c r="N27">
+        <f>N13*Shared_Lines!M12</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="2:14">
+      <c r="B28" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C28">
+        <f>C14*Shared_Lines!B13</f>
+        <v>0</v>
+      </c>
+      <c r="D28">
+        <f>D14*Shared_Lines!C13</f>
+        <v>0</v>
+      </c>
+      <c r="E28">
+        <f>E14*Shared_Lines!D13</f>
+        <v>0</v>
+      </c>
+      <c r="F28">
+        <f>F14*Shared_Lines!E13</f>
+        <v>0</v>
+      </c>
+      <c r="G28">
+        <f>G14*Shared_Lines!F13</f>
+        <v>0</v>
+      </c>
+      <c r="H28">
+        <f>H14*Shared_Lines!G13</f>
+        <v>0</v>
+      </c>
+      <c r="I28">
+        <f>I14*Shared_Lines!H13</f>
+        <v>0</v>
+      </c>
+      <c r="J28">
+        <f>J14*Shared_Lines!I13</f>
+        <v>0</v>
+      </c>
+      <c r="K28">
+        <f>K14*Shared_Lines!J13</f>
+        <v>0</v>
+      </c>
+      <c r="L28">
+        <f>L14*Shared_Lines!K13</f>
+        <v>0</v>
+      </c>
+      <c r="M28">
+        <f>M14*Shared_Lines!L13</f>
+        <v>0</v>
+      </c>
+      <c r="N28">
+        <f>N14*Shared_Lines!M13</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="2:14">
+      <c r="B30" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="G30" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="H30" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="I30" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="J30" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="K30" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="L30" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="M30" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="N30" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="31" spans="2:14">
+      <c r="B31" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C31" t="b">
+        <f>AND(C17=-Shared_Lines_Offset!B2,C17&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="D31" t="b">
+        <f>AND(D17=-Shared_Lines_Offset!C2,D17&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="E31" t="b">
+        <f>AND(E17=-Shared_Lines_Offset!D2,E17&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="F31" t="b">
+        <f>AND(F17=-Shared_Lines_Offset!E2,F17&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="G31" t="b">
+        <f>AND(G17=-Shared_Lines_Offset!F2,G17&lt;&gt;0)</f>
+        <v>1</v>
+      </c>
+      <c r="H31" t="b">
+        <f>AND(H17=-Shared_Lines_Offset!G2,H17&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="I31" t="b">
+        <f>AND(I17=-Shared_Lines_Offset!H2,I17&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="J31" t="b">
+        <f>AND(J17=-Shared_Lines_Offset!I2,J17&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="K31" t="b">
+        <f>AND(K17=-Shared_Lines_Offset!J2,K17&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="L31" t="b">
+        <f>AND(L17=-Shared_Lines_Offset!K2,L17&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="M31" t="b">
+        <f>AND(M17=-Shared_Lines_Offset!L2,M17&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="N31" t="b">
+        <f>AND(N17=-Shared_Lines_Offset!M2,N17&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="2:14">
+      <c r="B32" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C32" t="b">
+        <f>AND(C18=-Shared_Lines_Offset!B3,C18&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="D32" t="b">
+        <f>AND(D18=-Shared_Lines_Offset!C3,D18&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="E32" t="b">
+        <f>AND(E18=-Shared_Lines_Offset!D3,E18&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="F32" t="b">
+        <f>AND(F18=-Shared_Lines_Offset!E3,F18&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="G32" t="b">
+        <f>AND(G18=-Shared_Lines_Offset!F3,G18&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="H32" t="b">
+        <f>AND(H18=-Shared_Lines_Offset!G3,H18&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="I32" t="b">
+        <f>AND(I18=-Shared_Lines_Offset!H3,I18&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="J32" t="b">
+        <f>AND(J18=-Shared_Lines_Offset!I3,J18&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="K32" t="b">
+        <f>AND(K18=-Shared_Lines_Offset!J3,K18&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="L32" t="b">
+        <f>AND(L18=-Shared_Lines_Offset!K3,L18&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="M32" t="b">
+        <f>AND(M18=-Shared_Lines_Offset!L3,M18&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="N32" t="b">
+        <f>AND(N18=-Shared_Lines_Offset!M3,N18&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="2:14">
+      <c r="B33" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="C33" t="b">
+        <f>AND(C19=-Shared_Lines_Offset!B4,C19&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="D33" t="b">
+        <f>AND(D19=-Shared_Lines_Offset!C4,D19&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="E33" t="b">
+        <f>AND(E19=-Shared_Lines_Offset!D4,E19&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="F33" t="b">
+        <f>AND(F19=-Shared_Lines_Offset!E4,F19&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="G33" t="b">
+        <f>AND(G19=-Shared_Lines_Offset!F4,G19&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="H33" t="b">
+        <f>AND(H19=-Shared_Lines_Offset!G4,H19&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="I33" t="b">
+        <f>AND(I19=-Shared_Lines_Offset!H4,I19&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="J33" t="b">
+        <f>AND(J19=-Shared_Lines_Offset!I4,J19&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="K33" t="b">
+        <f>AND(K19=-Shared_Lines_Offset!J4,K19&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="L33" t="b">
+        <f>AND(L19=-Shared_Lines_Offset!K4,L19&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="M33" t="b">
+        <f>AND(M19=-Shared_Lines_Offset!L4,M19&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="N33" t="b">
+        <f>AND(N19=-Shared_Lines_Offset!M4,N19&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="2:14">
+      <c r="B34" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="C34" t="b">
+        <f>AND(C20=-Shared_Lines_Offset!B5,C20&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="D34" t="b">
+        <f>AND(D20=-Shared_Lines_Offset!C5,D20&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="E34" t="b">
+        <f>AND(E20=-Shared_Lines_Offset!D5,E20&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="F34" t="b">
+        <f>AND(F20=-Shared_Lines_Offset!E5,F20&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="G34" t="b">
+        <f>AND(G20=-Shared_Lines_Offset!F5,G20&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="H34" t="b">
+        <f>AND(H20=-Shared_Lines_Offset!G5,H20&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="I34" t="b">
+        <f>AND(I20=-Shared_Lines_Offset!H5,I20&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="J34" t="b">
+        <f>AND(J20=-Shared_Lines_Offset!I5,J20&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="K34" t="b">
+        <f>AND(K20=-Shared_Lines_Offset!J5,K20&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="L34" t="b">
+        <f>AND(L20=-Shared_Lines_Offset!K5,L20&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="M34" t="b">
+        <f>AND(M20=-Shared_Lines_Offset!L5,M20&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="N34" t="b">
+        <f>AND(N20=-Shared_Lines_Offset!M5,N20&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="2:14">
+      <c r="B35" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="C35" t="b">
+        <f>AND(C21=-Shared_Lines_Offset!B6,C21&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="D35" t="b">
+        <f>AND(D21=-Shared_Lines_Offset!C6,D21&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="E35" t="b">
+        <f>AND(E21=-Shared_Lines_Offset!D6,E21&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="F35" t="b">
+        <f>AND(F21=-Shared_Lines_Offset!E6,F21&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="G35" t="b">
+        <f>AND(G21=-Shared_Lines_Offset!F6,G21&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="H35" t="b">
+        <f>AND(H21=-Shared_Lines_Offset!G6,H21&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="I35" t="b">
+        <f>AND(I21=-Shared_Lines_Offset!H6,I21&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="J35" t="b">
+        <f>AND(J21=-Shared_Lines_Offset!I6,J21&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="K35" t="b">
+        <f>AND(K21=-Shared_Lines_Offset!J6,K21&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="L35" t="b">
+        <f>AND(L21=-Shared_Lines_Offset!K6,L21&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="M35" t="b">
+        <f>AND(M21=-Shared_Lines_Offset!L6,M21&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="N35" t="b">
+        <f>AND(N21=-Shared_Lines_Offset!M6,N21&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="2:14">
+      <c r="B36" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="C36" t="b">
+        <f>AND(C22=-Shared_Lines_Offset!B7,C22&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="D36" t="b">
+        <f>AND(D22=-Shared_Lines_Offset!C7,D22&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="E36" t="b">
+        <f>AND(E22=-Shared_Lines_Offset!D7,E22&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="F36" t="b">
+        <f>AND(F22=-Shared_Lines_Offset!E7,F22&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="G36" t="b">
+        <f>AND(G22=-Shared_Lines_Offset!F7,G22&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="H36" t="b">
+        <f>AND(H22=-Shared_Lines_Offset!G7,H22&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="I36" t="b">
+        <f>AND(I22=-Shared_Lines_Offset!H7,I22&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="J36" t="b">
+        <f>AND(J22=-Shared_Lines_Offset!I7,J22&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="K36" t="b">
+        <f>AND(K22=-Shared_Lines_Offset!J7,K22&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="L36" s="3" t="b">
+        <f>AND(L22=-Shared_Lines_Offset!K7,L22&lt;&gt;0)</f>
+        <v>1</v>
+      </c>
+      <c r="M36" t="b">
+        <f>AND(M22=-Shared_Lines_Offset!L7,M22&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="N36" t="b">
+        <f>AND(N22=-Shared_Lines_Offset!M7,N22&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="2:14">
+      <c r="B37" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="C37" t="b">
+        <f>AND(C23=-Shared_Lines_Offset!B8,C23&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="D37" t="b">
+        <f>AND(D23=-Shared_Lines_Offset!C8,D23&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="E37" t="b">
+        <f>AND(E23=-Shared_Lines_Offset!D8,E23&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="F37" t="b">
+        <f>AND(F23=-Shared_Lines_Offset!E8,F23&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="G37" t="b">
+        <f>AND(G23=-Shared_Lines_Offset!F8,G23&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="H37" t="b">
+        <f>AND(H23=-Shared_Lines_Offset!G8,H23&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="I37" t="b">
+        <f>AND(I23=-Shared_Lines_Offset!H8,I23&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="J37" t="b">
+        <f>AND(J23=-Shared_Lines_Offset!I8,J23&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="K37" t="b">
+        <f>AND(K23=-Shared_Lines_Offset!J8,K23&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="L37" t="b">
+        <f>AND(L23=-Shared_Lines_Offset!K8,L23&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="M37" t="b">
+        <f>AND(M23=-Shared_Lines_Offset!L8,M23&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="N37" t="b">
+        <f>AND(N23=-Shared_Lines_Offset!M8,N23&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="2:14">
+      <c r="B38" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="C38" t="b">
+        <f>AND(C24=-Shared_Lines_Offset!B9,C24&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="D38" t="b">
+        <f>AND(D24=-Shared_Lines_Offset!C9,D24&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="E38" t="b">
+        <f>AND(E24=-Shared_Lines_Offset!D9,E24&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="F38" t="b">
+        <f>AND(F24=-Shared_Lines_Offset!E9,F24&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="G38" t="b">
+        <f>AND(G24=-Shared_Lines_Offset!F9,G24&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="H38" t="b">
+        <f>AND(H24=-Shared_Lines_Offset!G9,H24&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="I38" t="b">
+        <f>AND(I24=-Shared_Lines_Offset!H9,I24&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="J38" t="b">
+        <f>AND(J24=-Shared_Lines_Offset!I9,J24&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="K38" t="b">
+        <f>AND(K24=-Shared_Lines_Offset!J9,K24&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="L38" t="b">
+        <f>AND(L24=-Shared_Lines_Offset!K9,L24&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="M38" t="b">
+        <f>AND(M24=-Shared_Lines_Offset!L9,M24&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="N38" t="b">
+        <f>AND(N24=-Shared_Lines_Offset!M9,N24&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="2:14">
+      <c r="B39" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="C39" t="b">
+        <f>AND(C25=-Shared_Lines_Offset!B10,C25&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="D39" t="b">
+        <f>AND(D25=-Shared_Lines_Offset!C10,D25&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="E39" t="b">
+        <f>AND(E25=-Shared_Lines_Offset!D10,E25&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="F39" t="b">
+        <f>AND(F25=-Shared_Lines_Offset!E10,F25&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="G39" t="b">
+        <f>AND(G25=-Shared_Lines_Offset!F10,G25&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="H39" t="b">
+        <f>AND(H25=-Shared_Lines_Offset!G10,H25&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="I39" t="b">
+        <f>AND(I25=-Shared_Lines_Offset!H10,I25&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="J39" t="b">
+        <f>AND(J25=-Shared_Lines_Offset!I10,J25&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="K39" t="b">
+        <f>AND(K25=-Shared_Lines_Offset!J10,K25&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="L39" t="b">
+        <f>AND(L25=-Shared_Lines_Offset!K10,L25&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="M39" t="b">
+        <f>AND(M25=-Shared_Lines_Offset!L10,M25&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="N39" t="b">
+        <f>AND(N25=-Shared_Lines_Offset!M10,N25&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="2:14">
+      <c r="B40" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C40" t="b">
+        <f>AND(C26=-Shared_Lines_Offset!B11,C26&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="D40" t="b">
+        <f>AND(D26=-Shared_Lines_Offset!C11,D26&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="E40" t="b">
+        <f>AND(E26=-Shared_Lines_Offset!D11,E26&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="F40" t="b">
+        <f>AND(F26=-Shared_Lines_Offset!E11,F26&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="G40" t="b">
+        <f>AND(G26=-Shared_Lines_Offset!F11,G26&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="H40" t="b">
+        <f>AND(H26=-Shared_Lines_Offset!G11,H26&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="I40" t="b">
+        <f>AND(I26=-Shared_Lines_Offset!H11,I26&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="J40" t="b">
+        <f>AND(J26=-Shared_Lines_Offset!I11,J26&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="K40" t="b">
+        <f>AND(K26=-Shared_Lines_Offset!J11,K26&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="L40" t="b">
+        <f>AND(L26=-Shared_Lines_Offset!K11,L26&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="M40" t="b">
+        <f>AND(M26=-Shared_Lines_Offset!L11,M26&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="N40" t="b">
+        <f>AND(N26=-Shared_Lines_Offset!M11,N26&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="2:14">
+      <c r="B41" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="C41" t="b">
+        <f>AND(C27=-Shared_Lines_Offset!B12,C27&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="D41" t="b">
+        <f>AND(D27=-Shared_Lines_Offset!C12,D27&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="E41" t="b">
+        <f>AND(E27=-Shared_Lines_Offset!D12,E27&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="F41" t="b">
+        <f>AND(F27=-Shared_Lines_Offset!E12,F27&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="G41" t="b">
+        <f>AND(G27=-Shared_Lines_Offset!F12,G27&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="H41" t="b">
+        <f>AND(H27=-Shared_Lines_Offset!G12,H27&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="I41" t="b">
+        <f>AND(I27=-Shared_Lines_Offset!H12,I27&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="J41" t="b">
+        <f>AND(J27=-Shared_Lines_Offset!I12,J27&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="K41" t="b">
+        <f>AND(K27=-Shared_Lines_Offset!J12,K27&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="L41" t="b">
+        <f>AND(L27=-Shared_Lines_Offset!K12,L27&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="M41" t="b">
+        <f>AND(M27=-Shared_Lines_Offset!L12,M27&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="N41" t="b">
+        <f>AND(N27=-Shared_Lines_Offset!M12,N27&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="2:14">
+      <c r="B42" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C42" t="b">
+        <f>AND(C28=-Shared_Lines_Offset!B13,C28&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="D42" t="b">
+        <f>AND(D28=-Shared_Lines_Offset!C13,D28&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="E42" t="b">
+        <f>AND(E28=-Shared_Lines_Offset!D13,E28&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="F42" t="b">
+        <f>AND(F28=-Shared_Lines_Offset!E13,F28&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="G42" t="b">
+        <f>AND(G28=-Shared_Lines_Offset!F13,G28&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="H42" t="b">
+        <f>AND(H28=-Shared_Lines_Offset!G13,H28&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="I42" t="b">
+        <f>AND(I28=-Shared_Lines_Offset!H13,I28&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="J42" t="b">
+        <f>AND(J28=-Shared_Lines_Offset!I13,J28&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="K42" t="b">
+        <f>AND(K28=-Shared_Lines_Offset!J13,K28&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="L42" t="b">
+        <f>AND(L28=-Shared_Lines_Offset!K13,L28&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="M42" t="b">
+        <f>AND(M28=-Shared_Lines_Offset!L13,M28&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="N42" t="b">
+        <f>AND(N28=-Shared_Lines_Offset!M13,N28&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="2:14">
+      <c r="B44" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="45" spans="2:14">
+      <c r="B45" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O16" sqref="O16"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="B50" sqref="B50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -6639,34 +8854,34 @@
         <v>4</v>
       </c>
       <c r="D2" s="1">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E2" s="1">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="F2" s="1">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="G2" s="1">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="H2" s="1">
         <v>9</v>
       </c>
       <c r="I2" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J2" s="1">
+        <v>11</v>
+      </c>
+      <c r="K2" s="1">
+        <v>4</v>
+      </c>
+      <c r="L2" s="1">
         <v>9</v>
       </c>
-      <c r="K2" s="1">
-        <v>8</v>
-      </c>
-      <c r="L2" s="1">
-        <v>7</v>
-      </c>
       <c r="M2" s="1">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="N2" s="1">
         <v>9</v>
@@ -6685,43 +8900,43 @@
       </c>
       <c r="D3">
         <f t="shared" ref="D3:N14" si="0">$B3-D$2</f>
+        <v>-5</v>
+      </c>
+      <c r="E3">
+        <f t="shared" si="0"/>
+        <v>-6</v>
+      </c>
+      <c r="F3">
+        <f t="shared" si="0"/>
+        <v>-5</v>
+      </c>
+      <c r="G3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <f t="shared" si="0"/>
+        <v>-5</v>
+      </c>
+      <c r="I3">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="J3">
+        <f t="shared" si="0"/>
         <v>-7</v>
       </c>
-      <c r="E3">
-        <f t="shared" si="0"/>
-        <v>-1</v>
-      </c>
-      <c r="F3">
-        <f t="shared" si="0"/>
-        <v>-1</v>
-      </c>
-      <c r="G3">
-        <f t="shared" si="0"/>
-        <v>-2</v>
-      </c>
-      <c r="H3">
+      <c r="K3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L3">
         <f t="shared" si="0"/>
         <v>-5</v>
       </c>
-      <c r="I3">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="J3">
-        <f t="shared" si="0"/>
-        <v>-5</v>
-      </c>
-      <c r="K3">
-        <f t="shared" si="0"/>
-        <v>-4</v>
-      </c>
-      <c r="L3">
-        <f t="shared" si="0"/>
-        <v>-3</v>
-      </c>
       <c r="M3">
         <f t="shared" si="0"/>
-        <v>-7</v>
+        <v>-6</v>
       </c>
       <c r="N3">
         <f t="shared" si="0"/>
@@ -6733,11 +8948,11 @@
         <v>16</v>
       </c>
       <c r="B4" s="1">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C4">
         <f t="shared" ref="C4:C14" si="1">$B4-C$2</f>
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D4">
         <f t="shared" si="0"/>
@@ -6745,11 +8960,11 @@
       </c>
       <c r="E4">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>-1</v>
       </c>
       <c r="F4">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="G4">
         <f t="shared" si="0"/>
@@ -6757,7 +8972,7 @@
       </c>
       <c r="H4">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I4">
         <f t="shared" si="0"/>
@@ -6765,23 +8980,23 @@
       </c>
       <c r="J4">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>-2</v>
       </c>
       <c r="K4">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="L4">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="M4">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="N4">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:14">
@@ -6789,55 +9004,55 @@
         <v>95</v>
       </c>
       <c r="B5" s="1">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C5">
         <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="D5">
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="D5">
-        <f t="shared" si="0"/>
-        <v>-6</v>
-      </c>
       <c r="E5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G5">
         <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="H5">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="I5">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="J5">
+        <f t="shared" si="0"/>
         <v>-1</v>
       </c>
-      <c r="H5">
-        <f t="shared" si="0"/>
-        <v>-4</v>
-      </c>
-      <c r="I5">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="J5">
-        <f t="shared" si="0"/>
-        <v>-4</v>
-      </c>
       <c r="K5">
         <f t="shared" si="0"/>
-        <v>-3</v>
+        <v>6</v>
       </c>
       <c r="L5">
         <f t="shared" si="0"/>
-        <v>-2</v>
+        <v>1</v>
       </c>
       <c r="M5">
         <f t="shared" si="0"/>
-        <v>-6</v>
+        <v>0</v>
       </c>
       <c r="N5">
         <f t="shared" si="0"/>
-        <v>-4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:14">
@@ -6845,19 +9060,19 @@
         <v>96</v>
       </c>
       <c r="B6" s="1">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="C6">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D6">
         <f t="shared" si="0"/>
-        <v>-6</v>
+        <v>0</v>
       </c>
       <c r="E6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="F6">
         <f t="shared" si="0"/>
@@ -6865,35 +9080,35 @@
       </c>
       <c r="G6">
         <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="H6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I6">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="J6">
+        <f t="shared" si="0"/>
+        <v>-2</v>
+      </c>
+      <c r="K6">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="L6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M6">
+        <f t="shared" si="0"/>
         <v>-1</v>
       </c>
-      <c r="H6">
-        <f t="shared" si="0"/>
-        <v>-4</v>
-      </c>
-      <c r="I6">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="J6">
-        <f t="shared" si="0"/>
-        <v>-4</v>
-      </c>
-      <c r="K6">
-        <f t="shared" si="0"/>
-        <v>-3</v>
-      </c>
-      <c r="L6">
-        <f t="shared" si="0"/>
-        <v>-2</v>
-      </c>
-      <c r="M6">
-        <f t="shared" si="0"/>
-        <v>-6</v>
-      </c>
       <c r="N6">
         <f t="shared" si="0"/>
-        <v>-4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:14">
@@ -6901,11 +9116,11 @@
         <v>97</v>
       </c>
       <c r="B7" s="1">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C7">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D7">
         <f t="shared" si="0"/>
@@ -6913,11 +9128,11 @@
       </c>
       <c r="E7">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>-6</v>
       </c>
       <c r="F7">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>-5</v>
       </c>
       <c r="G7">
         <f t="shared" si="0"/>
@@ -6925,7 +9140,7 @@
       </c>
       <c r="H7">
         <f t="shared" si="0"/>
-        <v>-3</v>
+        <v>-5</v>
       </c>
       <c r="I7">
         <f t="shared" si="0"/>
@@ -6933,23 +9148,23 @@
       </c>
       <c r="J7">
         <f t="shared" si="0"/>
-        <v>-3</v>
+        <v>-7</v>
       </c>
       <c r="K7">
         <f t="shared" si="0"/>
-        <v>-2</v>
+        <v>0</v>
       </c>
       <c r="L7">
         <f t="shared" si="0"/>
-        <v>-1</v>
+        <v>-5</v>
       </c>
       <c r="M7">
         <f t="shared" si="0"/>
+        <v>-6</v>
+      </c>
+      <c r="N7">
+        <f t="shared" si="0"/>
         <v>-5</v>
-      </c>
-      <c r="N7">
-        <f t="shared" si="0"/>
-        <v>-3</v>
       </c>
     </row>
     <row r="8" spans="1:14">
@@ -6965,43 +9180,43 @@
       </c>
       <c r="D8">
         <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+      <c r="F8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="H8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I8">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="J8">
+        <f t="shared" si="0"/>
         <v>-2</v>
       </c>
-      <c r="E8">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="F8">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="G8">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="H8">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I8">
-        <f t="shared" si="0"/>
-        <v>7</v>
-      </c>
-      <c r="J8">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
       <c r="K8">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="L8">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M8">
         <f t="shared" si="0"/>
-        <v>-2</v>
+        <v>-1</v>
       </c>
       <c r="N8">
         <f t="shared" si="0"/>
@@ -7013,11 +9228,11 @@
         <v>99</v>
       </c>
       <c r="B9" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C9">
         <f t="shared" si="1"/>
-        <v>-2</v>
+        <v>-4</v>
       </c>
       <c r="D9">
         <f t="shared" si="0"/>
@@ -7025,11 +9240,11 @@
       </c>
       <c r="E9">
         <f t="shared" si="0"/>
-        <v>-3</v>
+        <v>-10</v>
       </c>
       <c r="F9">
         <f t="shared" si="0"/>
-        <v>-3</v>
+        <v>-9</v>
       </c>
       <c r="G9">
         <f t="shared" si="0"/>
@@ -7037,7 +9252,7 @@
       </c>
       <c r="H9">
         <f t="shared" si="0"/>
-        <v>-7</v>
+        <v>-9</v>
       </c>
       <c r="I9">
         <f t="shared" si="0"/>
@@ -7045,23 +9260,23 @@
       </c>
       <c r="J9">
         <f t="shared" si="0"/>
-        <v>-7</v>
+        <v>-11</v>
       </c>
       <c r="K9">
         <f t="shared" si="0"/>
-        <v>-6</v>
+        <v>-4</v>
       </c>
       <c r="L9">
         <f t="shared" si="0"/>
-        <v>-5</v>
+        <v>-9</v>
       </c>
       <c r="M9">
         <f t="shared" si="0"/>
+        <v>-10</v>
+      </c>
+      <c r="N9">
+        <f t="shared" si="0"/>
         <v>-9</v>
-      </c>
-      <c r="N9">
-        <f t="shared" si="0"/>
-        <v>-7</v>
       </c>
     </row>
     <row r="10" spans="1:14">
@@ -7069,55 +9284,55 @@
         <v>100</v>
       </c>
       <c r="B10" s="1">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C10">
         <f t="shared" si="1"/>
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D10">
         <f t="shared" si="0"/>
-        <v>-2</v>
+        <v>2</v>
       </c>
       <c r="E10">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="F10">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G10">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="H10">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I10">
         <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="J10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K10">
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="J10">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="K10">
+      <c r="L10">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="M10">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="L10">
+      <c r="N10">
         <f t="shared" si="0"/>
         <v>2</v>
-      </c>
-      <c r="M10">
-        <f t="shared" si="0"/>
-        <v>-2</v>
-      </c>
-      <c r="N10">
-        <f t="shared" si="0"/>
-        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:14">
@@ -7125,39 +9340,39 @@
         <v>101</v>
       </c>
       <c r="B11" s="1">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C11">
         <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <f t="shared" si="0"/>
+        <v>-5</v>
+      </c>
+      <c r="E11">
+        <f t="shared" si="0"/>
+        <v>-6</v>
+      </c>
+      <c r="F11">
+        <f t="shared" si="0"/>
+        <v>-5</v>
+      </c>
+      <c r="G11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H11">
+        <f t="shared" si="0"/>
+        <v>-5</v>
+      </c>
+      <c r="I11">
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="D11">
-        <f t="shared" si="0"/>
-        <v>-3</v>
-      </c>
-      <c r="E11">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="F11">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="G11">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="H11">
-        <f t="shared" si="0"/>
-        <v>-1</v>
-      </c>
-      <c r="I11">
-        <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
       <c r="J11">
         <f t="shared" si="0"/>
-        <v>-1</v>
+        <v>-7</v>
       </c>
       <c r="K11">
         <f t="shared" si="0"/>
@@ -7165,15 +9380,15 @@
       </c>
       <c r="L11">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>-5</v>
       </c>
       <c r="M11">
         <f t="shared" si="0"/>
-        <v>-3</v>
+        <v>-6</v>
       </c>
       <c r="N11">
         <f t="shared" si="0"/>
-        <v>-1</v>
+        <v>-5</v>
       </c>
     </row>
     <row r="12" spans="1:14">
@@ -7181,55 +9396,55 @@
         <v>102</v>
       </c>
       <c r="B12" s="1">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C12">
         <f t="shared" si="1"/>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D12">
         <f t="shared" si="0"/>
-        <v>-4</v>
+        <v>0</v>
       </c>
       <c r="E12">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>-1</v>
       </c>
       <c r="F12">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G12">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="H12">
         <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I12">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="J12">
+        <f t="shared" si="0"/>
         <v>-2</v>
       </c>
-      <c r="I12">
+      <c r="K12">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="J12">
-        <f t="shared" si="0"/>
-        <v>-2</v>
-      </c>
-      <c r="K12">
+      <c r="L12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M12">
         <f t="shared" si="0"/>
         <v>-1</v>
       </c>
-      <c r="L12">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M12">
-        <f t="shared" si="0"/>
-        <v>-4</v>
-      </c>
       <c r="N12">
         <f t="shared" si="0"/>
-        <v>-2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:14">
@@ -7237,47 +9452,47 @@
         <v>103</v>
       </c>
       <c r="B13" s="1">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C13">
         <f t="shared" si="1"/>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D13">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E13">
         <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F13">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="G13">
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="F13">
+      <c r="H13">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="I13">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="J13">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+      <c r="K13">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="G13">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="H13">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="I13">
-        <f t="shared" si="0"/>
-        <v>9</v>
-      </c>
-      <c r="J13">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="K13">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
       <c r="L13">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="M13">
         <f t="shared" si="0"/>
@@ -7285,7 +9500,7 @@
       </c>
       <c r="N13">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:14">
@@ -7301,43 +9516,43 @@
       </c>
       <c r="D14">
         <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E14">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+      <c r="F14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G14">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="H14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I14">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="J14">
+        <f t="shared" si="0"/>
         <v>-2</v>
       </c>
-      <c r="E14">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="F14">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="G14">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="H14">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I14">
-        <f t="shared" si="0"/>
-        <v>7</v>
-      </c>
-      <c r="J14">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
       <c r="K14">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="L14">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M14">
         <f t="shared" si="0"/>
-        <v>-2</v>
+        <v>-1</v>
       </c>
       <c r="N14">
         <f t="shared" si="0"/>
@@ -7407,7 +9622,7 @@
       </c>
       <c r="G17">
         <f>G3*Shared_Lines!F2</f>
-        <v>-2</v>
+        <v>0</v>
       </c>
       <c r="H17">
         <f>H3*Shared_Lines!G2</f>
@@ -7423,7 +9638,7 @@
       </c>
       <c r="K17">
         <f>K3*Shared_Lines!J2</f>
-        <v>-4</v>
+        <v>0</v>
       </c>
       <c r="L17">
         <f>L3*Shared_Lines!K2</f>
@@ -7431,7 +9646,7 @@
       </c>
       <c r="M17">
         <f>M3*Shared_Lines!L2</f>
-        <v>-7</v>
+        <v>-6</v>
       </c>
       <c r="N17">
         <f>N3*Shared_Lines!M2</f>
@@ -7464,7 +9679,7 @@
       </c>
       <c r="H18">
         <f>H4*Shared_Lines!G3</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I18">
         <f>I4*Shared_Lines!H3</f>
@@ -7480,7 +9695,7 @@
       </c>
       <c r="L18">
         <f>L4*Shared_Lines!K3</f>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="M18">
         <f>M4*Shared_Lines!L3</f>
@@ -7488,7 +9703,7 @@
       </c>
       <c r="N18">
         <f>N4*Shared_Lines!M3</f>
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="2:14">
@@ -7537,7 +9752,7 @@
       </c>
       <c r="M19">
         <f>M5*Shared_Lines!L4</f>
-        <v>-6</v>
+        <v>0</v>
       </c>
       <c r="N19">
         <f>N5*Shared_Lines!M4</f>
@@ -7594,7 +9809,7 @@
       </c>
       <c r="N20">
         <f>N6*Shared_Lines!M5</f>
-        <v>-4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21" spans="2:14">
@@ -7635,7 +9850,7 @@
       </c>
       <c r="K21">
         <f>K7*Shared_Lines!J6</f>
-        <v>-2</v>
+        <v>0</v>
       </c>
       <c r="L21">
         <f>L7*Shared_Lines!K6</f>
@@ -7692,7 +9907,7 @@
       </c>
       <c r="L22">
         <f>L8*Shared_Lines!K7</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M22">
         <f>M8*Shared_Lines!L7</f>
@@ -8067,51 +10282,51 @@
         <v>22</v>
       </c>
       <c r="C31" t="b">
-        <f>AND(C17=Shared_Lines_Offset!B2,C17&lt;&gt;0)</f>
+        <f>AND(C17=-Shared_Lines_Offset!B2,C17&lt;&gt;0)</f>
         <v>0</v>
       </c>
       <c r="D31" t="b">
-        <f>AND(D17=Shared_Lines_Offset!C2,D17&lt;&gt;0)</f>
+        <f>AND(D17=-Shared_Lines_Offset!C2,D17&lt;&gt;0)</f>
         <v>0</v>
       </c>
       <c r="E31" t="b">
-        <f>AND(E17=Shared_Lines_Offset!D2,E17&lt;&gt;0)</f>
+        <f>AND(E17=-Shared_Lines_Offset!D2,E17&lt;&gt;0)</f>
         <v>0</v>
       </c>
       <c r="F31" t="b">
-        <f>AND(F17=Shared_Lines_Offset!E2,F17&lt;&gt;0)</f>
+        <f>AND(F17=-Shared_Lines_Offset!E2,F17&lt;&gt;0)</f>
         <v>0</v>
       </c>
       <c r="G31" t="b">
-        <f>AND(G17=Shared_Lines_Offset!F2,G17&lt;&gt;0)</f>
+        <f>AND(G17=-Shared_Lines_Offset!F2,G17&lt;&gt;0)</f>
         <v>0</v>
       </c>
       <c r="H31" t="b">
-        <f>AND(H17=Shared_Lines_Offset!G2,H17&lt;&gt;0)</f>
+        <f>AND(H17=-Shared_Lines_Offset!G2,H17&lt;&gt;0)</f>
         <v>0</v>
       </c>
       <c r="I31" t="b">
-        <f>AND(I17=Shared_Lines_Offset!H2,I17&lt;&gt;0)</f>
+        <f>AND(I17=-Shared_Lines_Offset!H2,I17&lt;&gt;0)</f>
         <v>0</v>
       </c>
       <c r="J31" t="b">
-        <f>AND(J17=Shared_Lines_Offset!I2,J17&lt;&gt;0)</f>
+        <f>AND(J17=-Shared_Lines_Offset!I2,J17&lt;&gt;0)</f>
         <v>0</v>
       </c>
       <c r="K31" t="b">
-        <f>AND(K17=Shared_Lines_Offset!J2,K17&lt;&gt;0)</f>
+        <f>AND(K17=-Shared_Lines_Offset!J2,K17&lt;&gt;0)</f>
         <v>0</v>
       </c>
       <c r="L31" t="b">
-        <f>AND(L17=Shared_Lines_Offset!K2,L17&lt;&gt;0)</f>
+        <f>AND(L17=-Shared_Lines_Offset!K2,L17&lt;&gt;0)</f>
         <v>0</v>
       </c>
       <c r="M31" t="b">
-        <f>AND(M17=Shared_Lines_Offset!L2,M17&lt;&gt;0)</f>
+        <f>AND(M17=-Shared_Lines_Offset!L2,M17&lt;&gt;0)</f>
         <v>0</v>
       </c>
       <c r="N31" t="b">
-        <f>AND(N17=Shared_Lines_Offset!M2,N17&lt;&gt;0)</f>
+        <f>AND(N17=-Shared_Lines_Offset!M2,N17&lt;&gt;0)</f>
         <v>0</v>
       </c>
     </row>
@@ -8120,51 +10335,51 @@
         <v>16</v>
       </c>
       <c r="C32" t="b">
-        <f>AND(C18=Shared_Lines_Offset!B3,C18&lt;&gt;0)</f>
+        <f>AND(C18=-Shared_Lines_Offset!B3,C18&lt;&gt;0)</f>
         <v>0</v>
       </c>
       <c r="D32" t="b">
-        <f>AND(D18=Shared_Lines_Offset!C3,D18&lt;&gt;0)</f>
+        <f>AND(D18=-Shared_Lines_Offset!C3,D18&lt;&gt;0)</f>
         <v>0</v>
       </c>
       <c r="E32" t="b">
-        <f>AND(E18=Shared_Lines_Offset!D3,E18&lt;&gt;0)</f>
+        <f>AND(E18=-Shared_Lines_Offset!D3,E18&lt;&gt;0)</f>
         <v>0</v>
       </c>
       <c r="F32" t="b">
-        <f>AND(F18=Shared_Lines_Offset!E3,F18&lt;&gt;0)</f>
+        <f>AND(F18=-Shared_Lines_Offset!E3,F18&lt;&gt;0)</f>
         <v>0</v>
       </c>
       <c r="G32" t="b">
-        <f>AND(G18=Shared_Lines_Offset!F3,G18&lt;&gt;0)</f>
+        <f>AND(G18=-Shared_Lines_Offset!F3,G18&lt;&gt;0)</f>
         <v>0</v>
       </c>
       <c r="H32" t="b">
-        <f>AND(H18=Shared_Lines_Offset!G3,H18&lt;&gt;0)</f>
+        <f>AND(H18=-Shared_Lines_Offset!G3,H18&lt;&gt;0)</f>
         <v>0</v>
       </c>
       <c r="I32" t="b">
-        <f>AND(I18=Shared_Lines_Offset!H3,I18&lt;&gt;0)</f>
+        <f>AND(I18=-Shared_Lines_Offset!H3,I18&lt;&gt;0)</f>
         <v>0</v>
       </c>
       <c r="J32" t="b">
-        <f>AND(J18=Shared_Lines_Offset!I3,J18&lt;&gt;0)</f>
+        <f>AND(J18=-Shared_Lines_Offset!I3,J18&lt;&gt;0)</f>
         <v>0</v>
       </c>
       <c r="K32" t="b">
-        <f>AND(K18=Shared_Lines_Offset!J3,K18&lt;&gt;0)</f>
+        <f>AND(K18=-Shared_Lines_Offset!J3,K18&lt;&gt;0)</f>
         <v>0</v>
       </c>
       <c r="L32" t="b">
-        <f>AND(L18=Shared_Lines_Offset!K3,L18&lt;&gt;0)</f>
+        <f>AND(L18=-Shared_Lines_Offset!K3,L18&lt;&gt;0)</f>
         <v>0</v>
       </c>
       <c r="M32" t="b">
-        <f>AND(M18=Shared_Lines_Offset!L3,M18&lt;&gt;0)</f>
+        <f>AND(M18=-Shared_Lines_Offset!L3,M18&lt;&gt;0)</f>
         <v>0</v>
       </c>
       <c r="N32" t="b">
-        <f>AND(N18=Shared_Lines_Offset!M3,N18&lt;&gt;0)</f>
+        <f>AND(N18=-Shared_Lines_Offset!M3,N18&lt;&gt;0)</f>
         <v>0</v>
       </c>
     </row>
@@ -8173,51 +10388,51 @@
         <v>95</v>
       </c>
       <c r="C33" t="b">
-        <f>AND(C19=Shared_Lines_Offset!B4,C19&lt;&gt;0)</f>
+        <f>AND(C19=-Shared_Lines_Offset!B4,C19&lt;&gt;0)</f>
         <v>0</v>
       </c>
       <c r="D33" t="b">
-        <f>AND(D19=Shared_Lines_Offset!C4,D19&lt;&gt;0)</f>
+        <f>AND(D19=-Shared_Lines_Offset!C4,D19&lt;&gt;0)</f>
         <v>0</v>
       </c>
       <c r="E33" t="b">
-        <f>AND(E19=Shared_Lines_Offset!D4,E19&lt;&gt;0)</f>
+        <f>AND(E19=-Shared_Lines_Offset!D4,E19&lt;&gt;0)</f>
         <v>0</v>
       </c>
       <c r="F33" t="b">
-        <f>AND(F19=Shared_Lines_Offset!E4,F19&lt;&gt;0)</f>
+        <f>AND(F19=-Shared_Lines_Offset!E4,F19&lt;&gt;0)</f>
         <v>0</v>
       </c>
       <c r="G33" t="b">
-        <f>AND(G19=Shared_Lines_Offset!F4,G19&lt;&gt;0)</f>
+        <f>AND(G19=-Shared_Lines_Offset!F4,G19&lt;&gt;0)</f>
         <v>0</v>
       </c>
       <c r="H33" t="b">
-        <f>AND(H19=Shared_Lines_Offset!G4,H19&lt;&gt;0)</f>
+        <f>AND(H19=-Shared_Lines_Offset!G4,H19&lt;&gt;0)</f>
         <v>0</v>
       </c>
       <c r="I33" t="b">
-        <f>AND(I19=Shared_Lines_Offset!H4,I19&lt;&gt;0)</f>
+        <f>AND(I19=-Shared_Lines_Offset!H4,I19&lt;&gt;0)</f>
         <v>0</v>
       </c>
       <c r="J33" t="b">
-        <f>AND(J19=Shared_Lines_Offset!I4,J19&lt;&gt;0)</f>
+        <f>AND(J19=-Shared_Lines_Offset!I4,J19&lt;&gt;0)</f>
         <v>0</v>
       </c>
       <c r="K33" t="b">
-        <f>AND(K19=Shared_Lines_Offset!J4,K19&lt;&gt;0)</f>
+        <f>AND(K19=-Shared_Lines_Offset!J4,K19&lt;&gt;0)</f>
         <v>0</v>
       </c>
       <c r="L33" t="b">
-        <f>AND(L19=Shared_Lines_Offset!K4,L19&lt;&gt;0)</f>
+        <f>AND(L19=-Shared_Lines_Offset!K4,L19&lt;&gt;0)</f>
         <v>0</v>
       </c>
       <c r="M33" t="b">
-        <f>AND(M19=Shared_Lines_Offset!L4,M19&lt;&gt;0)</f>
+        <f>AND(M19=-Shared_Lines_Offset!L4,M19&lt;&gt;0)</f>
         <v>0</v>
       </c>
       <c r="N33" t="b">
-        <f>AND(N19=Shared_Lines_Offset!M4,N19&lt;&gt;0)</f>
+        <f>AND(N19=-Shared_Lines_Offset!M4,N19&lt;&gt;0)</f>
         <v>0</v>
       </c>
     </row>
@@ -8226,51 +10441,51 @@
         <v>96</v>
       </c>
       <c r="C34" t="b">
-        <f>AND(C20=Shared_Lines_Offset!B5,C20&lt;&gt;0)</f>
+        <f>AND(C20=-Shared_Lines_Offset!B5,C20&lt;&gt;0)</f>
         <v>0</v>
       </c>
       <c r="D34" t="b">
-        <f>AND(D20=Shared_Lines_Offset!C5,D20&lt;&gt;0)</f>
+        <f>AND(D20=-Shared_Lines_Offset!C5,D20&lt;&gt;0)</f>
         <v>0</v>
       </c>
       <c r="E34" t="b">
-        <f>AND(E20=Shared_Lines_Offset!D5,E20&lt;&gt;0)</f>
+        <f>AND(E20=-Shared_Lines_Offset!D5,E20&lt;&gt;0)</f>
         <v>0</v>
       </c>
       <c r="F34" t="b">
-        <f>AND(F20=Shared_Lines_Offset!E5,F20&lt;&gt;0)</f>
+        <f>AND(F20=-Shared_Lines_Offset!E5,F20&lt;&gt;0)</f>
         <v>0</v>
       </c>
       <c r="G34" t="b">
-        <f>AND(G20=Shared_Lines_Offset!F5,G20&lt;&gt;0)</f>
+        <f>AND(G20=-Shared_Lines_Offset!F5,G20&lt;&gt;0)</f>
         <v>0</v>
       </c>
       <c r="H34" t="b">
-        <f>AND(H20=Shared_Lines_Offset!G5,H20&lt;&gt;0)</f>
+        <f>AND(H20=-Shared_Lines_Offset!G5,H20&lt;&gt;0)</f>
         <v>0</v>
       </c>
       <c r="I34" t="b">
-        <f>AND(I20=Shared_Lines_Offset!H5,I20&lt;&gt;0)</f>
+        <f>AND(I20=-Shared_Lines_Offset!H5,I20&lt;&gt;0)</f>
         <v>0</v>
       </c>
       <c r="J34" t="b">
-        <f>AND(J20=Shared_Lines_Offset!I5,J20&lt;&gt;0)</f>
+        <f>AND(J20=-Shared_Lines_Offset!I5,J20&lt;&gt;0)</f>
         <v>0</v>
       </c>
       <c r="K34" t="b">
-        <f>AND(K20=Shared_Lines_Offset!J5,K20&lt;&gt;0)</f>
+        <f>AND(K20=-Shared_Lines_Offset!J5,K20&lt;&gt;0)</f>
         <v>0</v>
       </c>
       <c r="L34" t="b">
-        <f>AND(L20=Shared_Lines_Offset!K5,L20&lt;&gt;0)</f>
+        <f>AND(L20=-Shared_Lines_Offset!K5,L20&lt;&gt;0)</f>
         <v>0</v>
       </c>
       <c r="M34" t="b">
-        <f>AND(M20=Shared_Lines_Offset!L5,M20&lt;&gt;0)</f>
+        <f>AND(M20=-Shared_Lines_Offset!L5,M20&lt;&gt;0)</f>
         <v>0</v>
       </c>
       <c r="N34" t="b">
-        <f>AND(N20=Shared_Lines_Offset!M5,N20&lt;&gt;0)</f>
+        <f>AND(N20=-Shared_Lines_Offset!M5,N20&lt;&gt;0)</f>
         <v>0</v>
       </c>
     </row>
@@ -8279,51 +10494,51 @@
         <v>97</v>
       </c>
       <c r="C35" t="b">
-        <f>AND(C21=Shared_Lines_Offset!B6,C21&lt;&gt;0)</f>
+        <f>AND(C21=-Shared_Lines_Offset!B6,C21&lt;&gt;0)</f>
         <v>0</v>
       </c>
       <c r="D35" t="b">
-        <f>AND(D21=Shared_Lines_Offset!C6,D21&lt;&gt;0)</f>
+        <f>AND(D21=-Shared_Lines_Offset!C6,D21&lt;&gt;0)</f>
         <v>0</v>
       </c>
       <c r="E35" t="b">
-        <f>AND(E21=Shared_Lines_Offset!D6,E21&lt;&gt;0)</f>
+        <f>AND(E21=-Shared_Lines_Offset!D6,E21&lt;&gt;0)</f>
         <v>0</v>
       </c>
       <c r="F35" t="b">
-        <f>AND(F21=Shared_Lines_Offset!E6,F21&lt;&gt;0)</f>
+        <f>AND(F21=-Shared_Lines_Offset!E6,F21&lt;&gt;0)</f>
         <v>0</v>
       </c>
       <c r="G35" t="b">
-        <f>AND(G21=Shared_Lines_Offset!F6,G21&lt;&gt;0)</f>
+        <f>AND(G21=-Shared_Lines_Offset!F6,G21&lt;&gt;0)</f>
         <v>0</v>
       </c>
       <c r="H35" t="b">
-        <f>AND(H21=Shared_Lines_Offset!G6,H21&lt;&gt;0)</f>
+        <f>AND(H21=-Shared_Lines_Offset!G6,H21&lt;&gt;0)</f>
         <v>0</v>
       </c>
       <c r="I35" t="b">
-        <f>AND(I21=Shared_Lines_Offset!H6,I21&lt;&gt;0)</f>
+        <f>AND(I21=-Shared_Lines_Offset!H6,I21&lt;&gt;0)</f>
         <v>0</v>
       </c>
       <c r="J35" t="b">
-        <f>AND(J21=Shared_Lines_Offset!I6,J21&lt;&gt;0)</f>
+        <f>AND(J21=-Shared_Lines_Offset!I6,J21&lt;&gt;0)</f>
         <v>0</v>
       </c>
       <c r="K35" t="b">
-        <f>AND(K21=Shared_Lines_Offset!J6,K21&lt;&gt;0)</f>
+        <f>AND(K21=-Shared_Lines_Offset!J6,K21&lt;&gt;0)</f>
         <v>0</v>
       </c>
       <c r="L35" t="b">
-        <f>AND(L21=Shared_Lines_Offset!K6,L21&lt;&gt;0)</f>
+        <f>AND(L21=-Shared_Lines_Offset!K6,L21&lt;&gt;0)</f>
         <v>0</v>
       </c>
       <c r="M35" t="b">
-        <f>AND(M21=Shared_Lines_Offset!L6,M21&lt;&gt;0)</f>
+        <f>AND(M21=-Shared_Lines_Offset!L6,M21&lt;&gt;0)</f>
         <v>0</v>
       </c>
       <c r="N35" t="b">
-        <f>AND(N21=Shared_Lines_Offset!M6,N21&lt;&gt;0)</f>
+        <f>AND(N21=-Shared_Lines_Offset!M6,N21&lt;&gt;0)</f>
         <v>0</v>
       </c>
     </row>
@@ -8332,51 +10547,51 @@
         <v>98</v>
       </c>
       <c r="C36" t="b">
-        <f>AND(C22=Shared_Lines_Offset!B7,C22&lt;&gt;0)</f>
+        <f>AND(C22=-Shared_Lines_Offset!B7,C22&lt;&gt;0)</f>
         <v>0</v>
       </c>
       <c r="D36" t="b">
-        <f>AND(D22=Shared_Lines_Offset!C7,D22&lt;&gt;0)</f>
+        <f>AND(D22=-Shared_Lines_Offset!C7,D22&lt;&gt;0)</f>
         <v>0</v>
       </c>
       <c r="E36" t="b">
-        <f>AND(E22=Shared_Lines_Offset!D7,E22&lt;&gt;0)</f>
+        <f>AND(E22=-Shared_Lines_Offset!D7,E22&lt;&gt;0)</f>
         <v>0</v>
       </c>
       <c r="F36" t="b">
-        <f>AND(F22=Shared_Lines_Offset!E7,F22&lt;&gt;0)</f>
+        <f>AND(F22=-Shared_Lines_Offset!E7,F22&lt;&gt;0)</f>
         <v>0</v>
       </c>
       <c r="G36" t="b">
-        <f>AND(G22=Shared_Lines_Offset!F7,G22&lt;&gt;0)</f>
+        <f>AND(G22=-Shared_Lines_Offset!F7,G22&lt;&gt;0)</f>
         <v>0</v>
       </c>
       <c r="H36" t="b">
-        <f>AND(H22=Shared_Lines_Offset!G7,H22&lt;&gt;0)</f>
+        <f>AND(H22=-Shared_Lines_Offset!G7,H22&lt;&gt;0)</f>
         <v>0</v>
       </c>
       <c r="I36" t="b">
-        <f>AND(I22=Shared_Lines_Offset!H7,I22&lt;&gt;0)</f>
+        <f>AND(I22=-Shared_Lines_Offset!H7,I22&lt;&gt;0)</f>
         <v>0</v>
       </c>
       <c r="J36" t="b">
-        <f>AND(J22=Shared_Lines_Offset!I7,J22&lt;&gt;0)</f>
+        <f>AND(J22=-Shared_Lines_Offset!I7,J22&lt;&gt;0)</f>
         <v>0</v>
       </c>
       <c r="K36" t="b">
-        <f>AND(K22=Shared_Lines_Offset!J7,K22&lt;&gt;0)</f>
-        <v>0</v>
-      </c>
-      <c r="L36" t="b">
-        <f>AND(L22=Shared_Lines_Offset!K7,L22&lt;&gt;0)</f>
+        <f>AND(K22=-Shared_Lines_Offset!J7,K22&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="L36" s="4" t="b">
+        <f>AND(L22=-Shared_Lines_Offset!K7,L22&lt;&gt;0)</f>
         <v>0</v>
       </c>
       <c r="M36" t="b">
-        <f>AND(M22=Shared_Lines_Offset!L7,M22&lt;&gt;0)</f>
+        <f>AND(M22=-Shared_Lines_Offset!L7,M22&lt;&gt;0)</f>
         <v>0</v>
       </c>
       <c r="N36" t="b">
-        <f>AND(N22=Shared_Lines_Offset!M7,N22&lt;&gt;0)</f>
+        <f>AND(N22=-Shared_Lines_Offset!M7,N22&lt;&gt;0)</f>
         <v>0</v>
       </c>
     </row>
@@ -8385,51 +10600,51 @@
         <v>99</v>
       </c>
       <c r="C37" t="b">
-        <f>AND(C23=Shared_Lines_Offset!B8,C23&lt;&gt;0)</f>
+        <f>AND(C23=-Shared_Lines_Offset!B8,C23&lt;&gt;0)</f>
         <v>0</v>
       </c>
       <c r="D37" t="b">
-        <f>AND(D23=Shared_Lines_Offset!C8,D23&lt;&gt;0)</f>
+        <f>AND(D23=-Shared_Lines_Offset!C8,D23&lt;&gt;0)</f>
         <v>0</v>
       </c>
       <c r="E37" t="b">
-        <f>AND(E23=Shared_Lines_Offset!D8,E23&lt;&gt;0)</f>
+        <f>AND(E23=-Shared_Lines_Offset!D8,E23&lt;&gt;0)</f>
         <v>0</v>
       </c>
       <c r="F37" t="b">
-        <f>AND(F23=Shared_Lines_Offset!E8,F23&lt;&gt;0)</f>
+        <f>AND(F23=-Shared_Lines_Offset!E8,F23&lt;&gt;0)</f>
         <v>0</v>
       </c>
       <c r="G37" t="b">
-        <f>AND(G23=Shared_Lines_Offset!F8,G23&lt;&gt;0)</f>
+        <f>AND(G23=-Shared_Lines_Offset!F8,G23&lt;&gt;0)</f>
         <v>0</v>
       </c>
       <c r="H37" t="b">
-        <f>AND(H23=Shared_Lines_Offset!G8,H23&lt;&gt;0)</f>
+        <f>AND(H23=-Shared_Lines_Offset!G8,H23&lt;&gt;0)</f>
         <v>0</v>
       </c>
       <c r="I37" t="b">
-        <f>AND(I23=Shared_Lines_Offset!H8,I23&lt;&gt;0)</f>
+        <f>AND(I23=-Shared_Lines_Offset!H8,I23&lt;&gt;0)</f>
         <v>0</v>
       </c>
       <c r="J37" t="b">
-        <f>AND(J23=Shared_Lines_Offset!I8,J23&lt;&gt;0)</f>
+        <f>AND(J23=-Shared_Lines_Offset!I8,J23&lt;&gt;0)</f>
         <v>0</v>
       </c>
       <c r="K37" t="b">
-        <f>AND(K23=Shared_Lines_Offset!J8,K23&lt;&gt;0)</f>
+        <f>AND(K23=-Shared_Lines_Offset!J8,K23&lt;&gt;0)</f>
         <v>0</v>
       </c>
       <c r="L37" t="b">
-        <f>AND(L23=Shared_Lines_Offset!K8,L23&lt;&gt;0)</f>
+        <f>AND(L23=-Shared_Lines_Offset!K8,L23&lt;&gt;0)</f>
         <v>0</v>
       </c>
       <c r="M37" t="b">
-        <f>AND(M23=Shared_Lines_Offset!L8,M23&lt;&gt;0)</f>
+        <f>AND(M23=-Shared_Lines_Offset!L8,M23&lt;&gt;0)</f>
         <v>0</v>
       </c>
       <c r="N37" t="b">
-        <f>AND(N23=Shared_Lines_Offset!M8,N23&lt;&gt;0)</f>
+        <f>AND(N23=-Shared_Lines_Offset!M8,N23&lt;&gt;0)</f>
         <v>0</v>
       </c>
     </row>
@@ -8438,51 +10653,51 @@
         <v>100</v>
       </c>
       <c r="C38" t="b">
-        <f>AND(C24=Shared_Lines_Offset!B9,C24&lt;&gt;0)</f>
+        <f>AND(C24=-Shared_Lines_Offset!B9,C24&lt;&gt;0)</f>
         <v>0</v>
       </c>
       <c r="D38" t="b">
-        <f>AND(D24=Shared_Lines_Offset!C9,D24&lt;&gt;0)</f>
+        <f>AND(D24=-Shared_Lines_Offset!C9,D24&lt;&gt;0)</f>
         <v>0</v>
       </c>
       <c r="E38" t="b">
-        <f>AND(E24=Shared_Lines_Offset!D9,E24&lt;&gt;0)</f>
+        <f>AND(E24=-Shared_Lines_Offset!D9,E24&lt;&gt;0)</f>
         <v>0</v>
       </c>
       <c r="F38" t="b">
-        <f>AND(F24=Shared_Lines_Offset!E9,F24&lt;&gt;0)</f>
+        <f>AND(F24=-Shared_Lines_Offset!E9,F24&lt;&gt;0)</f>
         <v>0</v>
       </c>
       <c r="G38" t="b">
-        <f>AND(G24=Shared_Lines_Offset!F9,G24&lt;&gt;0)</f>
+        <f>AND(G24=-Shared_Lines_Offset!F9,G24&lt;&gt;0)</f>
         <v>0</v>
       </c>
       <c r="H38" t="b">
-        <f>AND(H24=Shared_Lines_Offset!G9,H24&lt;&gt;0)</f>
+        <f>AND(H24=-Shared_Lines_Offset!G9,H24&lt;&gt;0)</f>
         <v>0</v>
       </c>
       <c r="I38" t="b">
-        <f>AND(I24=Shared_Lines_Offset!H9,I24&lt;&gt;0)</f>
+        <f>AND(I24=-Shared_Lines_Offset!H9,I24&lt;&gt;0)</f>
         <v>0</v>
       </c>
       <c r="J38" t="b">
-        <f>AND(J24=Shared_Lines_Offset!I9,J24&lt;&gt;0)</f>
+        <f>AND(J24=-Shared_Lines_Offset!I9,J24&lt;&gt;0)</f>
         <v>0</v>
       </c>
       <c r="K38" t="b">
-        <f>AND(K24=Shared_Lines_Offset!J9,K24&lt;&gt;0)</f>
+        <f>AND(K24=-Shared_Lines_Offset!J9,K24&lt;&gt;0)</f>
         <v>0</v>
       </c>
       <c r="L38" t="b">
-        <f>AND(L24=Shared_Lines_Offset!K9,L24&lt;&gt;0)</f>
+        <f>AND(L24=-Shared_Lines_Offset!K9,L24&lt;&gt;0)</f>
         <v>0</v>
       </c>
       <c r="M38" t="b">
-        <f>AND(M24=Shared_Lines_Offset!L9,M24&lt;&gt;0)</f>
+        <f>AND(M24=-Shared_Lines_Offset!L9,M24&lt;&gt;0)</f>
         <v>0</v>
       </c>
       <c r="N38" t="b">
-        <f>AND(N24=Shared_Lines_Offset!M9,N24&lt;&gt;0)</f>
+        <f>AND(N24=-Shared_Lines_Offset!M9,N24&lt;&gt;0)</f>
         <v>0</v>
       </c>
     </row>
@@ -8491,51 +10706,51 @@
         <v>101</v>
       </c>
       <c r="C39" t="b">
-        <f>AND(C25=Shared_Lines_Offset!B10,C25&lt;&gt;0)</f>
+        <f>AND(C25=-Shared_Lines_Offset!B10,C25&lt;&gt;0)</f>
         <v>0</v>
       </c>
       <c r="D39" t="b">
-        <f>AND(D25=Shared_Lines_Offset!C10,D25&lt;&gt;0)</f>
+        <f>AND(D25=-Shared_Lines_Offset!C10,D25&lt;&gt;0)</f>
         <v>0</v>
       </c>
       <c r="E39" t="b">
-        <f>AND(E25=Shared_Lines_Offset!D10,E25&lt;&gt;0)</f>
+        <f>AND(E25=-Shared_Lines_Offset!D10,E25&lt;&gt;0)</f>
         <v>0</v>
       </c>
       <c r="F39" t="b">
-        <f>AND(F25=Shared_Lines_Offset!E10,F25&lt;&gt;0)</f>
+        <f>AND(F25=-Shared_Lines_Offset!E10,F25&lt;&gt;0)</f>
         <v>0</v>
       </c>
       <c r="G39" t="b">
-        <f>AND(G25=Shared_Lines_Offset!F10,G25&lt;&gt;0)</f>
+        <f>AND(G25=-Shared_Lines_Offset!F10,G25&lt;&gt;0)</f>
         <v>0</v>
       </c>
       <c r="H39" t="b">
-        <f>AND(H25=Shared_Lines_Offset!G10,H25&lt;&gt;0)</f>
+        <f>AND(H25=-Shared_Lines_Offset!G10,H25&lt;&gt;0)</f>
         <v>0</v>
       </c>
       <c r="I39" t="b">
-        <f>AND(I25=Shared_Lines_Offset!H10,I25&lt;&gt;0)</f>
+        <f>AND(I25=-Shared_Lines_Offset!H10,I25&lt;&gt;0)</f>
         <v>0</v>
       </c>
       <c r="J39" t="b">
-        <f>AND(J25=Shared_Lines_Offset!I10,J25&lt;&gt;0)</f>
+        <f>AND(J25=-Shared_Lines_Offset!I10,J25&lt;&gt;0)</f>
         <v>0</v>
       </c>
       <c r="K39" t="b">
-        <f>AND(K25=Shared_Lines_Offset!J10,K25&lt;&gt;0)</f>
+        <f>AND(K25=-Shared_Lines_Offset!J10,K25&lt;&gt;0)</f>
         <v>0</v>
       </c>
       <c r="L39" t="b">
-        <f>AND(L25=Shared_Lines_Offset!K10,L25&lt;&gt;0)</f>
+        <f>AND(L25=-Shared_Lines_Offset!K10,L25&lt;&gt;0)</f>
         <v>0</v>
       </c>
       <c r="M39" t="b">
-        <f>AND(M25=Shared_Lines_Offset!L10,M25&lt;&gt;0)</f>
+        <f>AND(M25=-Shared_Lines_Offset!L10,M25&lt;&gt;0)</f>
         <v>0</v>
       </c>
       <c r="N39" t="b">
-        <f>AND(N25=Shared_Lines_Offset!M10,N25&lt;&gt;0)</f>
+        <f>AND(N25=-Shared_Lines_Offset!M10,N25&lt;&gt;0)</f>
         <v>0</v>
       </c>
     </row>
@@ -8544,51 +10759,51 @@
         <v>102</v>
       </c>
       <c r="C40" t="b">
-        <f>AND(C26=Shared_Lines_Offset!B11,C26&lt;&gt;0)</f>
+        <f>AND(C26=-Shared_Lines_Offset!B11,C26&lt;&gt;0)</f>
         <v>0</v>
       </c>
       <c r="D40" t="b">
-        <f>AND(D26=Shared_Lines_Offset!C11,D26&lt;&gt;0)</f>
+        <f>AND(D26=-Shared_Lines_Offset!C11,D26&lt;&gt;0)</f>
         <v>0</v>
       </c>
       <c r="E40" t="b">
-        <f>AND(E26=Shared_Lines_Offset!D11,E26&lt;&gt;0)</f>
+        <f>AND(E26=-Shared_Lines_Offset!D11,E26&lt;&gt;0)</f>
         <v>0</v>
       </c>
       <c r="F40" t="b">
-        <f>AND(F26=Shared_Lines_Offset!E11,F26&lt;&gt;0)</f>
+        <f>AND(F26=-Shared_Lines_Offset!E11,F26&lt;&gt;0)</f>
         <v>0</v>
       </c>
       <c r="G40" t="b">
-        <f>AND(G26=Shared_Lines_Offset!F11,G26&lt;&gt;0)</f>
+        <f>AND(G26=-Shared_Lines_Offset!F11,G26&lt;&gt;0)</f>
         <v>0</v>
       </c>
       <c r="H40" t="b">
-        <f>AND(H26=Shared_Lines_Offset!G11,H26&lt;&gt;0)</f>
+        <f>AND(H26=-Shared_Lines_Offset!G11,H26&lt;&gt;0)</f>
         <v>0</v>
       </c>
       <c r="I40" t="b">
-        <f>AND(I26=Shared_Lines_Offset!H11,I26&lt;&gt;0)</f>
+        <f>AND(I26=-Shared_Lines_Offset!H11,I26&lt;&gt;0)</f>
         <v>0</v>
       </c>
       <c r="J40" t="b">
-        <f>AND(J26=Shared_Lines_Offset!I11,J26&lt;&gt;0)</f>
+        <f>AND(J26=-Shared_Lines_Offset!I11,J26&lt;&gt;0)</f>
         <v>0</v>
       </c>
       <c r="K40" t="b">
-        <f>AND(K26=Shared_Lines_Offset!J11,K26&lt;&gt;0)</f>
+        <f>AND(K26=-Shared_Lines_Offset!J11,K26&lt;&gt;0)</f>
         <v>0</v>
       </c>
       <c r="L40" t="b">
-        <f>AND(L26=Shared_Lines_Offset!K11,L26&lt;&gt;0)</f>
+        <f>AND(L26=-Shared_Lines_Offset!K11,L26&lt;&gt;0)</f>
         <v>0</v>
       </c>
       <c r="M40" t="b">
-        <f>AND(M26=Shared_Lines_Offset!L11,M26&lt;&gt;0)</f>
+        <f>AND(M26=-Shared_Lines_Offset!L11,M26&lt;&gt;0)</f>
         <v>0</v>
       </c>
       <c r="N40" t="b">
-        <f>AND(N26=Shared_Lines_Offset!M11,N26&lt;&gt;0)</f>
+        <f>AND(N26=-Shared_Lines_Offset!M11,N26&lt;&gt;0)</f>
         <v>0</v>
       </c>
     </row>
@@ -8597,51 +10812,51 @@
         <v>103</v>
       </c>
       <c r="C41" t="b">
-        <f>AND(C27=Shared_Lines_Offset!B12,C27&lt;&gt;0)</f>
+        <f>AND(C27=-Shared_Lines_Offset!B12,C27&lt;&gt;0)</f>
         <v>0</v>
       </c>
       <c r="D41" t="b">
-        <f>AND(D27=Shared_Lines_Offset!C12,D27&lt;&gt;0)</f>
+        <f>AND(D27=-Shared_Lines_Offset!C12,D27&lt;&gt;0)</f>
         <v>0</v>
       </c>
       <c r="E41" t="b">
-        <f>AND(E27=Shared_Lines_Offset!D12,E27&lt;&gt;0)</f>
+        <f>AND(E27=-Shared_Lines_Offset!D12,E27&lt;&gt;0)</f>
         <v>0</v>
       </c>
       <c r="F41" t="b">
-        <f>AND(F27=Shared_Lines_Offset!E12,F27&lt;&gt;0)</f>
+        <f>AND(F27=-Shared_Lines_Offset!E12,F27&lt;&gt;0)</f>
         <v>0</v>
       </c>
       <c r="G41" t="b">
-        <f>AND(G27=Shared_Lines_Offset!F12,G27&lt;&gt;0)</f>
+        <f>AND(G27=-Shared_Lines_Offset!F12,G27&lt;&gt;0)</f>
         <v>0</v>
       </c>
       <c r="H41" t="b">
-        <f>AND(H27=Shared_Lines_Offset!G12,H27&lt;&gt;0)</f>
+        <f>AND(H27=-Shared_Lines_Offset!G12,H27&lt;&gt;0)</f>
         <v>0</v>
       </c>
       <c r="I41" t="b">
-        <f>AND(I27=Shared_Lines_Offset!H12,I27&lt;&gt;0)</f>
+        <f>AND(I27=-Shared_Lines_Offset!H12,I27&lt;&gt;0)</f>
         <v>0</v>
       </c>
       <c r="J41" t="b">
-        <f>AND(J27=Shared_Lines_Offset!I12,J27&lt;&gt;0)</f>
+        <f>AND(J27=-Shared_Lines_Offset!I12,J27&lt;&gt;0)</f>
         <v>0</v>
       </c>
       <c r="K41" t="b">
-        <f>AND(K27=Shared_Lines_Offset!J12,K27&lt;&gt;0)</f>
+        <f>AND(K27=-Shared_Lines_Offset!J12,K27&lt;&gt;0)</f>
         <v>0</v>
       </c>
       <c r="L41" t="b">
-        <f>AND(L27=Shared_Lines_Offset!K12,L27&lt;&gt;0)</f>
+        <f>AND(L27=-Shared_Lines_Offset!K12,L27&lt;&gt;0)</f>
         <v>0</v>
       </c>
       <c r="M41" t="b">
-        <f>AND(M27=Shared_Lines_Offset!L12,M27&lt;&gt;0)</f>
+        <f>AND(M27=-Shared_Lines_Offset!L12,M27&lt;&gt;0)</f>
         <v>0</v>
       </c>
       <c r="N41" t="b">
-        <f>AND(N27=Shared_Lines_Offset!M12,N27&lt;&gt;0)</f>
+        <f>AND(N27=-Shared_Lines_Offset!M12,N27&lt;&gt;0)</f>
         <v>0</v>
       </c>
     </row>
@@ -8650,51 +10865,51 @@
         <v>17</v>
       </c>
       <c r="C42" t="b">
-        <f>AND(C28=Shared_Lines_Offset!B13,C28&lt;&gt;0)</f>
+        <f>AND(C28=-Shared_Lines_Offset!B13,C28&lt;&gt;0)</f>
         <v>0</v>
       </c>
       <c r="D42" t="b">
-        <f>AND(D28=Shared_Lines_Offset!C13,D28&lt;&gt;0)</f>
+        <f>AND(D28=-Shared_Lines_Offset!C13,D28&lt;&gt;0)</f>
         <v>0</v>
       </c>
       <c r="E42" t="b">
-        <f>AND(E28=Shared_Lines_Offset!D13,E28&lt;&gt;0)</f>
+        <f>AND(E28=-Shared_Lines_Offset!D13,E28&lt;&gt;0)</f>
         <v>0</v>
       </c>
       <c r="F42" t="b">
-        <f>AND(F28=Shared_Lines_Offset!E13,F28&lt;&gt;0)</f>
+        <f>AND(F28=-Shared_Lines_Offset!E13,F28&lt;&gt;0)</f>
         <v>0</v>
       </c>
       <c r="G42" t="b">
-        <f>AND(G28=Shared_Lines_Offset!F13,G28&lt;&gt;0)</f>
+        <f>AND(G28=-Shared_Lines_Offset!F13,G28&lt;&gt;0)</f>
         <v>0</v>
       </c>
       <c r="H42" t="b">
-        <f>AND(H28=Shared_Lines_Offset!G13,H28&lt;&gt;0)</f>
+        <f>AND(H28=-Shared_Lines_Offset!G13,H28&lt;&gt;0)</f>
         <v>0</v>
       </c>
       <c r="I42" t="b">
-        <f>AND(I28=Shared_Lines_Offset!H13,I28&lt;&gt;0)</f>
+        <f>AND(I28=-Shared_Lines_Offset!H13,I28&lt;&gt;0)</f>
         <v>0</v>
       </c>
       <c r="J42" t="b">
-        <f>AND(J28=Shared_Lines_Offset!I13,J28&lt;&gt;0)</f>
+        <f>AND(J28=-Shared_Lines_Offset!I13,J28&lt;&gt;0)</f>
         <v>0</v>
       </c>
       <c r="K42" t="b">
-        <f>AND(K28=Shared_Lines_Offset!J13,K28&lt;&gt;0)</f>
+        <f>AND(K28=-Shared_Lines_Offset!J13,K28&lt;&gt;0)</f>
         <v>0</v>
       </c>
       <c r="L42" t="b">
-        <f>AND(L28=Shared_Lines_Offset!K13,L28&lt;&gt;0)</f>
+        <f>AND(L28=-Shared_Lines_Offset!K13,L28&lt;&gt;0)</f>
         <v>0</v>
       </c>
       <c r="M42" t="b">
-        <f>AND(M28=Shared_Lines_Offset!L13,M28&lt;&gt;0)</f>
+        <f>AND(M28=-Shared_Lines_Offset!L13,M28&lt;&gt;0)</f>
         <v>0</v>
       </c>
       <c r="N42" t="b">
-        <f>AND(N28=Shared_Lines_Offset!M13,N28&lt;&gt;0)</f>
+        <f>AND(N28=-Shared_Lines_Offset!M13,N28&lt;&gt;0)</f>
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added test for sat eve abs1
</commit_message>
<xml_diff>
--- a/data/Times_to_Transfer_Stations.xlsx
+++ b/data/Times_to_Transfer_Stations.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25725"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="8760" yWindow="0" windowWidth="25600" windowHeight="15860" tabRatio="564" firstSheet="5" activeTab="8"/>
+    <workbookView xWindow="3960" yWindow="0" windowWidth="25600" windowHeight="15860" tabRatio="564" firstSheet="7" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="Station_Time_Calculations" sheetId="1" r:id="rId1"/>
@@ -16,6 +16,7 @@
     <sheet name="Shared_Lines_Offset" sheetId="7" r:id="rId7"/>
     <sheet name="shared_test_sat_morn_orig" sheetId="8" r:id="rId8"/>
     <sheet name="shared_test_sat_morn_abs1" sheetId="9" r:id="rId9"/>
+    <sheet name="shared_test_sat_eve_abs1" sheetId="10" r:id="rId10"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="986" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1061" uniqueCount="113">
   <si>
     <t>-</t>
   </si>
@@ -432,8 +433,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="149">
+  <cellStyleXfs count="151">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -590,7 +593,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="149">
+  <cellStyles count="151">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -665,6 +668,7 @@
     <cellStyle name="Followed Hyperlink" xfId="144" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="146" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="148" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="150" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -739,6 +743,7 @@
     <cellStyle name="Hyperlink" xfId="143" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="145" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="147" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="149" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1688,6 +1693,2133 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:N42"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="M46" sqref="M46"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:14">
+      <c r="C1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14">
+      <c r="A2" s="1"/>
+      <c r="B2" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="C2" s="1">
+        <v>11</v>
+      </c>
+      <c r="D2" s="1">
+        <v>5</v>
+      </c>
+      <c r="E2" s="1">
+        <v>5</v>
+      </c>
+      <c r="F2" s="1">
+        <v>4</v>
+      </c>
+      <c r="G2" s="1">
+        <v>11</v>
+      </c>
+      <c r="H2" s="1">
+        <v>5</v>
+      </c>
+      <c r="I2" s="1">
+        <v>2</v>
+      </c>
+      <c r="J2" s="1">
+        <v>5</v>
+      </c>
+      <c r="K2" s="1">
+        <v>11</v>
+      </c>
+      <c r="L2" s="1">
+        <v>5</v>
+      </c>
+      <c r="M2" s="1">
+        <v>5</v>
+      </c>
+      <c r="N2" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14">
+      <c r="A3" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" s="1">
+        <v>11</v>
+      </c>
+      <c r="C3">
+        <f>$B3-C$2</f>
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <f t="shared" ref="D3:N14" si="0">$B3-D$2</f>
+        <v>6</v>
+      </c>
+      <c r="E3">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="F3">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="G3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="I3">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="J3">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="K3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L3">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="M3">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="N3">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14">
+      <c r="A4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="1">
+        <v>5</v>
+      </c>
+      <c r="C4">
+        <f t="shared" ref="C4:C14" si="1">$B4-C$2</f>
+        <v>-6</v>
+      </c>
+      <c r="D4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="G4">
+        <f t="shared" si="0"/>
+        <v>-6</v>
+      </c>
+      <c r="H4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I4">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="J4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K4">
+        <f t="shared" si="0"/>
+        <v>-6</v>
+      </c>
+      <c r="L4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14">
+      <c r="A5" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B5" s="1">
+        <v>5</v>
+      </c>
+      <c r="C5">
+        <f t="shared" si="1"/>
+        <v>-6</v>
+      </c>
+      <c r="D5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="G5">
+        <f t="shared" si="0"/>
+        <v>-6</v>
+      </c>
+      <c r="H5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="J5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K5">
+        <f t="shared" si="0"/>
+        <v>-6</v>
+      </c>
+      <c r="L5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14">
+      <c r="A6" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B6" s="1">
+        <v>4</v>
+      </c>
+      <c r="C6">
+        <f t="shared" si="1"/>
+        <v>-7</v>
+      </c>
+      <c r="D6">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+      <c r="F6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <f t="shared" si="0"/>
+        <v>-7</v>
+      </c>
+      <c r="H6">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+      <c r="I6">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="J6">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+      <c r="K6">
+        <f t="shared" si="0"/>
+        <v>-7</v>
+      </c>
+      <c r="L6">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+      <c r="M6">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+      <c r="N6">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14">
+      <c r="A7" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B7" s="1">
+        <v>11</v>
+      </c>
+      <c r="C7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="F7">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="G7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H7">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="I7">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="J7">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="K7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L7">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="M7">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="N7">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14">
+      <c r="A8" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="B8" s="1">
+        <v>5</v>
+      </c>
+      <c r="C8">
+        <f t="shared" si="1"/>
+        <v>-6</v>
+      </c>
+      <c r="D8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="G8">
+        <f t="shared" si="0"/>
+        <v>-6</v>
+      </c>
+      <c r="H8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I8">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="J8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K8">
+        <f t="shared" si="0"/>
+        <v>-6</v>
+      </c>
+      <c r="L8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14">
+      <c r="A9" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B9" s="1">
+        <v>2</v>
+      </c>
+      <c r="C9">
+        <f t="shared" si="1"/>
+        <v>-9</v>
+      </c>
+      <c r="D9">
+        <f t="shared" si="0"/>
+        <v>-3</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="0"/>
+        <v>-3</v>
+      </c>
+      <c r="F9">
+        <f t="shared" si="0"/>
+        <v>-2</v>
+      </c>
+      <c r="G9">
+        <f t="shared" si="0"/>
+        <v>-9</v>
+      </c>
+      <c r="H9">
+        <f t="shared" si="0"/>
+        <v>-3</v>
+      </c>
+      <c r="I9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J9">
+        <f t="shared" si="0"/>
+        <v>-3</v>
+      </c>
+      <c r="K9">
+        <f t="shared" si="0"/>
+        <v>-9</v>
+      </c>
+      <c r="L9">
+        <f t="shared" si="0"/>
+        <v>-3</v>
+      </c>
+      <c r="M9">
+        <f t="shared" si="0"/>
+        <v>-3</v>
+      </c>
+      <c r="N9">
+        <f t="shared" si="0"/>
+        <v>-3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14">
+      <c r="A10" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B10" s="1">
+        <v>5</v>
+      </c>
+      <c r="C10">
+        <f t="shared" si="1"/>
+        <v>-6</v>
+      </c>
+      <c r="D10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="G10">
+        <f t="shared" si="0"/>
+        <v>-6</v>
+      </c>
+      <c r="H10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I10">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="J10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K10">
+        <f t="shared" si="0"/>
+        <v>-6</v>
+      </c>
+      <c r="L10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14">
+      <c r="A11" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="B11" s="1">
+        <v>11</v>
+      </c>
+      <c r="C11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="E11">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="F11">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="G11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H11">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="I11">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="J11">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="K11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L11">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="M11">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="N11">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14">
+      <c r="A12" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="B12" s="1">
+        <v>5</v>
+      </c>
+      <c r="C12">
+        <f t="shared" si="1"/>
+        <v>-6</v>
+      </c>
+      <c r="D12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F12">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="G12">
+        <f t="shared" si="0"/>
+        <v>-6</v>
+      </c>
+      <c r="H12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I12">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="J12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K12">
+        <f t="shared" si="0"/>
+        <v>-6</v>
+      </c>
+      <c r="L12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14">
+      <c r="A13" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="B13" s="1">
+        <v>5</v>
+      </c>
+      <c r="C13">
+        <f t="shared" si="1"/>
+        <v>-6</v>
+      </c>
+      <c r="D13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F13">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="G13">
+        <f t="shared" si="0"/>
+        <v>-6</v>
+      </c>
+      <c r="H13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I13">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="J13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K13">
+        <f t="shared" si="0"/>
+        <v>-6</v>
+      </c>
+      <c r="L13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14">
+      <c r="A14" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B14" s="1">
+        <v>5</v>
+      </c>
+      <c r="C14">
+        <f t="shared" si="1"/>
+        <v>-6</v>
+      </c>
+      <c r="D14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F14">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="G14">
+        <f t="shared" si="0"/>
+        <v>-6</v>
+      </c>
+      <c r="H14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I14">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="J14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K14">
+        <f t="shared" si="0"/>
+        <v>-6</v>
+      </c>
+      <c r="L14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14">
+      <c r="B16" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="J16" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="K16" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="L16" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="M16" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="N16" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="17" spans="2:14">
+      <c r="B17" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C17">
+        <f>C3*Shared_Lines!B2</f>
+        <v>0</v>
+      </c>
+      <c r="D17">
+        <f>D3*Shared_Lines!C2</f>
+        <v>0</v>
+      </c>
+      <c r="E17">
+        <f>E3*Shared_Lines!D2</f>
+        <v>0</v>
+      </c>
+      <c r="F17">
+        <f>F3*Shared_Lines!E2</f>
+        <v>0</v>
+      </c>
+      <c r="G17">
+        <f>G3*Shared_Lines!F2</f>
+        <v>0</v>
+      </c>
+      <c r="H17">
+        <f>H3*Shared_Lines!G2</f>
+        <v>0</v>
+      </c>
+      <c r="I17">
+        <f>I3*Shared_Lines!H2</f>
+        <v>0</v>
+      </c>
+      <c r="J17">
+        <f>J3*Shared_Lines!I2</f>
+        <v>0</v>
+      </c>
+      <c r="K17">
+        <f>K3*Shared_Lines!J2</f>
+        <v>0</v>
+      </c>
+      <c r="L17">
+        <f>L3*Shared_Lines!K2</f>
+        <v>0</v>
+      </c>
+      <c r="M17">
+        <f>M3*Shared_Lines!L2</f>
+        <v>6</v>
+      </c>
+      <c r="N17">
+        <f>N3*Shared_Lines!M2</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="2:14">
+      <c r="B18" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C18">
+        <f>C4*Shared_Lines!B3</f>
+        <v>0</v>
+      </c>
+      <c r="D18">
+        <f>D4*Shared_Lines!C3</f>
+        <v>0</v>
+      </c>
+      <c r="E18">
+        <f>E4*Shared_Lines!D3</f>
+        <v>0</v>
+      </c>
+      <c r="F18">
+        <f>F4*Shared_Lines!E3</f>
+        <v>0</v>
+      </c>
+      <c r="G18">
+        <f>G4*Shared_Lines!F3</f>
+        <v>0</v>
+      </c>
+      <c r="H18">
+        <f>H4*Shared_Lines!G3</f>
+        <v>0</v>
+      </c>
+      <c r="I18">
+        <f>I4*Shared_Lines!H3</f>
+        <v>0</v>
+      </c>
+      <c r="J18">
+        <f>J4*Shared_Lines!I3</f>
+        <v>0</v>
+      </c>
+      <c r="K18">
+        <f>K4*Shared_Lines!J3</f>
+        <v>0</v>
+      </c>
+      <c r="L18">
+        <f>L4*Shared_Lines!K3</f>
+        <v>0</v>
+      </c>
+      <c r="M18">
+        <f>M4*Shared_Lines!L3</f>
+        <v>0</v>
+      </c>
+      <c r="N18">
+        <f>N4*Shared_Lines!M3</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="2:14">
+      <c r="B19" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="C19">
+        <f>C5*Shared_Lines!B4</f>
+        <v>0</v>
+      </c>
+      <c r="D19">
+        <f>D5*Shared_Lines!C4</f>
+        <v>0</v>
+      </c>
+      <c r="E19">
+        <f>E5*Shared_Lines!D4</f>
+        <v>0</v>
+      </c>
+      <c r="F19">
+        <f>F5*Shared_Lines!E4</f>
+        <v>0</v>
+      </c>
+      <c r="G19">
+        <f>G5*Shared_Lines!F4</f>
+        <v>0</v>
+      </c>
+      <c r="H19">
+        <f>H5*Shared_Lines!G4</f>
+        <v>0</v>
+      </c>
+      <c r="I19">
+        <f>I5*Shared_Lines!H4</f>
+        <v>0</v>
+      </c>
+      <c r="J19">
+        <f>J5*Shared_Lines!I4</f>
+        <v>0</v>
+      </c>
+      <c r="K19">
+        <f>K5*Shared_Lines!J4</f>
+        <v>0</v>
+      </c>
+      <c r="L19">
+        <f>L5*Shared_Lines!K4</f>
+        <v>0</v>
+      </c>
+      <c r="M19">
+        <f>M5*Shared_Lines!L4</f>
+        <v>0</v>
+      </c>
+      <c r="N19">
+        <f>N5*Shared_Lines!M4</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="2:14">
+      <c r="B20" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="C20">
+        <f>C6*Shared_Lines!B5</f>
+        <v>0</v>
+      </c>
+      <c r="D20">
+        <f>D6*Shared_Lines!C5</f>
+        <v>0</v>
+      </c>
+      <c r="E20">
+        <f>E6*Shared_Lines!D5</f>
+        <v>0</v>
+      </c>
+      <c r="F20">
+        <f>F6*Shared_Lines!E5</f>
+        <v>0</v>
+      </c>
+      <c r="G20">
+        <f>G6*Shared_Lines!F5</f>
+        <v>0</v>
+      </c>
+      <c r="H20">
+        <f>H6*Shared_Lines!G5</f>
+        <v>0</v>
+      </c>
+      <c r="I20">
+        <f>I6*Shared_Lines!H5</f>
+        <v>0</v>
+      </c>
+      <c r="J20">
+        <f>J6*Shared_Lines!I5</f>
+        <v>0</v>
+      </c>
+      <c r="K20">
+        <f>K6*Shared_Lines!J5</f>
+        <v>0</v>
+      </c>
+      <c r="L20">
+        <f>L6*Shared_Lines!K5</f>
+        <v>0</v>
+      </c>
+      <c r="M20">
+        <f>M6*Shared_Lines!L5</f>
+        <v>0</v>
+      </c>
+      <c r="N20">
+        <f>N6*Shared_Lines!M5</f>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="21" spans="2:14">
+      <c r="B21" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="C21">
+        <f>C7*Shared_Lines!B6</f>
+        <v>0</v>
+      </c>
+      <c r="D21">
+        <f>D7*Shared_Lines!C6</f>
+        <v>0</v>
+      </c>
+      <c r="E21">
+        <f>E7*Shared_Lines!D6</f>
+        <v>0</v>
+      </c>
+      <c r="F21">
+        <f>F7*Shared_Lines!E6</f>
+        <v>0</v>
+      </c>
+      <c r="G21">
+        <f>G7*Shared_Lines!F6</f>
+        <v>0</v>
+      </c>
+      <c r="H21">
+        <f>H7*Shared_Lines!G6</f>
+        <v>0</v>
+      </c>
+      <c r="I21">
+        <f>I7*Shared_Lines!H6</f>
+        <v>0</v>
+      </c>
+      <c r="J21">
+        <f>J7*Shared_Lines!I6</f>
+        <v>0</v>
+      </c>
+      <c r="K21">
+        <f>K7*Shared_Lines!J6</f>
+        <v>0</v>
+      </c>
+      <c r="L21">
+        <f>L7*Shared_Lines!K6</f>
+        <v>0</v>
+      </c>
+      <c r="M21">
+        <f>M7*Shared_Lines!L6</f>
+        <v>0</v>
+      </c>
+      <c r="N21">
+        <f>N7*Shared_Lines!M6</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="2:14">
+      <c r="B22" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="C22">
+        <f>C8*Shared_Lines!B7</f>
+        <v>0</v>
+      </c>
+      <c r="D22">
+        <f>D8*Shared_Lines!C7</f>
+        <v>0</v>
+      </c>
+      <c r="E22">
+        <f>E8*Shared_Lines!D7</f>
+        <v>0</v>
+      </c>
+      <c r="F22">
+        <f>F8*Shared_Lines!E7</f>
+        <v>0</v>
+      </c>
+      <c r="G22">
+        <f>G8*Shared_Lines!F7</f>
+        <v>0</v>
+      </c>
+      <c r="H22">
+        <f>H8*Shared_Lines!G7</f>
+        <v>0</v>
+      </c>
+      <c r="I22">
+        <f>I8*Shared_Lines!H7</f>
+        <v>0</v>
+      </c>
+      <c r="J22">
+        <f>J8*Shared_Lines!I7</f>
+        <v>0</v>
+      </c>
+      <c r="K22">
+        <f>K8*Shared_Lines!J7</f>
+        <v>0</v>
+      </c>
+      <c r="L22">
+        <f>L8*Shared_Lines!K7</f>
+        <v>0</v>
+      </c>
+      <c r="M22">
+        <f>M8*Shared_Lines!L7</f>
+        <v>0</v>
+      </c>
+      <c r="N22">
+        <f>N8*Shared_Lines!M7</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="2:14">
+      <c r="B23" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="C23">
+        <f>C9*Shared_Lines!B8</f>
+        <v>0</v>
+      </c>
+      <c r="D23">
+        <f>D9*Shared_Lines!C8</f>
+        <v>0</v>
+      </c>
+      <c r="E23">
+        <f>E9*Shared_Lines!D8</f>
+        <v>0</v>
+      </c>
+      <c r="F23">
+        <f>F9*Shared_Lines!E8</f>
+        <v>0</v>
+      </c>
+      <c r="G23">
+        <f>G9*Shared_Lines!F8</f>
+        <v>0</v>
+      </c>
+      <c r="H23">
+        <f>H9*Shared_Lines!G8</f>
+        <v>0</v>
+      </c>
+      <c r="I23">
+        <f>I9*Shared_Lines!H8</f>
+        <v>0</v>
+      </c>
+      <c r="J23">
+        <f>J9*Shared_Lines!I8</f>
+        <v>0</v>
+      </c>
+      <c r="K23">
+        <f>K9*Shared_Lines!J8</f>
+        <v>0</v>
+      </c>
+      <c r="L23">
+        <f>L9*Shared_Lines!K8</f>
+        <v>0</v>
+      </c>
+      <c r="M23">
+        <f>M9*Shared_Lines!L8</f>
+        <v>0</v>
+      </c>
+      <c r="N23">
+        <f>N9*Shared_Lines!M8</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="2:14">
+      <c r="B24" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="C24">
+        <f>C10*Shared_Lines!B9</f>
+        <v>0</v>
+      </c>
+      <c r="D24">
+        <f>D10*Shared_Lines!C9</f>
+        <v>0</v>
+      </c>
+      <c r="E24">
+        <f>E10*Shared_Lines!D9</f>
+        <v>0</v>
+      </c>
+      <c r="F24">
+        <f>F10*Shared_Lines!E9</f>
+        <v>0</v>
+      </c>
+      <c r="G24">
+        <f>G10*Shared_Lines!F9</f>
+        <v>0</v>
+      </c>
+      <c r="H24">
+        <f>H10*Shared_Lines!G9</f>
+        <v>0</v>
+      </c>
+      <c r="I24">
+        <f>I10*Shared_Lines!H9</f>
+        <v>0</v>
+      </c>
+      <c r="J24">
+        <f>J10*Shared_Lines!I9</f>
+        <v>0</v>
+      </c>
+      <c r="K24">
+        <f>K10*Shared_Lines!J9</f>
+        <v>0</v>
+      </c>
+      <c r="L24">
+        <f>L10*Shared_Lines!K9</f>
+        <v>0</v>
+      </c>
+      <c r="M24">
+        <f>M10*Shared_Lines!L9</f>
+        <v>0</v>
+      </c>
+      <c r="N24">
+        <f>N10*Shared_Lines!M9</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="2:14">
+      <c r="B25" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="C25">
+        <f>C11*Shared_Lines!B10</f>
+        <v>0</v>
+      </c>
+      <c r="D25">
+        <f>D11*Shared_Lines!C10</f>
+        <v>0</v>
+      </c>
+      <c r="E25">
+        <f>E11*Shared_Lines!D10</f>
+        <v>0</v>
+      </c>
+      <c r="F25">
+        <f>F11*Shared_Lines!E10</f>
+        <v>0</v>
+      </c>
+      <c r="G25">
+        <f>G11*Shared_Lines!F10</f>
+        <v>0</v>
+      </c>
+      <c r="H25">
+        <f>H11*Shared_Lines!G10</f>
+        <v>0</v>
+      </c>
+      <c r="I25">
+        <f>I11*Shared_Lines!H10</f>
+        <v>0</v>
+      </c>
+      <c r="J25">
+        <f>J11*Shared_Lines!I10</f>
+        <v>0</v>
+      </c>
+      <c r="K25">
+        <f>K11*Shared_Lines!J10</f>
+        <v>0</v>
+      </c>
+      <c r="L25">
+        <f>L11*Shared_Lines!K10</f>
+        <v>0</v>
+      </c>
+      <c r="M25">
+        <f>M11*Shared_Lines!L10</f>
+        <v>0</v>
+      </c>
+      <c r="N25">
+        <f>N11*Shared_Lines!M10</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="2:14">
+      <c r="B26" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C26">
+        <f>C12*Shared_Lines!B11</f>
+        <v>0</v>
+      </c>
+      <c r="D26">
+        <f>D12*Shared_Lines!C11</f>
+        <v>0</v>
+      </c>
+      <c r="E26">
+        <f>E12*Shared_Lines!D11</f>
+        <v>0</v>
+      </c>
+      <c r="F26">
+        <f>F12*Shared_Lines!E11</f>
+        <v>0</v>
+      </c>
+      <c r="G26">
+        <f>G12*Shared_Lines!F11</f>
+        <v>0</v>
+      </c>
+      <c r="H26">
+        <f>H12*Shared_Lines!G11</f>
+        <v>0</v>
+      </c>
+      <c r="I26">
+        <f>I12*Shared_Lines!H11</f>
+        <v>0</v>
+      </c>
+      <c r="J26">
+        <f>J12*Shared_Lines!I11</f>
+        <v>0</v>
+      </c>
+      <c r="K26">
+        <f>K12*Shared_Lines!J11</f>
+        <v>0</v>
+      </c>
+      <c r="L26">
+        <f>L12*Shared_Lines!K11</f>
+        <v>0</v>
+      </c>
+      <c r="M26">
+        <f>M12*Shared_Lines!L11</f>
+        <v>0</v>
+      </c>
+      <c r="N26">
+        <f>N12*Shared_Lines!M11</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="2:14">
+      <c r="B27" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="C27">
+        <f>C13*Shared_Lines!B12</f>
+        <v>0</v>
+      </c>
+      <c r="D27">
+        <f>D13*Shared_Lines!C12</f>
+        <v>0</v>
+      </c>
+      <c r="E27">
+        <f>E13*Shared_Lines!D12</f>
+        <v>0</v>
+      </c>
+      <c r="F27">
+        <f>F13*Shared_Lines!E12</f>
+        <v>0</v>
+      </c>
+      <c r="G27">
+        <f>G13*Shared_Lines!F12</f>
+        <v>0</v>
+      </c>
+      <c r="H27">
+        <f>H13*Shared_Lines!G12</f>
+        <v>0</v>
+      </c>
+      <c r="I27">
+        <f>I13*Shared_Lines!H12</f>
+        <v>0</v>
+      </c>
+      <c r="J27">
+        <f>J13*Shared_Lines!I12</f>
+        <v>0</v>
+      </c>
+      <c r="K27">
+        <f>K13*Shared_Lines!J12</f>
+        <v>0</v>
+      </c>
+      <c r="L27">
+        <f>L13*Shared_Lines!K12</f>
+        <v>0</v>
+      </c>
+      <c r="M27">
+        <f>M13*Shared_Lines!L12</f>
+        <v>0</v>
+      </c>
+      <c r="N27">
+        <f>N13*Shared_Lines!M12</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="2:14">
+      <c r="B28" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C28">
+        <f>C14*Shared_Lines!B13</f>
+        <v>0</v>
+      </c>
+      <c r="D28">
+        <f>D14*Shared_Lines!C13</f>
+        <v>0</v>
+      </c>
+      <c r="E28">
+        <f>E14*Shared_Lines!D13</f>
+        <v>0</v>
+      </c>
+      <c r="F28">
+        <f>F14*Shared_Lines!E13</f>
+        <v>0</v>
+      </c>
+      <c r="G28">
+        <f>G14*Shared_Lines!F13</f>
+        <v>0</v>
+      </c>
+      <c r="H28">
+        <f>H14*Shared_Lines!G13</f>
+        <v>0</v>
+      </c>
+      <c r="I28">
+        <f>I14*Shared_Lines!H13</f>
+        <v>0</v>
+      </c>
+      <c r="J28">
+        <f>J14*Shared_Lines!I13</f>
+        <v>0</v>
+      </c>
+      <c r="K28">
+        <f>K14*Shared_Lines!J13</f>
+        <v>0</v>
+      </c>
+      <c r="L28">
+        <f>L14*Shared_Lines!K13</f>
+        <v>0</v>
+      </c>
+      <c r="M28">
+        <f>M14*Shared_Lines!L13</f>
+        <v>0</v>
+      </c>
+      <c r="N28">
+        <f>N14*Shared_Lines!M13</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="2:14">
+      <c r="B30" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="G30" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="H30" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="I30" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="J30" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="K30" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="L30" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="M30" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="N30" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="31" spans="2:14">
+      <c r="B31" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C31" t="b">
+        <f>AND(C17=-Shared_Lines_Offset!B2,C17&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="D31" t="b">
+        <f>AND(D17=-Shared_Lines_Offset!C2,D17&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="E31" t="b">
+        <f>AND(E17=-Shared_Lines_Offset!D2,E17&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="F31" t="b">
+        <f>AND(F17=-Shared_Lines_Offset!E2,F17&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="G31" t="b">
+        <f>AND(G17=-Shared_Lines_Offset!F2,G17&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="H31" t="b">
+        <f>AND(H17=-Shared_Lines_Offset!G2,H17&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="I31" t="b">
+        <f>AND(I17=-Shared_Lines_Offset!H2,I17&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="J31" t="b">
+        <f>AND(J17=-Shared_Lines_Offset!I2,J17&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="K31" t="b">
+        <f>AND(K17=-Shared_Lines_Offset!J2,K17&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="L31" t="b">
+        <f>AND(L17=-Shared_Lines_Offset!K2,L17&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="M31" t="b">
+        <f>AND(M17=-Shared_Lines_Offset!L2,M17&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="N31" t="b">
+        <f>AND(N17=-Shared_Lines_Offset!M2,N17&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="2:14">
+      <c r="B32" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C32" t="b">
+        <f>AND(C18=-Shared_Lines_Offset!B3,C18&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="D32" t="b">
+        <f>AND(D18=-Shared_Lines_Offset!C3,D18&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="E32" t="b">
+        <f>AND(E18=-Shared_Lines_Offset!D3,E18&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="F32" t="b">
+        <f>AND(F18=-Shared_Lines_Offset!E3,F18&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="G32" t="b">
+        <f>AND(G18=-Shared_Lines_Offset!F3,G18&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="H32" t="b">
+        <f>AND(H18=-Shared_Lines_Offset!G3,H18&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="I32" t="b">
+        <f>AND(I18=-Shared_Lines_Offset!H3,I18&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="J32" t="b">
+        <f>AND(J18=-Shared_Lines_Offset!I3,J18&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="K32" t="b">
+        <f>AND(K18=-Shared_Lines_Offset!J3,K18&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="L32" t="b">
+        <f>AND(L18=-Shared_Lines_Offset!K3,L18&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="M32" t="b">
+        <f>AND(M18=-Shared_Lines_Offset!L3,M18&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="N32" t="b">
+        <f>AND(N18=-Shared_Lines_Offset!M3,N18&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="2:14">
+      <c r="B33" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="C33" t="b">
+        <f>AND(C19=-Shared_Lines_Offset!B4,C19&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="D33" t="b">
+        <f>AND(D19=-Shared_Lines_Offset!C4,D19&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="E33" t="b">
+        <f>AND(E19=-Shared_Lines_Offset!D4,E19&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="F33" t="b">
+        <f>AND(F19=-Shared_Lines_Offset!E4,F19&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="G33" t="b">
+        <f>AND(G19=-Shared_Lines_Offset!F4,G19&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="H33" t="b">
+        <f>AND(H19=-Shared_Lines_Offset!G4,H19&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="I33" t="b">
+        <f>AND(I19=-Shared_Lines_Offset!H4,I19&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="J33" t="b">
+        <f>AND(J19=-Shared_Lines_Offset!I4,J19&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="K33" t="b">
+        <f>AND(K19=-Shared_Lines_Offset!J4,K19&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="L33" t="b">
+        <f>AND(L19=-Shared_Lines_Offset!K4,L19&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="M33" t="b">
+        <f>AND(M19=-Shared_Lines_Offset!L4,M19&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="N33" t="b">
+        <f>AND(N19=-Shared_Lines_Offset!M4,N19&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="2:14">
+      <c r="B34" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="C34" t="b">
+        <f>AND(C20=-Shared_Lines_Offset!B5,C20&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="D34" t="b">
+        <f>AND(D20=-Shared_Lines_Offset!C5,D20&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="E34" t="b">
+        <f>AND(E20=-Shared_Lines_Offset!D5,E20&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="F34" t="b">
+        <f>AND(F20=-Shared_Lines_Offset!E5,F20&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="G34" t="b">
+        <f>AND(G20=-Shared_Lines_Offset!F5,G20&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="H34" t="b">
+        <f>AND(H20=-Shared_Lines_Offset!G5,H20&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="I34" t="b">
+        <f>AND(I20=-Shared_Lines_Offset!H5,I20&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="J34" t="b">
+        <f>AND(J20=-Shared_Lines_Offset!I5,J20&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="K34" t="b">
+        <f>AND(K20=-Shared_Lines_Offset!J5,K20&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="L34" t="b">
+        <f>AND(L20=-Shared_Lines_Offset!K5,L20&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="M34" t="b">
+        <f>AND(M20=-Shared_Lines_Offset!L5,M20&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="N34" t="b">
+        <f>AND(N20=-Shared_Lines_Offset!M5,N20&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="2:14">
+      <c r="B35" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="C35" t="b">
+        <f>AND(C21=-Shared_Lines_Offset!B6,C21&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="D35" t="b">
+        <f>AND(D21=-Shared_Lines_Offset!C6,D21&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="E35" t="b">
+        <f>AND(E21=-Shared_Lines_Offset!D6,E21&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="F35" t="b">
+        <f>AND(F21=-Shared_Lines_Offset!E6,F21&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="G35" t="b">
+        <f>AND(G21=-Shared_Lines_Offset!F6,G21&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="H35" t="b">
+        <f>AND(H21=-Shared_Lines_Offset!G6,H21&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="I35" t="b">
+        <f>AND(I21=-Shared_Lines_Offset!H6,I21&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="J35" t="b">
+        <f>AND(J21=-Shared_Lines_Offset!I6,J21&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="K35" t="b">
+        <f>AND(K21=-Shared_Lines_Offset!J6,K21&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="L35" t="b">
+        <f>AND(L21=-Shared_Lines_Offset!K6,L21&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="M35" t="b">
+        <f>AND(M21=-Shared_Lines_Offset!L6,M21&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="N35" t="b">
+        <f>AND(N21=-Shared_Lines_Offset!M6,N21&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="2:14">
+      <c r="B36" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="C36" t="b">
+        <f>AND(C22=-Shared_Lines_Offset!B7,C22&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="D36" t="b">
+        <f>AND(D22=-Shared_Lines_Offset!C7,D22&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="E36" t="b">
+        <f>AND(E22=-Shared_Lines_Offset!D7,E22&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="F36" t="b">
+        <f>AND(F22=-Shared_Lines_Offset!E7,F22&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="G36" t="b">
+        <f>AND(G22=-Shared_Lines_Offset!F7,G22&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="H36" t="b">
+        <f>AND(H22=-Shared_Lines_Offset!G7,H22&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="I36" t="b">
+        <f>AND(I22=-Shared_Lines_Offset!H7,I22&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="J36" t="b">
+        <f>AND(J22=-Shared_Lines_Offset!I7,J22&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="K36" t="b">
+        <f>AND(K22=-Shared_Lines_Offset!J7,K22&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="L36" s="4" t="b">
+        <f>AND(L22=-Shared_Lines_Offset!K7,L22&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="M36" t="b">
+        <f>AND(M22=-Shared_Lines_Offset!L7,M22&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="N36" t="b">
+        <f>AND(N22=-Shared_Lines_Offset!M7,N22&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="2:14">
+      <c r="B37" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="C37" t="b">
+        <f>AND(C23=-Shared_Lines_Offset!B8,C23&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="D37" t="b">
+        <f>AND(D23=-Shared_Lines_Offset!C8,D23&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="E37" t="b">
+        <f>AND(E23=-Shared_Lines_Offset!D8,E23&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="F37" t="b">
+        <f>AND(F23=-Shared_Lines_Offset!E8,F23&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="G37" t="b">
+        <f>AND(G23=-Shared_Lines_Offset!F8,G23&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="H37" t="b">
+        <f>AND(H23=-Shared_Lines_Offset!G8,H23&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="I37" t="b">
+        <f>AND(I23=-Shared_Lines_Offset!H8,I23&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="J37" t="b">
+        <f>AND(J23=-Shared_Lines_Offset!I8,J23&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="K37" t="b">
+        <f>AND(K23=-Shared_Lines_Offset!J8,K23&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="L37" t="b">
+        <f>AND(L23=-Shared_Lines_Offset!K8,L23&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="M37" t="b">
+        <f>AND(M23=-Shared_Lines_Offset!L8,M23&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="N37" t="b">
+        <f>AND(N23=-Shared_Lines_Offset!M8,N23&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="2:14">
+      <c r="B38" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="C38" t="b">
+        <f>AND(C24=-Shared_Lines_Offset!B9,C24&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="D38" t="b">
+        <f>AND(D24=-Shared_Lines_Offset!C9,D24&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="E38" t="b">
+        <f>AND(E24=-Shared_Lines_Offset!D9,E24&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="F38" t="b">
+        <f>AND(F24=-Shared_Lines_Offset!E9,F24&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="G38" t="b">
+        <f>AND(G24=-Shared_Lines_Offset!F9,G24&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="H38" t="b">
+        <f>AND(H24=-Shared_Lines_Offset!G9,H24&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="I38" t="b">
+        <f>AND(I24=-Shared_Lines_Offset!H9,I24&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="J38" t="b">
+        <f>AND(J24=-Shared_Lines_Offset!I9,J24&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="K38" t="b">
+        <f>AND(K24=-Shared_Lines_Offset!J9,K24&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="L38" t="b">
+        <f>AND(L24=-Shared_Lines_Offset!K9,L24&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="M38" t="b">
+        <f>AND(M24=-Shared_Lines_Offset!L9,M24&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="N38" t="b">
+        <f>AND(N24=-Shared_Lines_Offset!M9,N24&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="2:14">
+      <c r="B39" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="C39" t="b">
+        <f>AND(C25=-Shared_Lines_Offset!B10,C25&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="D39" t="b">
+        <f>AND(D25=-Shared_Lines_Offset!C10,D25&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="E39" t="b">
+        <f>AND(E25=-Shared_Lines_Offset!D10,E25&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="F39" t="b">
+        <f>AND(F25=-Shared_Lines_Offset!E10,F25&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="G39" t="b">
+        <f>AND(G25=-Shared_Lines_Offset!F10,G25&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="H39" t="b">
+        <f>AND(H25=-Shared_Lines_Offset!G10,H25&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="I39" t="b">
+        <f>AND(I25=-Shared_Lines_Offset!H10,I25&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="J39" t="b">
+        <f>AND(J25=-Shared_Lines_Offset!I10,J25&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="K39" t="b">
+        <f>AND(K25=-Shared_Lines_Offset!J10,K25&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="L39" t="b">
+        <f>AND(L25=-Shared_Lines_Offset!K10,L25&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="M39" t="b">
+        <f>AND(M25=-Shared_Lines_Offset!L10,M25&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="N39" t="b">
+        <f>AND(N25=-Shared_Lines_Offset!M10,N25&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="2:14">
+      <c r="B40" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C40" t="b">
+        <f>AND(C26=-Shared_Lines_Offset!B11,C26&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="D40" t="b">
+        <f>AND(D26=-Shared_Lines_Offset!C11,D26&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="E40" t="b">
+        <f>AND(E26=-Shared_Lines_Offset!D11,E26&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="F40" t="b">
+        <f>AND(F26=-Shared_Lines_Offset!E11,F26&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="G40" t="b">
+        <f>AND(G26=-Shared_Lines_Offset!F11,G26&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="H40" t="b">
+        <f>AND(H26=-Shared_Lines_Offset!G11,H26&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="I40" t="b">
+        <f>AND(I26=-Shared_Lines_Offset!H11,I26&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="J40" t="b">
+        <f>AND(J26=-Shared_Lines_Offset!I11,J26&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="K40" t="b">
+        <f>AND(K26=-Shared_Lines_Offset!J11,K26&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="L40" t="b">
+        <f>AND(L26=-Shared_Lines_Offset!K11,L26&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="M40" t="b">
+        <f>AND(M26=-Shared_Lines_Offset!L11,M26&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="N40" t="b">
+        <f>AND(N26=-Shared_Lines_Offset!M11,N26&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="2:14">
+      <c r="B41" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="C41" t="b">
+        <f>AND(C27=-Shared_Lines_Offset!B12,C27&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="D41" t="b">
+        <f>AND(D27=-Shared_Lines_Offset!C12,D27&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="E41" t="b">
+        <f>AND(E27=-Shared_Lines_Offset!D12,E27&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="F41" t="b">
+        <f>AND(F27=-Shared_Lines_Offset!E12,F27&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="G41" t="b">
+        <f>AND(G27=-Shared_Lines_Offset!F12,G27&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="H41" t="b">
+        <f>AND(H27=-Shared_Lines_Offset!G12,H27&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="I41" t="b">
+        <f>AND(I27=-Shared_Lines_Offset!H12,I27&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="J41" t="b">
+        <f>AND(J27=-Shared_Lines_Offset!I12,J27&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="K41" t="b">
+        <f>AND(K27=-Shared_Lines_Offset!J12,K27&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="L41" t="b">
+        <f>AND(L27=-Shared_Lines_Offset!K12,L27&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="M41" t="b">
+        <f>AND(M27=-Shared_Lines_Offset!L12,M27&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="N41" t="b">
+        <f>AND(N27=-Shared_Lines_Offset!M12,N27&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="2:14">
+      <c r="B42" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C42" t="b">
+        <f>AND(C28=-Shared_Lines_Offset!B13,C28&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="D42" t="b">
+        <f>AND(D28=-Shared_Lines_Offset!C13,D28&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="E42" t="b">
+        <f>AND(E28=-Shared_Lines_Offset!D13,E28&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="F42" t="b">
+        <f>AND(F28=-Shared_Lines_Offset!E13,F28&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="G42" t="b">
+        <f>AND(G28=-Shared_Lines_Offset!F13,G28&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="H42" t="b">
+        <f>AND(H28=-Shared_Lines_Offset!G13,H28&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="I42" t="b">
+        <f>AND(I28=-Shared_Lines_Offset!H13,I28&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="J42" t="b">
+        <f>AND(J28=-Shared_Lines_Offset!I13,J28&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="K42" t="b">
+        <f>AND(K28=-Shared_Lines_Offset!J13,K28&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="L42" t="b">
+        <f>AND(L28=-Shared_Lines_Offset!K13,L28&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="M42" t="b">
+        <f>AND(M28=-Shared_Lines_Offset!L13,M28&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="N42" t="b">
+        <f>AND(N28=-Shared_Lines_Offset!M13,N28&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N67"/>
@@ -8801,7 +10933,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+    <sheetView topLeftCell="A20" workbookViewId="0">
       <selection activeCell="B50" sqref="B50"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
added sat eve orig test
</commit_message>
<xml_diff>
--- a/data/Times_to_Transfer_Stations.xlsx
+++ b/data/Times_to_Transfer_Stations.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25725"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="3960" yWindow="0" windowWidth="25600" windowHeight="15860" tabRatio="564" firstSheet="7" activeTab="9"/>
+    <workbookView xWindow="3960" yWindow="0" windowWidth="25600" windowHeight="15860" tabRatio="564" firstSheet="7" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="Station_Time_Calculations" sheetId="1" r:id="rId1"/>
@@ -15,8 +15,9 @@
     <sheet name="Shared_Lines" sheetId="6" r:id="rId6"/>
     <sheet name="Shared_Lines_Offset" sheetId="7" r:id="rId7"/>
     <sheet name="shared_test_sat_morn_orig" sheetId="8" r:id="rId8"/>
-    <sheet name="shared_test_sat_morn_abs1" sheetId="9" r:id="rId9"/>
-    <sheet name="shared_test_sat_eve_abs1" sheetId="10" r:id="rId10"/>
+    <sheet name="shared_test_sat_eve_orig" sheetId="11" r:id="rId9"/>
+    <sheet name="shared_test_sat_morn_abs1" sheetId="9" r:id="rId10"/>
+    <sheet name="shared_test_sat_eve_abs1" sheetId="10" r:id="rId11"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1061" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1137" uniqueCount="113">
   <si>
     <t>-</t>
   </si>
@@ -366,7 +367,7 @@
     <t>arrive rosslyn</t>
   </si>
   <si>
-    <t>*shared lines constraint violated for Orange_neg, Silver_neg</t>
+    <t>*shared lines constraint violated for Orange_neg, Silver_neg, and Blue_pos, Orange_pos</t>
   </si>
 </sst>
 </file>
@@ -433,8 +434,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="151">
+  <cellStyleXfs count="157">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -593,7 +600,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="151">
+  <cellStyles count="157">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -669,6 +676,9 @@
     <cellStyle name="Followed Hyperlink" xfId="146" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="148" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="150" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="152" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="154" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="156" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -744,6 +754,9 @@
     <cellStyle name="Hyperlink" xfId="145" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="147" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="149" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="151" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="153" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="155" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1697,7 +1710,2134 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+    <sheetView topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="B50" sqref="B50"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:14">
+      <c r="C1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14">
+      <c r="A2" s="1"/>
+      <c r="B2" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="C2" s="1">
+        <v>4</v>
+      </c>
+      <c r="D2" s="1">
+        <v>9</v>
+      </c>
+      <c r="E2" s="1">
+        <v>10</v>
+      </c>
+      <c r="F2" s="1">
+        <v>9</v>
+      </c>
+      <c r="G2" s="1">
+        <v>4</v>
+      </c>
+      <c r="H2" s="1">
+        <v>9</v>
+      </c>
+      <c r="I2" s="1">
+        <v>0</v>
+      </c>
+      <c r="J2" s="1">
+        <v>11</v>
+      </c>
+      <c r="K2" s="1">
+        <v>4</v>
+      </c>
+      <c r="L2" s="1">
+        <v>9</v>
+      </c>
+      <c r="M2" s="1">
+        <v>10</v>
+      </c>
+      <c r="N2" s="1">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14">
+      <c r="A3" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" s="1">
+        <v>4</v>
+      </c>
+      <c r="C3">
+        <f>$B3-C$2</f>
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <f t="shared" ref="D3:N14" si="0">$B3-D$2</f>
+        <v>-5</v>
+      </c>
+      <c r="E3">
+        <f t="shared" si="0"/>
+        <v>-6</v>
+      </c>
+      <c r="F3">
+        <f t="shared" si="0"/>
+        <v>-5</v>
+      </c>
+      <c r="G3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <f t="shared" si="0"/>
+        <v>-5</v>
+      </c>
+      <c r="I3">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="J3">
+        <f t="shared" si="0"/>
+        <v>-7</v>
+      </c>
+      <c r="K3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L3">
+        <f t="shared" si="0"/>
+        <v>-5</v>
+      </c>
+      <c r="M3">
+        <f t="shared" si="0"/>
+        <v>-6</v>
+      </c>
+      <c r="N3">
+        <f t="shared" si="0"/>
+        <v>-5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14">
+      <c r="A4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="1">
+        <v>9</v>
+      </c>
+      <c r="C4">
+        <f t="shared" ref="C4:C14" si="1">$B4-C$2</f>
+        <v>5</v>
+      </c>
+      <c r="D4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+      <c r="F4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="H4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I4">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="J4">
+        <f t="shared" si="0"/>
+        <v>-2</v>
+      </c>
+      <c r="K4">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="L4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M4">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+      <c r="N4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14">
+      <c r="A5" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B5" s="1">
+        <v>10</v>
+      </c>
+      <c r="C5">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="D5">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="G5">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="H5">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="I5">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="J5">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+      <c r="K5">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="L5">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="M5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N5">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14">
+      <c r="A6" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B6" s="1">
+        <v>9</v>
+      </c>
+      <c r="C6">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="D6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+      <c r="F6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="H6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I6">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="J6">
+        <f t="shared" si="0"/>
+        <v>-2</v>
+      </c>
+      <c r="K6">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="L6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M6">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+      <c r="N6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14">
+      <c r="A7" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B7" s="1">
+        <v>4</v>
+      </c>
+      <c r="C7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <f t="shared" si="0"/>
+        <v>-5</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="0"/>
+        <v>-6</v>
+      </c>
+      <c r="F7">
+        <f t="shared" si="0"/>
+        <v>-5</v>
+      </c>
+      <c r="G7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H7">
+        <f t="shared" si="0"/>
+        <v>-5</v>
+      </c>
+      <c r="I7">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="J7">
+        <f t="shared" si="0"/>
+        <v>-7</v>
+      </c>
+      <c r="K7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L7">
+        <f t="shared" si="0"/>
+        <v>-5</v>
+      </c>
+      <c r="M7">
+        <f t="shared" si="0"/>
+        <v>-6</v>
+      </c>
+      <c r="N7">
+        <f t="shared" si="0"/>
+        <v>-5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14">
+      <c r="A8" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="B8" s="1">
+        <v>9</v>
+      </c>
+      <c r="C8">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="D8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+      <c r="F8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="H8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I8">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="J8">
+        <f t="shared" si="0"/>
+        <v>-2</v>
+      </c>
+      <c r="K8">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="L8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M8">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+      <c r="N8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14">
+      <c r="A9" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B9" s="1">
+        <v>0</v>
+      </c>
+      <c r="C9">
+        <f t="shared" si="1"/>
+        <v>-4</v>
+      </c>
+      <c r="D9">
+        <f t="shared" si="0"/>
+        <v>-9</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="0"/>
+        <v>-10</v>
+      </c>
+      <c r="F9">
+        <f t="shared" si="0"/>
+        <v>-9</v>
+      </c>
+      <c r="G9">
+        <f t="shared" si="0"/>
+        <v>-4</v>
+      </c>
+      <c r="H9">
+        <f t="shared" si="0"/>
+        <v>-9</v>
+      </c>
+      <c r="I9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J9">
+        <f t="shared" si="0"/>
+        <v>-11</v>
+      </c>
+      <c r="K9">
+        <f t="shared" si="0"/>
+        <v>-4</v>
+      </c>
+      <c r="L9">
+        <f t="shared" si="0"/>
+        <v>-9</v>
+      </c>
+      <c r="M9">
+        <f t="shared" si="0"/>
+        <v>-10</v>
+      </c>
+      <c r="N9">
+        <f t="shared" si="0"/>
+        <v>-9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14">
+      <c r="A10" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B10" s="1">
+        <v>11</v>
+      </c>
+      <c r="C10">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="D10">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="F10">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="G10">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="H10">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="I10">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="J10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K10">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="L10">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="M10">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="N10">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14">
+      <c r="A11" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="B11" s="1">
+        <v>4</v>
+      </c>
+      <c r="C11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <f t="shared" si="0"/>
+        <v>-5</v>
+      </c>
+      <c r="E11">
+        <f t="shared" si="0"/>
+        <v>-6</v>
+      </c>
+      <c r="F11">
+        <f t="shared" si="0"/>
+        <v>-5</v>
+      </c>
+      <c r="G11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H11">
+        <f t="shared" si="0"/>
+        <v>-5</v>
+      </c>
+      <c r="I11">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="J11">
+        <f t="shared" si="0"/>
+        <v>-7</v>
+      </c>
+      <c r="K11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L11">
+        <f t="shared" si="0"/>
+        <v>-5</v>
+      </c>
+      <c r="M11">
+        <f t="shared" si="0"/>
+        <v>-6</v>
+      </c>
+      <c r="N11">
+        <f t="shared" si="0"/>
+        <v>-5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14">
+      <c r="A12" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="B12" s="1">
+        <v>9</v>
+      </c>
+      <c r="C12">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="D12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E12">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+      <c r="F12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G12">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="H12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I12">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="J12">
+        <f t="shared" si="0"/>
+        <v>-2</v>
+      </c>
+      <c r="K12">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="L12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M12">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+      <c r="N12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14">
+      <c r="A13" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="B13" s="1">
+        <v>10</v>
+      </c>
+      <c r="C13">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="D13">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F13">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="G13">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="H13">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="I13">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="J13">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+      <c r="K13">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="L13">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="M13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N13">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14">
+      <c r="A14" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B14" s="1">
+        <v>9</v>
+      </c>
+      <c r="C14">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="D14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E14">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+      <c r="F14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G14">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="H14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I14">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="J14">
+        <f t="shared" si="0"/>
+        <v>-2</v>
+      </c>
+      <c r="K14">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="L14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M14">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+      <c r="N14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14">
+      <c r="B16" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="J16" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="K16" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="L16" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="M16" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="N16" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="17" spans="2:14">
+      <c r="B17" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C17">
+        <f>C3*Shared_Lines!B2</f>
+        <v>0</v>
+      </c>
+      <c r="D17">
+        <f>D3*Shared_Lines!C2</f>
+        <v>0</v>
+      </c>
+      <c r="E17">
+        <f>E3*Shared_Lines!D2</f>
+        <v>0</v>
+      </c>
+      <c r="F17">
+        <f>F3*Shared_Lines!E2</f>
+        <v>0</v>
+      </c>
+      <c r="G17">
+        <f>G3*Shared_Lines!F2</f>
+        <v>0</v>
+      </c>
+      <c r="H17">
+        <f>H3*Shared_Lines!G2</f>
+        <v>0</v>
+      </c>
+      <c r="I17">
+        <f>I3*Shared_Lines!H2</f>
+        <v>0</v>
+      </c>
+      <c r="J17">
+        <f>J3*Shared_Lines!I2</f>
+        <v>0</v>
+      </c>
+      <c r="K17">
+        <f>K3*Shared_Lines!J2</f>
+        <v>0</v>
+      </c>
+      <c r="L17">
+        <f>L3*Shared_Lines!K2</f>
+        <v>0</v>
+      </c>
+      <c r="M17">
+        <f>M3*Shared_Lines!L2</f>
+        <v>-6</v>
+      </c>
+      <c r="N17">
+        <f>N3*Shared_Lines!M2</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="2:14">
+      <c r="B18" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C18">
+        <f>C4*Shared_Lines!B3</f>
+        <v>0</v>
+      </c>
+      <c r="D18">
+        <f>D4*Shared_Lines!C3</f>
+        <v>0</v>
+      </c>
+      <c r="E18">
+        <f>E4*Shared_Lines!D3</f>
+        <v>0</v>
+      </c>
+      <c r="F18">
+        <f>F4*Shared_Lines!E3</f>
+        <v>0</v>
+      </c>
+      <c r="G18">
+        <f>G4*Shared_Lines!F3</f>
+        <v>0</v>
+      </c>
+      <c r="H18">
+        <f>H4*Shared_Lines!G3</f>
+        <v>0</v>
+      </c>
+      <c r="I18">
+        <f>I4*Shared_Lines!H3</f>
+        <v>0</v>
+      </c>
+      <c r="J18">
+        <f>J4*Shared_Lines!I3</f>
+        <v>0</v>
+      </c>
+      <c r="K18">
+        <f>K4*Shared_Lines!J3</f>
+        <v>0</v>
+      </c>
+      <c r="L18">
+        <f>L4*Shared_Lines!K3</f>
+        <v>0</v>
+      </c>
+      <c r="M18">
+        <f>M4*Shared_Lines!L3</f>
+        <v>0</v>
+      </c>
+      <c r="N18">
+        <f>N4*Shared_Lines!M3</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="2:14">
+      <c r="B19" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="C19">
+        <f>C5*Shared_Lines!B4</f>
+        <v>0</v>
+      </c>
+      <c r="D19">
+        <f>D5*Shared_Lines!C4</f>
+        <v>0</v>
+      </c>
+      <c r="E19">
+        <f>E5*Shared_Lines!D4</f>
+        <v>0</v>
+      </c>
+      <c r="F19">
+        <f>F5*Shared_Lines!E4</f>
+        <v>0</v>
+      </c>
+      <c r="G19">
+        <f>G5*Shared_Lines!F4</f>
+        <v>0</v>
+      </c>
+      <c r="H19">
+        <f>H5*Shared_Lines!G4</f>
+        <v>0</v>
+      </c>
+      <c r="I19">
+        <f>I5*Shared_Lines!H4</f>
+        <v>0</v>
+      </c>
+      <c r="J19">
+        <f>J5*Shared_Lines!I4</f>
+        <v>0</v>
+      </c>
+      <c r="K19">
+        <f>K5*Shared_Lines!J4</f>
+        <v>0</v>
+      </c>
+      <c r="L19">
+        <f>L5*Shared_Lines!K4</f>
+        <v>0</v>
+      </c>
+      <c r="M19">
+        <f>M5*Shared_Lines!L4</f>
+        <v>0</v>
+      </c>
+      <c r="N19">
+        <f>N5*Shared_Lines!M4</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="2:14">
+      <c r="B20" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="C20">
+        <f>C6*Shared_Lines!B5</f>
+        <v>0</v>
+      </c>
+      <c r="D20">
+        <f>D6*Shared_Lines!C5</f>
+        <v>0</v>
+      </c>
+      <c r="E20">
+        <f>E6*Shared_Lines!D5</f>
+        <v>0</v>
+      </c>
+      <c r="F20">
+        <f>F6*Shared_Lines!E5</f>
+        <v>0</v>
+      </c>
+      <c r="G20">
+        <f>G6*Shared_Lines!F5</f>
+        <v>0</v>
+      </c>
+      <c r="H20">
+        <f>H6*Shared_Lines!G5</f>
+        <v>0</v>
+      </c>
+      <c r="I20">
+        <f>I6*Shared_Lines!H5</f>
+        <v>0</v>
+      </c>
+      <c r="J20">
+        <f>J6*Shared_Lines!I5</f>
+        <v>0</v>
+      </c>
+      <c r="K20">
+        <f>K6*Shared_Lines!J5</f>
+        <v>0</v>
+      </c>
+      <c r="L20">
+        <f>L6*Shared_Lines!K5</f>
+        <v>0</v>
+      </c>
+      <c r="M20">
+        <f>M6*Shared_Lines!L5</f>
+        <v>0</v>
+      </c>
+      <c r="N20">
+        <f>N6*Shared_Lines!M5</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="2:14">
+      <c r="B21" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="C21">
+        <f>C7*Shared_Lines!B6</f>
+        <v>0</v>
+      </c>
+      <c r="D21">
+        <f>D7*Shared_Lines!C6</f>
+        <v>0</v>
+      </c>
+      <c r="E21">
+        <f>E7*Shared_Lines!D6</f>
+        <v>0</v>
+      </c>
+      <c r="F21">
+        <f>F7*Shared_Lines!E6</f>
+        <v>0</v>
+      </c>
+      <c r="G21">
+        <f>G7*Shared_Lines!F6</f>
+        <v>0</v>
+      </c>
+      <c r="H21">
+        <f>H7*Shared_Lines!G6</f>
+        <v>0</v>
+      </c>
+      <c r="I21">
+        <f>I7*Shared_Lines!H6</f>
+        <v>0</v>
+      </c>
+      <c r="J21">
+        <f>J7*Shared_Lines!I6</f>
+        <v>0</v>
+      </c>
+      <c r="K21">
+        <f>K7*Shared_Lines!J6</f>
+        <v>0</v>
+      </c>
+      <c r="L21">
+        <f>L7*Shared_Lines!K6</f>
+        <v>0</v>
+      </c>
+      <c r="M21">
+        <f>M7*Shared_Lines!L6</f>
+        <v>0</v>
+      </c>
+      <c r="N21">
+        <f>N7*Shared_Lines!M6</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="2:14">
+      <c r="B22" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="C22">
+        <f>C8*Shared_Lines!B7</f>
+        <v>0</v>
+      </c>
+      <c r="D22">
+        <f>D8*Shared_Lines!C7</f>
+        <v>0</v>
+      </c>
+      <c r="E22">
+        <f>E8*Shared_Lines!D7</f>
+        <v>0</v>
+      </c>
+      <c r="F22">
+        <f>F8*Shared_Lines!E7</f>
+        <v>0</v>
+      </c>
+      <c r="G22">
+        <f>G8*Shared_Lines!F7</f>
+        <v>0</v>
+      </c>
+      <c r="H22">
+        <f>H8*Shared_Lines!G7</f>
+        <v>0</v>
+      </c>
+      <c r="I22">
+        <f>I8*Shared_Lines!H7</f>
+        <v>0</v>
+      </c>
+      <c r="J22">
+        <f>J8*Shared_Lines!I7</f>
+        <v>0</v>
+      </c>
+      <c r="K22">
+        <f>K8*Shared_Lines!J7</f>
+        <v>0</v>
+      </c>
+      <c r="L22">
+        <f>L8*Shared_Lines!K7</f>
+        <v>0</v>
+      </c>
+      <c r="M22">
+        <f>M8*Shared_Lines!L7</f>
+        <v>0</v>
+      </c>
+      <c r="N22">
+        <f>N8*Shared_Lines!M7</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="2:14">
+      <c r="B23" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="C23">
+        <f>C9*Shared_Lines!B8</f>
+        <v>0</v>
+      </c>
+      <c r="D23">
+        <f>D9*Shared_Lines!C8</f>
+        <v>0</v>
+      </c>
+      <c r="E23">
+        <f>E9*Shared_Lines!D8</f>
+        <v>0</v>
+      </c>
+      <c r="F23">
+        <f>F9*Shared_Lines!E8</f>
+        <v>0</v>
+      </c>
+      <c r="G23">
+        <f>G9*Shared_Lines!F8</f>
+        <v>0</v>
+      </c>
+      <c r="H23">
+        <f>H9*Shared_Lines!G8</f>
+        <v>0</v>
+      </c>
+      <c r="I23">
+        <f>I9*Shared_Lines!H8</f>
+        <v>0</v>
+      </c>
+      <c r="J23">
+        <f>J9*Shared_Lines!I8</f>
+        <v>0</v>
+      </c>
+      <c r="K23">
+        <f>K9*Shared_Lines!J8</f>
+        <v>0</v>
+      </c>
+      <c r="L23">
+        <f>L9*Shared_Lines!K8</f>
+        <v>0</v>
+      </c>
+      <c r="M23">
+        <f>M9*Shared_Lines!L8</f>
+        <v>0</v>
+      </c>
+      <c r="N23">
+        <f>N9*Shared_Lines!M8</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="2:14">
+      <c r="B24" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="C24">
+        <f>C10*Shared_Lines!B9</f>
+        <v>0</v>
+      </c>
+      <c r="D24">
+        <f>D10*Shared_Lines!C9</f>
+        <v>0</v>
+      </c>
+      <c r="E24">
+        <f>E10*Shared_Lines!D9</f>
+        <v>0</v>
+      </c>
+      <c r="F24">
+        <f>F10*Shared_Lines!E9</f>
+        <v>0</v>
+      </c>
+      <c r="G24">
+        <f>G10*Shared_Lines!F9</f>
+        <v>0</v>
+      </c>
+      <c r="H24">
+        <f>H10*Shared_Lines!G9</f>
+        <v>0</v>
+      </c>
+      <c r="I24">
+        <f>I10*Shared_Lines!H9</f>
+        <v>0</v>
+      </c>
+      <c r="J24">
+        <f>J10*Shared_Lines!I9</f>
+        <v>0</v>
+      </c>
+      <c r="K24">
+        <f>K10*Shared_Lines!J9</f>
+        <v>0</v>
+      </c>
+      <c r="L24">
+        <f>L10*Shared_Lines!K9</f>
+        <v>0</v>
+      </c>
+      <c r="M24">
+        <f>M10*Shared_Lines!L9</f>
+        <v>0</v>
+      </c>
+      <c r="N24">
+        <f>N10*Shared_Lines!M9</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="2:14">
+      <c r="B25" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="C25">
+        <f>C11*Shared_Lines!B10</f>
+        <v>0</v>
+      </c>
+      <c r="D25">
+        <f>D11*Shared_Lines!C10</f>
+        <v>0</v>
+      </c>
+      <c r="E25">
+        <f>E11*Shared_Lines!D10</f>
+        <v>0</v>
+      </c>
+      <c r="F25">
+        <f>F11*Shared_Lines!E10</f>
+        <v>0</v>
+      </c>
+      <c r="G25">
+        <f>G11*Shared_Lines!F10</f>
+        <v>0</v>
+      </c>
+      <c r="H25">
+        <f>H11*Shared_Lines!G10</f>
+        <v>0</v>
+      </c>
+      <c r="I25">
+        <f>I11*Shared_Lines!H10</f>
+        <v>0</v>
+      </c>
+      <c r="J25">
+        <f>J11*Shared_Lines!I10</f>
+        <v>0</v>
+      </c>
+      <c r="K25">
+        <f>K11*Shared_Lines!J10</f>
+        <v>0</v>
+      </c>
+      <c r="L25">
+        <f>L11*Shared_Lines!K10</f>
+        <v>0</v>
+      </c>
+      <c r="M25">
+        <f>M11*Shared_Lines!L10</f>
+        <v>0</v>
+      </c>
+      <c r="N25">
+        <f>N11*Shared_Lines!M10</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="2:14">
+      <c r="B26" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C26">
+        <f>C12*Shared_Lines!B11</f>
+        <v>0</v>
+      </c>
+      <c r="D26">
+        <f>D12*Shared_Lines!C11</f>
+        <v>0</v>
+      </c>
+      <c r="E26">
+        <f>E12*Shared_Lines!D11</f>
+        <v>0</v>
+      </c>
+      <c r="F26">
+        <f>F12*Shared_Lines!E11</f>
+        <v>0</v>
+      </c>
+      <c r="G26">
+        <f>G12*Shared_Lines!F11</f>
+        <v>0</v>
+      </c>
+      <c r="H26">
+        <f>H12*Shared_Lines!G11</f>
+        <v>0</v>
+      </c>
+      <c r="I26">
+        <f>I12*Shared_Lines!H11</f>
+        <v>0</v>
+      </c>
+      <c r="J26">
+        <f>J12*Shared_Lines!I11</f>
+        <v>0</v>
+      </c>
+      <c r="K26">
+        <f>K12*Shared_Lines!J11</f>
+        <v>0</v>
+      </c>
+      <c r="L26">
+        <f>L12*Shared_Lines!K11</f>
+        <v>0</v>
+      </c>
+      <c r="M26">
+        <f>M12*Shared_Lines!L11</f>
+        <v>0</v>
+      </c>
+      <c r="N26">
+        <f>N12*Shared_Lines!M11</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="2:14">
+      <c r="B27" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="C27">
+        <f>C13*Shared_Lines!B12</f>
+        <v>0</v>
+      </c>
+      <c r="D27">
+        <f>D13*Shared_Lines!C12</f>
+        <v>0</v>
+      </c>
+      <c r="E27">
+        <f>E13*Shared_Lines!D12</f>
+        <v>0</v>
+      </c>
+      <c r="F27">
+        <f>F13*Shared_Lines!E12</f>
+        <v>0</v>
+      </c>
+      <c r="G27">
+        <f>G13*Shared_Lines!F12</f>
+        <v>0</v>
+      </c>
+      <c r="H27">
+        <f>H13*Shared_Lines!G12</f>
+        <v>0</v>
+      </c>
+      <c r="I27">
+        <f>I13*Shared_Lines!H12</f>
+        <v>0</v>
+      </c>
+      <c r="J27">
+        <f>J13*Shared_Lines!I12</f>
+        <v>0</v>
+      </c>
+      <c r="K27">
+        <f>K13*Shared_Lines!J12</f>
+        <v>0</v>
+      </c>
+      <c r="L27">
+        <f>L13*Shared_Lines!K12</f>
+        <v>0</v>
+      </c>
+      <c r="M27">
+        <f>M13*Shared_Lines!L12</f>
+        <v>0</v>
+      </c>
+      <c r="N27">
+        <f>N13*Shared_Lines!M12</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="2:14">
+      <c r="B28" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C28">
+        <f>C14*Shared_Lines!B13</f>
+        <v>0</v>
+      </c>
+      <c r="D28">
+        <f>D14*Shared_Lines!C13</f>
+        <v>0</v>
+      </c>
+      <c r="E28">
+        <f>E14*Shared_Lines!D13</f>
+        <v>0</v>
+      </c>
+      <c r="F28">
+        <f>F14*Shared_Lines!E13</f>
+        <v>0</v>
+      </c>
+      <c r="G28">
+        <f>G14*Shared_Lines!F13</f>
+        <v>0</v>
+      </c>
+      <c r="H28">
+        <f>H14*Shared_Lines!G13</f>
+        <v>0</v>
+      </c>
+      <c r="I28">
+        <f>I14*Shared_Lines!H13</f>
+        <v>0</v>
+      </c>
+      <c r="J28">
+        <f>J14*Shared_Lines!I13</f>
+        <v>0</v>
+      </c>
+      <c r="K28">
+        <f>K14*Shared_Lines!J13</f>
+        <v>0</v>
+      </c>
+      <c r="L28">
+        <f>L14*Shared_Lines!K13</f>
+        <v>0</v>
+      </c>
+      <c r="M28">
+        <f>M14*Shared_Lines!L13</f>
+        <v>0</v>
+      </c>
+      <c r="N28">
+        <f>N14*Shared_Lines!M13</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="2:14">
+      <c r="B30" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="G30" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="H30" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="I30" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="J30" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="K30" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="L30" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="M30" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="N30" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="31" spans="2:14">
+      <c r="B31" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C31" t="b">
+        <f>AND(C17=-Shared_Lines_Offset!B2,C17&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="D31" t="b">
+        <f>AND(D17=-Shared_Lines_Offset!C2,D17&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="E31" t="b">
+        <f>AND(E17=-Shared_Lines_Offset!D2,E17&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="F31" t="b">
+        <f>AND(F17=-Shared_Lines_Offset!E2,F17&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="G31" t="b">
+        <f>AND(G17=-Shared_Lines_Offset!F2,G17&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="H31" t="b">
+        <f>AND(H17=-Shared_Lines_Offset!G2,H17&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="I31" t="b">
+        <f>AND(I17=-Shared_Lines_Offset!H2,I17&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="J31" t="b">
+        <f>AND(J17=-Shared_Lines_Offset!I2,J17&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="K31" t="b">
+        <f>AND(K17=-Shared_Lines_Offset!J2,K17&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="L31" t="b">
+        <f>AND(L17=-Shared_Lines_Offset!K2,L17&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="M31" t="b">
+        <f>AND(M17=-Shared_Lines_Offset!L2,M17&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="N31" t="b">
+        <f>AND(N17=-Shared_Lines_Offset!M2,N17&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="2:14">
+      <c r="B32" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C32" t="b">
+        <f>AND(C18=-Shared_Lines_Offset!B3,C18&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="D32" t="b">
+        <f>AND(D18=-Shared_Lines_Offset!C3,D18&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="E32" t="b">
+        <f>AND(E18=-Shared_Lines_Offset!D3,E18&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="F32" t="b">
+        <f>AND(F18=-Shared_Lines_Offset!E3,F18&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="G32" t="b">
+        <f>AND(G18=-Shared_Lines_Offset!F3,G18&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="H32" t="b">
+        <f>AND(H18=-Shared_Lines_Offset!G3,H18&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="I32" t="b">
+        <f>AND(I18=-Shared_Lines_Offset!H3,I18&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="J32" t="b">
+        <f>AND(J18=-Shared_Lines_Offset!I3,J18&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="K32" t="b">
+        <f>AND(K18=-Shared_Lines_Offset!J3,K18&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="L32" t="b">
+        <f>AND(L18=-Shared_Lines_Offset!K3,L18&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="M32" t="b">
+        <f>AND(M18=-Shared_Lines_Offset!L3,M18&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="N32" t="b">
+        <f>AND(N18=-Shared_Lines_Offset!M3,N18&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="2:14">
+      <c r="B33" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="C33" t="b">
+        <f>AND(C19=-Shared_Lines_Offset!B4,C19&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="D33" t="b">
+        <f>AND(D19=-Shared_Lines_Offset!C4,D19&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="E33" t="b">
+        <f>AND(E19=-Shared_Lines_Offset!D4,E19&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="F33" t="b">
+        <f>AND(F19=-Shared_Lines_Offset!E4,F19&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="G33" t="b">
+        <f>AND(G19=-Shared_Lines_Offset!F4,G19&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="H33" t="b">
+        <f>AND(H19=-Shared_Lines_Offset!G4,H19&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="I33" t="b">
+        <f>AND(I19=-Shared_Lines_Offset!H4,I19&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="J33" t="b">
+        <f>AND(J19=-Shared_Lines_Offset!I4,J19&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="K33" t="b">
+        <f>AND(K19=-Shared_Lines_Offset!J4,K19&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="L33" t="b">
+        <f>AND(L19=-Shared_Lines_Offset!K4,L19&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="M33" t="b">
+        <f>AND(M19=-Shared_Lines_Offset!L4,M19&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="N33" t="b">
+        <f>AND(N19=-Shared_Lines_Offset!M4,N19&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="2:14">
+      <c r="B34" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="C34" t="b">
+        <f>AND(C20=-Shared_Lines_Offset!B5,C20&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="D34" t="b">
+        <f>AND(D20=-Shared_Lines_Offset!C5,D20&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="E34" t="b">
+        <f>AND(E20=-Shared_Lines_Offset!D5,E20&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="F34" t="b">
+        <f>AND(F20=-Shared_Lines_Offset!E5,F20&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="G34" t="b">
+        <f>AND(G20=-Shared_Lines_Offset!F5,G20&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="H34" t="b">
+        <f>AND(H20=-Shared_Lines_Offset!G5,H20&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="I34" t="b">
+        <f>AND(I20=-Shared_Lines_Offset!H5,I20&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="J34" t="b">
+        <f>AND(J20=-Shared_Lines_Offset!I5,J20&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="K34" t="b">
+        <f>AND(K20=-Shared_Lines_Offset!J5,K20&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="L34" t="b">
+        <f>AND(L20=-Shared_Lines_Offset!K5,L20&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="M34" t="b">
+        <f>AND(M20=-Shared_Lines_Offset!L5,M20&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="N34" t="b">
+        <f>AND(N20=-Shared_Lines_Offset!M5,N20&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="2:14">
+      <c r="B35" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="C35" t="b">
+        <f>AND(C21=-Shared_Lines_Offset!B6,C21&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="D35" t="b">
+        <f>AND(D21=-Shared_Lines_Offset!C6,D21&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="E35" t="b">
+        <f>AND(E21=-Shared_Lines_Offset!D6,E21&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="F35" t="b">
+        <f>AND(F21=-Shared_Lines_Offset!E6,F21&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="G35" t="b">
+        <f>AND(G21=-Shared_Lines_Offset!F6,G21&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="H35" t="b">
+        <f>AND(H21=-Shared_Lines_Offset!G6,H21&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="I35" t="b">
+        <f>AND(I21=-Shared_Lines_Offset!H6,I21&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="J35" t="b">
+        <f>AND(J21=-Shared_Lines_Offset!I6,J21&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="K35" t="b">
+        <f>AND(K21=-Shared_Lines_Offset!J6,K21&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="L35" t="b">
+        <f>AND(L21=-Shared_Lines_Offset!K6,L21&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="M35" t="b">
+        <f>AND(M21=-Shared_Lines_Offset!L6,M21&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="N35" t="b">
+        <f>AND(N21=-Shared_Lines_Offset!M6,N21&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="2:14">
+      <c r="B36" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="C36" t="b">
+        <f>AND(C22=-Shared_Lines_Offset!B7,C22&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="D36" t="b">
+        <f>AND(D22=-Shared_Lines_Offset!C7,D22&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="E36" t="b">
+        <f>AND(E22=-Shared_Lines_Offset!D7,E22&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="F36" t="b">
+        <f>AND(F22=-Shared_Lines_Offset!E7,F22&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="G36" t="b">
+        <f>AND(G22=-Shared_Lines_Offset!F7,G22&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="H36" t="b">
+        <f>AND(H22=-Shared_Lines_Offset!G7,H22&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="I36" t="b">
+        <f>AND(I22=-Shared_Lines_Offset!H7,I22&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="J36" t="b">
+        <f>AND(J22=-Shared_Lines_Offset!I7,J22&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="K36" t="b">
+        <f>AND(K22=-Shared_Lines_Offset!J7,K22&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="L36" s="4" t="b">
+        <f>AND(L22=-Shared_Lines_Offset!K7,L22&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="M36" t="b">
+        <f>AND(M22=-Shared_Lines_Offset!L7,M22&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="N36" t="b">
+        <f>AND(N22=-Shared_Lines_Offset!M7,N22&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="2:14">
+      <c r="B37" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="C37" t="b">
+        <f>AND(C23=-Shared_Lines_Offset!B8,C23&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="D37" t="b">
+        <f>AND(D23=-Shared_Lines_Offset!C8,D23&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="E37" t="b">
+        <f>AND(E23=-Shared_Lines_Offset!D8,E23&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="F37" t="b">
+        <f>AND(F23=-Shared_Lines_Offset!E8,F23&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="G37" t="b">
+        <f>AND(G23=-Shared_Lines_Offset!F8,G23&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="H37" t="b">
+        <f>AND(H23=-Shared_Lines_Offset!G8,H23&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="I37" t="b">
+        <f>AND(I23=-Shared_Lines_Offset!H8,I23&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="J37" t="b">
+        <f>AND(J23=-Shared_Lines_Offset!I8,J23&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="K37" t="b">
+        <f>AND(K23=-Shared_Lines_Offset!J8,K23&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="L37" t="b">
+        <f>AND(L23=-Shared_Lines_Offset!K8,L23&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="M37" t="b">
+        <f>AND(M23=-Shared_Lines_Offset!L8,M23&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="N37" t="b">
+        <f>AND(N23=-Shared_Lines_Offset!M8,N23&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="2:14">
+      <c r="B38" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="C38" t="b">
+        <f>AND(C24=-Shared_Lines_Offset!B9,C24&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="D38" t="b">
+        <f>AND(D24=-Shared_Lines_Offset!C9,D24&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="E38" t="b">
+        <f>AND(E24=-Shared_Lines_Offset!D9,E24&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="F38" t="b">
+        <f>AND(F24=-Shared_Lines_Offset!E9,F24&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="G38" t="b">
+        <f>AND(G24=-Shared_Lines_Offset!F9,G24&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="H38" t="b">
+        <f>AND(H24=-Shared_Lines_Offset!G9,H24&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="I38" t="b">
+        <f>AND(I24=-Shared_Lines_Offset!H9,I24&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="J38" t="b">
+        <f>AND(J24=-Shared_Lines_Offset!I9,J24&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="K38" t="b">
+        <f>AND(K24=-Shared_Lines_Offset!J9,K24&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="L38" t="b">
+        <f>AND(L24=-Shared_Lines_Offset!K9,L24&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="M38" t="b">
+        <f>AND(M24=-Shared_Lines_Offset!L9,M24&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="N38" t="b">
+        <f>AND(N24=-Shared_Lines_Offset!M9,N24&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="2:14">
+      <c r="B39" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="C39" t="b">
+        <f>AND(C25=-Shared_Lines_Offset!B10,C25&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="D39" t="b">
+        <f>AND(D25=-Shared_Lines_Offset!C10,D25&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="E39" t="b">
+        <f>AND(E25=-Shared_Lines_Offset!D10,E25&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="F39" t="b">
+        <f>AND(F25=-Shared_Lines_Offset!E10,F25&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="G39" t="b">
+        <f>AND(G25=-Shared_Lines_Offset!F10,G25&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="H39" t="b">
+        <f>AND(H25=-Shared_Lines_Offset!G10,H25&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="I39" t="b">
+        <f>AND(I25=-Shared_Lines_Offset!H10,I25&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="J39" t="b">
+        <f>AND(J25=-Shared_Lines_Offset!I10,J25&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="K39" t="b">
+        <f>AND(K25=-Shared_Lines_Offset!J10,K25&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="L39" t="b">
+        <f>AND(L25=-Shared_Lines_Offset!K10,L25&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="M39" t="b">
+        <f>AND(M25=-Shared_Lines_Offset!L10,M25&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="N39" t="b">
+        <f>AND(N25=-Shared_Lines_Offset!M10,N25&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="2:14">
+      <c r="B40" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C40" t="b">
+        <f>AND(C26=-Shared_Lines_Offset!B11,C26&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="D40" t="b">
+        <f>AND(D26=-Shared_Lines_Offset!C11,D26&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="E40" t="b">
+        <f>AND(E26=-Shared_Lines_Offset!D11,E26&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="F40" t="b">
+        <f>AND(F26=-Shared_Lines_Offset!E11,F26&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="G40" t="b">
+        <f>AND(G26=-Shared_Lines_Offset!F11,G26&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="H40" t="b">
+        <f>AND(H26=-Shared_Lines_Offset!G11,H26&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="I40" t="b">
+        <f>AND(I26=-Shared_Lines_Offset!H11,I26&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="J40" t="b">
+        <f>AND(J26=-Shared_Lines_Offset!I11,J26&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="K40" t="b">
+        <f>AND(K26=-Shared_Lines_Offset!J11,K26&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="L40" t="b">
+        <f>AND(L26=-Shared_Lines_Offset!K11,L26&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="M40" t="b">
+        <f>AND(M26=-Shared_Lines_Offset!L11,M26&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="N40" t="b">
+        <f>AND(N26=-Shared_Lines_Offset!M11,N26&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="2:14">
+      <c r="B41" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="C41" t="b">
+        <f>AND(C27=-Shared_Lines_Offset!B12,C27&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="D41" t="b">
+        <f>AND(D27=-Shared_Lines_Offset!C12,D27&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="E41" t="b">
+        <f>AND(E27=-Shared_Lines_Offset!D12,E27&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="F41" t="b">
+        <f>AND(F27=-Shared_Lines_Offset!E12,F27&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="G41" t="b">
+        <f>AND(G27=-Shared_Lines_Offset!F12,G27&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="H41" t="b">
+        <f>AND(H27=-Shared_Lines_Offset!G12,H27&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="I41" t="b">
+        <f>AND(I27=-Shared_Lines_Offset!H12,I27&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="J41" t="b">
+        <f>AND(J27=-Shared_Lines_Offset!I12,J27&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="K41" t="b">
+        <f>AND(K27=-Shared_Lines_Offset!J12,K27&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="L41" t="b">
+        <f>AND(L27=-Shared_Lines_Offset!K12,L27&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="M41" t="b">
+        <f>AND(M27=-Shared_Lines_Offset!L12,M27&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="N41" t="b">
+        <f>AND(N27=-Shared_Lines_Offset!M12,N27&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="2:14">
+      <c r="B42" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C42" t="b">
+        <f>AND(C28=-Shared_Lines_Offset!B13,C28&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="D42" t="b">
+        <f>AND(D28=-Shared_Lines_Offset!C13,D28&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="E42" t="b">
+        <f>AND(E28=-Shared_Lines_Offset!D13,E28&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="F42" t="b">
+        <f>AND(F28=-Shared_Lines_Offset!E13,F28&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="G42" t="b">
+        <f>AND(G28=-Shared_Lines_Offset!F13,G28&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="H42" t="b">
+        <f>AND(H28=-Shared_Lines_Offset!G13,H28&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="I42" t="b">
+        <f>AND(I28=-Shared_Lines_Offset!H13,I28&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="J42" t="b">
+        <f>AND(J28=-Shared_Lines_Offset!I13,J28&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="K42" t="b">
+        <f>AND(K28=-Shared_Lines_Offset!J13,K28&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="L42" t="b">
+        <f>AND(L28=-Shared_Lines_Offset!K13,L28&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="M42" t="b">
+        <f>AND(M28=-Shared_Lines_Offset!L13,M28&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="N42" t="b">
+        <f>AND(N28=-Shared_Lines_Offset!M13,N28&lt;&gt;0)</f>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:N42"/>
+  <sheetViews>
+    <sheetView topLeftCell="A24" workbookViewId="0">
       <selection activeCell="M46" sqref="M46"/>
     </sheetView>
   </sheetViews>
@@ -8763,8 +10903,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T45"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="D45" sqref="D45"/>
+    <sheetView topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="B44" sqref="B44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -10294,7 +12434,7 @@
         <f>AND(F17=-Shared_Lines_Offset!E2,F17&lt;&gt;0)</f>
         <v>0</v>
       </c>
-      <c r="G31" t="b">
+      <c r="G31" s="3" t="b">
         <f>AND(G17=-Shared_Lines_Offset!F2,G17&lt;&gt;0)</f>
         <v>1</v>
       </c>
@@ -10931,10 +13071,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N42"/>
+  <dimension ref="A1:N44"/>
   <sheetViews>
-    <sheetView topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="B50" sqref="B50"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="B44" sqref="B44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -10986,37 +13126,37 @@
         <v>4</v>
       </c>
       <c r="D2" s="1">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="E2" s="1">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="F2" s="1">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="G2" s="1">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="H2" s="1">
         <v>9</v>
       </c>
       <c r="I2" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J2" s="1">
+        <v>9</v>
+      </c>
+      <c r="K2" s="1">
+        <v>8</v>
+      </c>
+      <c r="L2" s="1">
+        <v>7</v>
+      </c>
+      <c r="M2" s="1">
+        <v>9</v>
+      </c>
+      <c r="N2" s="1">
         <v>11</v>
-      </c>
-      <c r="K2" s="1">
-        <v>4</v>
-      </c>
-      <c r="L2" s="1">
-        <v>9</v>
-      </c>
-      <c r="M2" s="1">
-        <v>10</v>
-      </c>
-      <c r="N2" s="1">
-        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:14">
@@ -11032,47 +13172,47 @@
       </c>
       <c r="D3">
         <f t="shared" ref="D3:N14" si="0">$B3-D$2</f>
+        <v>-7</v>
+      </c>
+      <c r="E3">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+      <c r="F3">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+      <c r="G3">
+        <f t="shared" si="0"/>
+        <v>-2</v>
+      </c>
+      <c r="H3">
+        <f t="shared" si="0"/>
         <v>-5</v>
       </c>
-      <c r="E3">
-        <f t="shared" si="0"/>
-        <v>-6</v>
-      </c>
-      <c r="F3">
+      <c r="I3">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="J3">
         <f t="shared" si="0"/>
         <v>-5</v>
       </c>
-      <c r="G3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H3">
+      <c r="K3">
+        <f t="shared" si="0"/>
+        <v>-4</v>
+      </c>
+      <c r="L3">
+        <f t="shared" si="0"/>
+        <v>-3</v>
+      </c>
+      <c r="M3">
         <f t="shared" si="0"/>
         <v>-5</v>
       </c>
-      <c r="I3">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="J3">
+      <c r="N3">
         <f t="shared" si="0"/>
         <v>-7</v>
-      </c>
-      <c r="K3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="L3">
-        <f t="shared" si="0"/>
-        <v>-5</v>
-      </c>
-      <c r="M3">
-        <f t="shared" si="0"/>
-        <v>-6</v>
-      </c>
-      <c r="N3">
-        <f t="shared" si="0"/>
-        <v>-5</v>
       </c>
     </row>
     <row r="4" spans="1:14">
@@ -11080,31 +13220,31 @@
         <v>16</v>
       </c>
       <c r="B4" s="1">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C4">
         <f t="shared" ref="C4:C14" si="1">$B4-C$2</f>
+        <v>7</v>
+      </c>
+      <c r="D4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="F4">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="G4">
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="D4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E4">
-        <f t="shared" si="0"/>
-        <v>-1</v>
-      </c>
-      <c r="F4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G4">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
       <c r="H4">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I4">
         <f t="shared" si="0"/>
@@ -11112,19 +13252,19 @@
       </c>
       <c r="J4">
         <f t="shared" si="0"/>
-        <v>-2</v>
+        <v>2</v>
       </c>
       <c r="K4">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="L4">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="M4">
         <f t="shared" si="0"/>
-        <v>-1</v>
+        <v>2</v>
       </c>
       <c r="N4">
         <f t="shared" si="0"/>
@@ -11136,15 +13276,15 @@
         <v>95</v>
       </c>
       <c r="B5" s="1">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C5">
         <f t="shared" si="1"/>
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="D5">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>-6</v>
       </c>
       <c r="E5">
         <f t="shared" si="0"/>
@@ -11152,39 +13292,39 @@
       </c>
       <c r="F5">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G5">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>-1</v>
       </c>
       <c r="H5">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>-4</v>
       </c>
       <c r="I5">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="J5">
         <f t="shared" si="0"/>
-        <v>-1</v>
+        <v>-4</v>
       </c>
       <c r="K5">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>-3</v>
       </c>
       <c r="L5">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>-2</v>
       </c>
       <c r="M5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>-4</v>
       </c>
       <c r="N5">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>-6</v>
       </c>
     </row>
     <row r="6" spans="1:14">
@@ -11192,55 +13332,55 @@
         <v>96</v>
       </c>
       <c r="B6" s="1">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C6">
         <f t="shared" si="1"/>
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>-6</v>
       </c>
       <c r="E6">
         <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <f t="shared" si="0"/>
         <v>-1</v>
       </c>
-      <c r="F6">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G6">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
       <c r="H6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>-4</v>
       </c>
       <c r="I6">
         <f t="shared" si="0"/>
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="J6">
         <f t="shared" si="0"/>
+        <v>-4</v>
+      </c>
+      <c r="K6">
+        <f t="shared" si="0"/>
+        <v>-3</v>
+      </c>
+      <c r="L6">
+        <f t="shared" si="0"/>
         <v>-2</v>
       </c>
-      <c r="K6">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="L6">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
       <c r="M6">
         <f t="shared" si="0"/>
-        <v>-1</v>
+        <v>-4</v>
       </c>
       <c r="N6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>-6</v>
       </c>
     </row>
     <row r="7" spans="1:14">
@@ -11248,11 +13388,11 @@
         <v>97</v>
       </c>
       <c r="B7" s="1">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C7">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D7">
         <f t="shared" si="0"/>
@@ -11260,11 +13400,11 @@
       </c>
       <c r="E7">
         <f t="shared" si="0"/>
-        <v>-6</v>
+        <v>1</v>
       </c>
       <c r="F7">
         <f t="shared" si="0"/>
-        <v>-5</v>
+        <v>1</v>
       </c>
       <c r="G7">
         <f t="shared" si="0"/>
@@ -11272,7 +13412,7 @@
       </c>
       <c r="H7">
         <f t="shared" si="0"/>
-        <v>-5</v>
+        <v>-3</v>
       </c>
       <c r="I7">
         <f t="shared" si="0"/>
@@ -11280,19 +13420,19 @@
       </c>
       <c r="J7">
         <f t="shared" si="0"/>
-        <v>-7</v>
+        <v>-3</v>
       </c>
       <c r="K7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="L7">
         <f t="shared" si="0"/>
-        <v>-5</v>
+        <v>-1</v>
       </c>
       <c r="M7">
         <f t="shared" si="0"/>
-        <v>-6</v>
+        <v>-3</v>
       </c>
       <c r="N7">
         <f t="shared" si="0"/>
@@ -11312,19 +13452,19 @@
       </c>
       <c r="D8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="E8">
         <f t="shared" si="0"/>
-        <v>-1</v>
+        <v>4</v>
       </c>
       <c r="F8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="G8">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="H8">
         <f t="shared" si="0"/>
@@ -11332,27 +13472,27 @@
       </c>
       <c r="I8">
         <f t="shared" si="0"/>
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="J8">
         <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K8">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="L8">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="M8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N8">
+        <f t="shared" si="0"/>
         <v>-2</v>
-      </c>
-      <c r="K8">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="L8">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M8">
-        <f t="shared" si="0"/>
-        <v>-1</v>
-      </c>
-      <c r="N8">
-        <f t="shared" si="0"/>
-        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:14">
@@ -11360,31 +13500,31 @@
         <v>99</v>
       </c>
       <c r="B9" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C9">
         <f t="shared" si="1"/>
+        <v>-2</v>
+      </c>
+      <c r="D9">
+        <f t="shared" si="0"/>
+        <v>-9</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="0"/>
+        <v>-3</v>
+      </c>
+      <c r="F9">
+        <f t="shared" si="0"/>
+        <v>-3</v>
+      </c>
+      <c r="G9">
+        <f t="shared" si="0"/>
         <v>-4</v>
       </c>
-      <c r="D9">
-        <f t="shared" si="0"/>
-        <v>-9</v>
-      </c>
-      <c r="E9">
-        <f t="shared" si="0"/>
-        <v>-10</v>
-      </c>
-      <c r="F9">
-        <f t="shared" si="0"/>
-        <v>-9</v>
-      </c>
-      <c r="G9">
-        <f t="shared" si="0"/>
-        <v>-4</v>
-      </c>
       <c r="H9">
         <f t="shared" si="0"/>
-        <v>-9</v>
+        <v>-7</v>
       </c>
       <c r="I9">
         <f t="shared" si="0"/>
@@ -11392,19 +13532,19 @@
       </c>
       <c r="J9">
         <f t="shared" si="0"/>
-        <v>-11</v>
+        <v>-7</v>
       </c>
       <c r="K9">
         <f t="shared" si="0"/>
-        <v>-4</v>
+        <v>-6</v>
       </c>
       <c r="L9">
         <f t="shared" si="0"/>
-        <v>-9</v>
+        <v>-5</v>
       </c>
       <c r="M9">
         <f t="shared" si="0"/>
-        <v>-10</v>
+        <v>-7</v>
       </c>
       <c r="N9">
         <f t="shared" si="0"/>
@@ -11416,55 +13556,55 @@
         <v>100</v>
       </c>
       <c r="B10" s="1">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C10">
         <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="D10">
+        <f t="shared" si="0"/>
+        <v>-2</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="F10">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="G10">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="H10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I10">
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="D10">
+      <c r="J10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K10">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="L10">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="E10">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="F10">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="G10">
-        <f t="shared" si="0"/>
-        <v>7</v>
-      </c>
-      <c r="H10">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="I10">
-        <f t="shared" si="0"/>
-        <v>11</v>
-      </c>
-      <c r="J10">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="K10">
-        <f t="shared" si="0"/>
-        <v>7</v>
-      </c>
-      <c r="L10">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
       <c r="M10">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N10">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>-2</v>
       </c>
     </row>
     <row r="11" spans="1:14">
@@ -11472,39 +13612,39 @@
         <v>101</v>
       </c>
       <c r="B11" s="1">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C11">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D11">
         <f t="shared" si="0"/>
-        <v>-5</v>
+        <v>-3</v>
       </c>
       <c r="E11">
         <f t="shared" si="0"/>
-        <v>-6</v>
+        <v>3</v>
       </c>
       <c r="F11">
         <f t="shared" si="0"/>
-        <v>-5</v>
+        <v>3</v>
       </c>
       <c r="G11">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H11">
         <f t="shared" si="0"/>
-        <v>-5</v>
+        <v>-1</v>
       </c>
       <c r="I11">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="J11">
         <f t="shared" si="0"/>
-        <v>-7</v>
+        <v>-1</v>
       </c>
       <c r="K11">
         <f t="shared" si="0"/>
@@ -11512,15 +13652,15 @@
       </c>
       <c r="L11">
         <f t="shared" si="0"/>
-        <v>-5</v>
+        <v>1</v>
       </c>
       <c r="M11">
         <f t="shared" si="0"/>
-        <v>-6</v>
+        <v>-1</v>
       </c>
       <c r="N11">
         <f t="shared" si="0"/>
-        <v>-5</v>
+        <v>-3</v>
       </c>
     </row>
     <row r="12" spans="1:14">
@@ -11528,55 +13668,55 @@
         <v>102</v>
       </c>
       <c r="B12" s="1">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C12">
         <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="D12">
+        <f t="shared" si="0"/>
+        <v>-4</v>
+      </c>
+      <c r="E12">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="F12">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="G12">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="H12">
+        <f t="shared" si="0"/>
+        <v>-2</v>
+      </c>
+      <c r="I12">
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="D12">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E12">
+      <c r="J12">
+        <f t="shared" si="0"/>
+        <v>-2</v>
+      </c>
+      <c r="K12">
         <f t="shared" si="0"/>
         <v>-1</v>
       </c>
-      <c r="F12">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G12">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="H12">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I12">
-        <f t="shared" si="0"/>
-        <v>9</v>
-      </c>
-      <c r="J12">
+      <c r="L12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M12">
         <f t="shared" si="0"/>
         <v>-2</v>
       </c>
-      <c r="K12">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="L12">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M12">
-        <f t="shared" si="0"/>
-        <v>-1</v>
-      </c>
       <c r="N12">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>-4</v>
       </c>
     </row>
     <row r="13" spans="1:14">
@@ -11584,47 +13724,47 @@
         <v>103</v>
       </c>
       <c r="B13" s="1">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C13">
         <f t="shared" si="1"/>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D13">
         <f t="shared" si="0"/>
+        <v>-2</v>
+      </c>
+      <c r="E13">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="F13">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="G13">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="H13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I13">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="J13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K13">
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="E13">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F13">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="G13">
-        <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="H13">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="I13">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="J13">
-        <f t="shared" si="0"/>
-        <v>-1</v>
-      </c>
-      <c r="K13">
-        <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
       <c r="L13">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M13">
         <f t="shared" si="0"/>
@@ -11632,7 +13772,7 @@
       </c>
       <c r="N13">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>-2</v>
       </c>
     </row>
     <row r="14" spans="1:14">
@@ -11640,31 +13780,31 @@
         <v>17</v>
       </c>
       <c r="B14" s="1">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C14">
         <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="D14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E14">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="F14">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="G14">
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="D14">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E14">
-        <f t="shared" si="0"/>
-        <v>-1</v>
-      </c>
-      <c r="F14">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G14">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
       <c r="H14">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I14">
         <f t="shared" si="0"/>
@@ -11672,19 +13812,19 @@
       </c>
       <c r="J14">
         <f t="shared" si="0"/>
-        <v>-2</v>
+        <v>2</v>
       </c>
       <c r="K14">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="L14">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="M14">
         <f t="shared" si="0"/>
-        <v>-1</v>
+        <v>2</v>
       </c>
       <c r="N14">
         <f t="shared" si="0"/>
@@ -11754,7 +13894,7 @@
       </c>
       <c r="G17">
         <f>G3*Shared_Lines!F2</f>
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="H17">
         <f>H3*Shared_Lines!G2</f>
@@ -11770,7 +13910,7 @@
       </c>
       <c r="K17">
         <f>K3*Shared_Lines!J2</f>
-        <v>0</v>
+        <v>-4</v>
       </c>
       <c r="L17">
         <f>L3*Shared_Lines!K2</f>
@@ -11778,7 +13918,7 @@
       </c>
       <c r="M17">
         <f>M3*Shared_Lines!L2</f>
-        <v>-6</v>
+        <v>-5</v>
       </c>
       <c r="N17">
         <f>N3*Shared_Lines!M2</f>
@@ -11811,7 +13951,7 @@
       </c>
       <c r="H18">
         <f>H4*Shared_Lines!G3</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I18">
         <f>I4*Shared_Lines!H3</f>
@@ -11827,7 +13967,7 @@
       </c>
       <c r="L18">
         <f>L4*Shared_Lines!K3</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="M18">
         <f>M4*Shared_Lines!L3</f>
@@ -11884,7 +14024,7 @@
       </c>
       <c r="M19">
         <f>M5*Shared_Lines!L4</f>
-        <v>0</v>
+        <v>-4</v>
       </c>
       <c r="N19">
         <f>N5*Shared_Lines!M4</f>
@@ -11941,7 +14081,7 @@
       </c>
       <c r="N20">
         <f>N6*Shared_Lines!M5</f>
-        <v>0</v>
+        <v>-6</v>
       </c>
     </row>
     <row r="21" spans="2:14">
@@ -11982,7 +14122,7 @@
       </c>
       <c r="K21">
         <f>K7*Shared_Lines!J6</f>
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="L21">
         <f>L7*Shared_Lines!K6</f>
@@ -12039,7 +14179,7 @@
       </c>
       <c r="L22">
         <f>L8*Shared_Lines!K7</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="M22">
         <f>M8*Shared_Lines!L7</f>
@@ -12429,9 +14569,9 @@
         <f>AND(F17=-Shared_Lines_Offset!E2,F17&lt;&gt;0)</f>
         <v>0</v>
       </c>
-      <c r="G31" t="b">
+      <c r="G31" s="3" t="b">
         <f>AND(G17=-Shared_Lines_Offset!F2,G17&lt;&gt;0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H31" t="b">
         <f>AND(H17=-Shared_Lines_Offset!G2,H17&lt;&gt;0)</f>
@@ -12714,9 +14854,9 @@
         <f>AND(K22=-Shared_Lines_Offset!J7,K22&lt;&gt;0)</f>
         <v>0</v>
       </c>
-      <c r="L36" s="4" t="b">
+      <c r="L36" s="3" t="b">
         <f>AND(L22=-Shared_Lines_Offset!K7,L22&lt;&gt;0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M36" t="b">
         <f>AND(M22=-Shared_Lines_Offset!L7,M22&lt;&gt;0)</f>
@@ -13043,6 +15183,11 @@
       <c r="N42" t="b">
         <f>AND(N28=-Shared_Lines_Offset!M13,N28&lt;&gt;0)</f>
         <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="2:14">
+      <c r="B44" s="1" t="s">
+        <v>112</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed error in times to stations
</commit_message>
<xml_diff>
--- a/data/Times_to_Transfer_Stations.xlsx
+++ b/data/Times_to_Transfer_Stations.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25725"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="6380" yWindow="0" windowWidth="25600" windowHeight="15960" tabRatio="564" firstSheet="10" activeTab="11"/>
+    <workbookView xWindow="6380" yWindow="0" windowWidth="25600" windowHeight="15960" tabRatio="564" firstSheet="10" activeTab="12"/>
   </bookViews>
   <sheets>
     <sheet name="Station_Time_Calculations" sheetId="1" r:id="rId1"/>
@@ -16,8 +16,8 @@
     <sheet name="Shared_Lines_Offset" sheetId="7" r:id="rId7"/>
     <sheet name="shared_test_sat_morn_orig" sheetId="8" r:id="rId8"/>
     <sheet name="shared_test_sat_eve_orig" sheetId="11" r:id="rId9"/>
-    <sheet name="shared_test_sat_eve_abs1" sheetId="10" r:id="rId10"/>
-    <sheet name="shared_test_sat_morn_abs1" sheetId="9" r:id="rId11"/>
+    <sheet name="shared_test_sat_morn_abs1" sheetId="9" r:id="rId10"/>
+    <sheet name="shared_test_sat_eve_abs1" sheetId="10" r:id="rId11"/>
     <sheet name="shared_test_sat_morn_abs2" sheetId="12" r:id="rId12"/>
     <sheet name="shared_test_sat_eve_abs2" sheetId="13" r:id="rId13"/>
   </sheets>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1287" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1284" uniqueCount="113">
   <si>
     <t>-</t>
   </si>
@@ -436,8 +436,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="173">
+  <cellStyleXfs count="181">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -618,7 +626,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="173">
+  <cellStyles count="181">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -705,6 +713,10 @@
     <cellStyle name="Followed Hyperlink" xfId="168" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="170" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="172" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="174" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="176" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="178" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="180" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -791,6 +803,10 @@
     <cellStyle name="Hyperlink" xfId="167" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="169" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="171" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="173" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="175" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="177" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="179" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1745,7 +1761,7 @@
   <dimension ref="A1:N42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="P3" sqref="P3"/>
+      <selection activeCell="B50" sqref="B50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1794,40 +1810,40 @@
         <v>106</v>
       </c>
       <c r="C2" s="1">
+        <v>4</v>
+      </c>
+      <c r="D2" s="1">
+        <v>9</v>
+      </c>
+      <c r="E2" s="1">
+        <v>10</v>
+      </c>
+      <c r="F2" s="1">
+        <v>9</v>
+      </c>
+      <c r="G2" s="1">
+        <v>4</v>
+      </c>
+      <c r="H2" s="1">
+        <v>9</v>
+      </c>
+      <c r="I2" s="1">
+        <v>0</v>
+      </c>
+      <c r="J2" s="1">
         <v>11</v>
       </c>
-      <c r="D2" s="1">
-        <v>5</v>
-      </c>
-      <c r="E2" s="1">
-        <v>5</v>
-      </c>
-      <c r="F2" s="1">
+      <c r="K2" s="1">
         <v>4</v>
       </c>
-      <c r="G2" s="1">
-        <v>11</v>
-      </c>
-      <c r="H2" s="1">
-        <v>5</v>
-      </c>
-      <c r="I2" s="1">
-        <v>2</v>
-      </c>
-      <c r="J2" s="1">
-        <v>5</v>
-      </c>
-      <c r="K2" s="1">
-        <v>11</v>
-      </c>
       <c r="L2" s="1">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="M2" s="1">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="N2" s="1">
-        <v>5</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:14">
@@ -1835,7 +1851,7 @@
         <v>22</v>
       </c>
       <c r="B3" s="1">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="C3">
         <f>$B3-C$2</f>
@@ -1843,15 +1859,15 @@
       </c>
       <c r="D3">
         <f t="shared" ref="D3:N14" si="0">$B3-D$2</f>
-        <v>6</v>
+        <v>-5</v>
       </c>
       <c r="E3">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>-6</v>
       </c>
       <c r="F3">
         <f t="shared" si="0"/>
-        <v>7</v>
+        <v>-5</v>
       </c>
       <c r="G3">
         <f t="shared" si="0"/>
@@ -1859,15 +1875,15 @@
       </c>
       <c r="H3">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>-5</v>
       </c>
       <c r="I3">
         <f t="shared" si="0"/>
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="J3">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>-7</v>
       </c>
       <c r="K3">
         <f t="shared" si="0"/>
@@ -1875,15 +1891,15 @@
       </c>
       <c r="L3">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>-5</v>
       </c>
       <c r="M3">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>-6</v>
       </c>
       <c r="N3">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>-5</v>
       </c>
     </row>
     <row r="4" spans="1:14">
@@ -1891,11 +1907,11 @@
         <v>16</v>
       </c>
       <c r="B4" s="1">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="C4">
         <f t="shared" ref="C4:C14" si="1">$B4-C$2</f>
-        <v>-6</v>
+        <v>5</v>
       </c>
       <c r="D4">
         <f t="shared" si="0"/>
@@ -1903,15 +1919,15 @@
       </c>
       <c r="E4">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="F4">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G4">
         <f t="shared" si="0"/>
-        <v>-6</v>
+        <v>5</v>
       </c>
       <c r="H4">
         <f t="shared" si="0"/>
@@ -1919,15 +1935,15 @@
       </c>
       <c r="I4">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="J4">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="K4">
         <f t="shared" si="0"/>
-        <v>-6</v>
+        <v>5</v>
       </c>
       <c r="L4">
         <f t="shared" si="0"/>
@@ -1935,7 +1951,7 @@
       </c>
       <c r="M4">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="N4">
         <f t="shared" si="0"/>
@@ -1947,15 +1963,15 @@
         <v>95</v>
       </c>
       <c r="B5" s="1">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C5">
         <f t="shared" si="1"/>
-        <v>-6</v>
+        <v>6</v>
       </c>
       <c r="D5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E5">
         <f t="shared" si="0"/>
@@ -1967,27 +1983,27 @@
       </c>
       <c r="G5">
         <f t="shared" si="0"/>
-        <v>-6</v>
+        <v>6</v>
       </c>
       <c r="H5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I5">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="J5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="K5">
         <f t="shared" si="0"/>
-        <v>-6</v>
+        <v>6</v>
       </c>
       <c r="L5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M5">
         <f t="shared" si="0"/>
@@ -1995,7 +2011,7 @@
       </c>
       <c r="N5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:14">
@@ -2003,55 +2019,55 @@
         <v>96</v>
       </c>
       <c r="B6" s="1">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="C6">
         <f t="shared" si="1"/>
-        <v>-7</v>
+        <v>5</v>
       </c>
       <c r="D6">
         <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="0"/>
         <v>-1</v>
       </c>
-      <c r="E6">
+      <c r="F6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="H6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I6">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="J6">
+        <f t="shared" si="0"/>
+        <v>-2</v>
+      </c>
+      <c r="K6">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="L6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M6">
         <f t="shared" si="0"/>
         <v>-1</v>
       </c>
-      <c r="F6">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G6">
-        <f t="shared" si="0"/>
-        <v>-7</v>
-      </c>
-      <c r="H6">
-        <f t="shared" si="0"/>
-        <v>-1</v>
-      </c>
-      <c r="I6">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="J6">
-        <f t="shared" si="0"/>
-        <v>-1</v>
-      </c>
-      <c r="K6">
-        <f t="shared" si="0"/>
-        <v>-7</v>
-      </c>
-      <c r="L6">
-        <f t="shared" si="0"/>
-        <v>-1</v>
-      </c>
-      <c r="M6">
-        <f t="shared" si="0"/>
-        <v>-1</v>
-      </c>
       <c r="N6">
         <f t="shared" si="0"/>
-        <v>-1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:14">
@@ -2059,7 +2075,7 @@
         <v>97</v>
       </c>
       <c r="B7" s="1">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="C7">
         <f t="shared" si="1"/>
@@ -2067,15 +2083,15 @@
       </c>
       <c r="D7">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>-5</v>
       </c>
       <c r="E7">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>-6</v>
       </c>
       <c r="F7">
         <f t="shared" si="0"/>
-        <v>7</v>
+        <v>-5</v>
       </c>
       <c r="G7">
         <f t="shared" si="0"/>
@@ -2083,15 +2099,15 @@
       </c>
       <c r="H7">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>-5</v>
       </c>
       <c r="I7">
         <f t="shared" si="0"/>
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="J7">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>-7</v>
       </c>
       <c r="K7">
         <f t="shared" si="0"/>
@@ -2099,15 +2115,15 @@
       </c>
       <c r="L7">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>-5</v>
       </c>
       <c r="M7">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>-6</v>
       </c>
       <c r="N7">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>-5</v>
       </c>
     </row>
     <row r="8" spans="1:14">
@@ -2115,11 +2131,11 @@
         <v>98</v>
       </c>
       <c r="B8" s="1">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="C8">
         <f t="shared" si="1"/>
-        <v>-6</v>
+        <v>5</v>
       </c>
       <c r="D8">
         <f t="shared" si="0"/>
@@ -2127,15 +2143,15 @@
       </c>
       <c r="E8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="F8">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G8">
         <f t="shared" si="0"/>
-        <v>-6</v>
+        <v>5</v>
       </c>
       <c r="H8">
         <f t="shared" si="0"/>
@@ -2143,15 +2159,15 @@
       </c>
       <c r="I8">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="J8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="K8">
         <f t="shared" si="0"/>
-        <v>-6</v>
+        <v>5</v>
       </c>
       <c r="L8">
         <f t="shared" si="0"/>
@@ -2159,7 +2175,7 @@
       </c>
       <c r="M8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="N8">
         <f t="shared" si="0"/>
@@ -2171,55 +2187,55 @@
         <v>99</v>
       </c>
       <c r="B9" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C9">
         <f t="shared" si="1"/>
+        <v>-4</v>
+      </c>
+      <c r="D9">
+        <f t="shared" si="0"/>
         <v>-9</v>
       </c>
-      <c r="D9">
-        <f t="shared" si="0"/>
-        <v>-3</v>
-      </c>
       <c r="E9">
         <f t="shared" si="0"/>
-        <v>-3</v>
+        <v>-10</v>
       </c>
       <c r="F9">
         <f t="shared" si="0"/>
-        <v>-2</v>
+        <v>-9</v>
       </c>
       <c r="G9">
         <f t="shared" si="0"/>
+        <v>-4</v>
+      </c>
+      <c r="H9">
+        <f t="shared" si="0"/>
         <v>-9</v>
       </c>
-      <c r="H9">
-        <f t="shared" si="0"/>
-        <v>-3</v>
-      </c>
       <c r="I9">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="J9">
         <f t="shared" si="0"/>
-        <v>-3</v>
+        <v>-11</v>
       </c>
       <c r="K9">
         <f t="shared" si="0"/>
+        <v>-4</v>
+      </c>
+      <c r="L9">
+        <f t="shared" si="0"/>
         <v>-9</v>
       </c>
-      <c r="L9">
-        <f t="shared" si="0"/>
-        <v>-3</v>
-      </c>
       <c r="M9">
         <f t="shared" si="0"/>
-        <v>-3</v>
+        <v>-10</v>
       </c>
       <c r="N9">
         <f t="shared" si="0"/>
-        <v>-3</v>
+        <v>-9</v>
       </c>
     </row>
     <row r="10" spans="1:14">
@@ -2227,55 +2243,55 @@
         <v>100</v>
       </c>
       <c r="B10" s="1">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="C10">
         <f t="shared" si="1"/>
-        <v>-6</v>
+        <v>7</v>
       </c>
       <c r="D10">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E10">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F10">
         <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="G10">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="H10">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="I10">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="J10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K10">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="L10">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="M10">
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="G10">
-        <f t="shared" si="0"/>
-        <v>-6</v>
-      </c>
-      <c r="H10">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I10">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="J10">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="K10">
-        <f t="shared" si="0"/>
-        <v>-6</v>
-      </c>
-      <c r="L10">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M10">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
       <c r="N10">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="11" spans="1:14">
@@ -2283,7 +2299,7 @@
         <v>101</v>
       </c>
       <c r="B11" s="1">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="C11">
         <f t="shared" si="1"/>
@@ -2291,15 +2307,15 @@
       </c>
       <c r="D11">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>-5</v>
       </c>
       <c r="E11">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>-6</v>
       </c>
       <c r="F11">
         <f t="shared" si="0"/>
-        <v>7</v>
+        <v>-5</v>
       </c>
       <c r="G11">
         <f t="shared" si="0"/>
@@ -2307,15 +2323,15 @@
       </c>
       <c r="H11">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>-5</v>
       </c>
       <c r="I11">
         <f t="shared" si="0"/>
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="J11">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>-7</v>
       </c>
       <c r="K11">
         <f t="shared" si="0"/>
@@ -2323,15 +2339,15 @@
       </c>
       <c r="L11">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>-5</v>
       </c>
       <c r="M11">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>-6</v>
       </c>
       <c r="N11">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>-5</v>
       </c>
     </row>
     <row r="12" spans="1:14">
@@ -2339,11 +2355,11 @@
         <v>102</v>
       </c>
       <c r="B12" s="1">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="C12">
         <f t="shared" si="1"/>
-        <v>-6</v>
+        <v>5</v>
       </c>
       <c r="D12">
         <f t="shared" si="0"/>
@@ -2351,15 +2367,15 @@
       </c>
       <c r="E12">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="F12">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G12">
         <f t="shared" si="0"/>
-        <v>-6</v>
+        <v>5</v>
       </c>
       <c r="H12">
         <f t="shared" si="0"/>
@@ -2367,15 +2383,15 @@
       </c>
       <c r="I12">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="J12">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="K12">
         <f t="shared" si="0"/>
-        <v>-6</v>
+        <v>5</v>
       </c>
       <c r="L12">
         <f t="shared" si="0"/>
@@ -2383,7 +2399,7 @@
       </c>
       <c r="M12">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="N12">
         <f t="shared" si="0"/>
@@ -2395,15 +2411,15 @@
         <v>103</v>
       </c>
       <c r="B13" s="1">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C13">
         <f t="shared" si="1"/>
-        <v>-6</v>
+        <v>6</v>
       </c>
       <c r="D13">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E13">
         <f t="shared" si="0"/>
@@ -2415,27 +2431,27 @@
       </c>
       <c r="G13">
         <f t="shared" si="0"/>
-        <v>-6</v>
+        <v>6</v>
       </c>
       <c r="H13">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I13">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="J13">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="K13">
         <f t="shared" si="0"/>
-        <v>-6</v>
+        <v>6</v>
       </c>
       <c r="L13">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M13">
         <f t="shared" si="0"/>
@@ -2443,7 +2459,7 @@
       </c>
       <c r="N13">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:14">
@@ -2451,11 +2467,11 @@
         <v>17</v>
       </c>
       <c r="B14" s="1">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="C14">
         <f t="shared" si="1"/>
-        <v>-6</v>
+        <v>5</v>
       </c>
       <c r="D14">
         <f t="shared" si="0"/>
@@ -2463,15 +2479,15 @@
       </c>
       <c r="E14">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="F14">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G14">
         <f t="shared" si="0"/>
-        <v>-6</v>
+        <v>5</v>
       </c>
       <c r="H14">
         <f t="shared" si="0"/>
@@ -2479,15 +2495,15 @@
       </c>
       <c r="I14">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="J14">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="K14">
         <f t="shared" si="0"/>
-        <v>-6</v>
+        <v>5</v>
       </c>
       <c r="L14">
         <f t="shared" si="0"/>
@@ -2495,7 +2511,7 @@
       </c>
       <c r="M14">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="N14">
         <f t="shared" si="0"/>
@@ -2589,7 +2605,7 @@
       </c>
       <c r="M17">
         <f>M3*Shared_Lines!L2</f>
-        <v>6</v>
+        <v>-6</v>
       </c>
       <c r="N17">
         <f>N3*Shared_Lines!M2</f>
@@ -2752,7 +2768,7 @@
       </c>
       <c r="N20">
         <f>N6*Shared_Lines!M5</f>
-        <v>-1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21" spans="2:14">
@@ -3872,7 +3888,7 @@
   <dimension ref="A1:N42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B50" sqref="B50"/>
+      <selection activeCell="J45" sqref="J45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3921,40 +3937,40 @@
         <v>106</v>
       </c>
       <c r="C2" s="1">
+        <v>11</v>
+      </c>
+      <c r="D2" s="1">
+        <v>5</v>
+      </c>
+      <c r="E2" s="1">
+        <v>5</v>
+      </c>
+      <c r="F2" s="1">
         <v>4</v>
       </c>
-      <c r="D2" s="1">
-        <v>9</v>
-      </c>
-      <c r="E2" s="1">
-        <v>10</v>
-      </c>
-      <c r="F2" s="1">
-        <v>9</v>
-      </c>
       <c r="G2" s="1">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="H2" s="1">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="I2" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J2" s="1">
+        <v>5</v>
+      </c>
+      <c r="K2" s="1">
         <v>11</v>
       </c>
-      <c r="K2" s="1">
-        <v>4</v>
-      </c>
       <c r="L2" s="1">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="M2" s="1">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="N2" s="1">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:14">
@@ -3962,7 +3978,7 @@
         <v>22</v>
       </c>
       <c r="B3" s="1">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="C3">
         <f>$B3-C$2</f>
@@ -3970,15 +3986,15 @@
       </c>
       <c r="D3">
         <f t="shared" ref="D3:N14" si="0">$B3-D$2</f>
-        <v>-5</v>
+        <v>6</v>
       </c>
       <c r="E3">
         <f t="shared" si="0"/>
-        <v>-6</v>
+        <v>6</v>
       </c>
       <c r="F3">
         <f t="shared" si="0"/>
-        <v>-5</v>
+        <v>7</v>
       </c>
       <c r="G3">
         <f t="shared" si="0"/>
@@ -3986,15 +4002,15 @@
       </c>
       <c r="H3">
         <f t="shared" si="0"/>
-        <v>-5</v>
+        <v>6</v>
       </c>
       <c r="I3">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="J3">
         <f t="shared" si="0"/>
-        <v>-7</v>
+        <v>6</v>
       </c>
       <c r="K3">
         <f t="shared" si="0"/>
@@ -4002,15 +4018,15 @@
       </c>
       <c r="L3">
         <f t="shared" si="0"/>
-        <v>-5</v>
+        <v>6</v>
       </c>
       <c r="M3">
         <f t="shared" si="0"/>
-        <v>-6</v>
+        <v>6</v>
       </c>
       <c r="N3">
         <f t="shared" si="0"/>
-        <v>-5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:14">
@@ -4018,11 +4034,11 @@
         <v>16</v>
       </c>
       <c r="B4" s="1">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C4">
         <f t="shared" ref="C4:C14" si="1">$B4-C$2</f>
-        <v>5</v>
+        <v>-6</v>
       </c>
       <c r="D4">
         <f t="shared" si="0"/>
@@ -4030,15 +4046,15 @@
       </c>
       <c r="E4">
         <f t="shared" si="0"/>
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="F4">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G4">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>-6</v>
       </c>
       <c r="H4">
         <f t="shared" si="0"/>
@@ -4046,15 +4062,15 @@
       </c>
       <c r="I4">
         <f t="shared" si="0"/>
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="J4">
         <f t="shared" si="0"/>
-        <v>-2</v>
+        <v>0</v>
       </c>
       <c r="K4">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>-6</v>
       </c>
       <c r="L4">
         <f t="shared" si="0"/>
@@ -4062,7 +4078,7 @@
       </c>
       <c r="M4">
         <f t="shared" si="0"/>
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="N4">
         <f t="shared" si="0"/>
@@ -4074,47 +4090,47 @@
         <v>95</v>
       </c>
       <c r="B5" s="1">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C5">
         <f t="shared" si="1"/>
-        <v>6</v>
+        <v>-6</v>
       </c>
       <c r="D5">
         <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="E5">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F5">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
       <c r="G5">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>-6</v>
       </c>
       <c r="H5">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I5">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="J5">
         <f t="shared" si="0"/>
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="K5">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>-6</v>
       </c>
       <c r="L5">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M5">
         <f t="shared" si="0"/>
@@ -4122,7 +4138,7 @@
       </c>
       <c r="N5">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:14">
@@ -4130,15 +4146,15 @@
         <v>96</v>
       </c>
       <c r="B6" s="1">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="C6">
         <f t="shared" si="1"/>
-        <v>5</v>
+        <v>-7</v>
       </c>
       <c r="D6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="E6">
         <f t="shared" si="0"/>
@@ -4150,27 +4166,27 @@
       </c>
       <c r="G6">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>-7</v>
       </c>
       <c r="H6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="I6">
         <f t="shared" si="0"/>
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="J6">
         <f t="shared" si="0"/>
-        <v>-2</v>
+        <v>-1</v>
       </c>
       <c r="K6">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>-7</v>
       </c>
       <c r="L6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="M6">
         <f t="shared" si="0"/>
@@ -4178,7 +4194,7 @@
       </c>
       <c r="N6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="7" spans="1:14">
@@ -4186,7 +4202,7 @@
         <v>97</v>
       </c>
       <c r="B7" s="1">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="C7">
         <f t="shared" si="1"/>
@@ -4194,15 +4210,15 @@
       </c>
       <c r="D7">
         <f t="shared" si="0"/>
-        <v>-5</v>
+        <v>6</v>
       </c>
       <c r="E7">
         <f t="shared" si="0"/>
-        <v>-6</v>
+        <v>6</v>
       </c>
       <c r="F7">
         <f t="shared" si="0"/>
-        <v>-5</v>
+        <v>7</v>
       </c>
       <c r="G7">
         <f t="shared" si="0"/>
@@ -4210,15 +4226,15 @@
       </c>
       <c r="H7">
         <f t="shared" si="0"/>
-        <v>-5</v>
+        <v>6</v>
       </c>
       <c r="I7">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="J7">
         <f t="shared" si="0"/>
-        <v>-7</v>
+        <v>6</v>
       </c>
       <c r="K7">
         <f t="shared" si="0"/>
@@ -4226,15 +4242,15 @@
       </c>
       <c r="L7">
         <f t="shared" si="0"/>
-        <v>-5</v>
+        <v>6</v>
       </c>
       <c r="M7">
         <f t="shared" si="0"/>
-        <v>-6</v>
+        <v>6</v>
       </c>
       <c r="N7">
         <f t="shared" si="0"/>
-        <v>-5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:14">
@@ -4242,11 +4258,11 @@
         <v>98</v>
       </c>
       <c r="B8" s="1">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C8">
         <f t="shared" si="1"/>
-        <v>5</v>
+        <v>-6</v>
       </c>
       <c r="D8">
         <f t="shared" si="0"/>
@@ -4254,15 +4270,15 @@
       </c>
       <c r="E8">
         <f t="shared" si="0"/>
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="F8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G8">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>-6</v>
       </c>
       <c r="H8">
         <f t="shared" si="0"/>
@@ -4270,15 +4286,15 @@
       </c>
       <c r="I8">
         <f t="shared" si="0"/>
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="J8">
         <f t="shared" si="0"/>
-        <v>-2</v>
+        <v>0</v>
       </c>
       <c r="K8">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>-6</v>
       </c>
       <c r="L8">
         <f t="shared" si="0"/>
@@ -4286,7 +4302,7 @@
       </c>
       <c r="M8">
         <f t="shared" si="0"/>
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="N8">
         <f t="shared" si="0"/>
@@ -4298,55 +4314,55 @@
         <v>99</v>
       </c>
       <c r="B9" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C9">
         <f t="shared" si="1"/>
-        <v>-4</v>
+        <v>-9</v>
       </c>
       <c r="D9">
         <f t="shared" si="0"/>
+        <v>-3</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="0"/>
+        <v>-3</v>
+      </c>
+      <c r="F9">
+        <f t="shared" si="0"/>
+        <v>-2</v>
+      </c>
+      <c r="G9">
+        <f t="shared" si="0"/>
         <v>-9</v>
       </c>
-      <c r="E9">
-        <f t="shared" si="0"/>
-        <v>-10</v>
-      </c>
-      <c r="F9">
+      <c r="H9">
+        <f t="shared" si="0"/>
+        <v>-3</v>
+      </c>
+      <c r="I9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J9">
+        <f t="shared" si="0"/>
+        <v>-3</v>
+      </c>
+      <c r="K9">
         <f t="shared" si="0"/>
         <v>-9</v>
       </c>
-      <c r="G9">
-        <f t="shared" si="0"/>
-        <v>-4</v>
-      </c>
-      <c r="H9">
-        <f t="shared" si="0"/>
-        <v>-9</v>
-      </c>
-      <c r="I9">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="J9">
-        <f t="shared" si="0"/>
-        <v>-11</v>
-      </c>
-      <c r="K9">
-        <f t="shared" si="0"/>
-        <v>-4</v>
-      </c>
       <c r="L9">
         <f t="shared" si="0"/>
-        <v>-9</v>
+        <v>-3</v>
       </c>
       <c r="M9">
         <f t="shared" si="0"/>
-        <v>-10</v>
+        <v>-3</v>
       </c>
       <c r="N9">
         <f t="shared" si="0"/>
-        <v>-9</v>
+        <v>-3</v>
       </c>
     </row>
     <row r="10" spans="1:14">
@@ -4354,35 +4370,35 @@
         <v>100</v>
       </c>
       <c r="B10" s="1">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="C10">
         <f t="shared" si="1"/>
-        <v>7</v>
+        <v>-6</v>
       </c>
       <c r="D10">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E10">
         <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="F10">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
       <c r="G10">
         <f t="shared" si="0"/>
-        <v>7</v>
+        <v>-6</v>
       </c>
       <c r="H10">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I10">
         <f t="shared" si="0"/>
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="J10">
         <f t="shared" si="0"/>
@@ -4390,19 +4406,19 @@
       </c>
       <c r="K10">
         <f t="shared" si="0"/>
-        <v>7</v>
+        <v>-6</v>
       </c>
       <c r="L10">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M10">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N10">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:14">
@@ -4410,7 +4426,7 @@
         <v>101</v>
       </c>
       <c r="B11" s="1">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="C11">
         <f t="shared" si="1"/>
@@ -4418,15 +4434,15 @@
       </c>
       <c r="D11">
         <f t="shared" si="0"/>
-        <v>-5</v>
+        <v>6</v>
       </c>
       <c r="E11">
         <f t="shared" si="0"/>
-        <v>-6</v>
+        <v>6</v>
       </c>
       <c r="F11">
         <f t="shared" si="0"/>
-        <v>-5</v>
+        <v>7</v>
       </c>
       <c r="G11">
         <f t="shared" si="0"/>
@@ -4434,15 +4450,15 @@
       </c>
       <c r="H11">
         <f t="shared" si="0"/>
-        <v>-5</v>
+        <v>6</v>
       </c>
       <c r="I11">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="J11">
         <f t="shared" si="0"/>
-        <v>-7</v>
+        <v>6</v>
       </c>
       <c r="K11">
         <f t="shared" si="0"/>
@@ -4450,15 +4466,15 @@
       </c>
       <c r="L11">
         <f t="shared" si="0"/>
-        <v>-5</v>
+        <v>6</v>
       </c>
       <c r="M11">
         <f t="shared" si="0"/>
-        <v>-6</v>
+        <v>6</v>
       </c>
       <c r="N11">
         <f t="shared" si="0"/>
-        <v>-5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="12" spans="1:14">
@@ -4466,11 +4482,11 @@
         <v>102</v>
       </c>
       <c r="B12" s="1">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C12">
         <f t="shared" si="1"/>
-        <v>5</v>
+        <v>-6</v>
       </c>
       <c r="D12">
         <f t="shared" si="0"/>
@@ -4478,15 +4494,15 @@
       </c>
       <c r="E12">
         <f t="shared" si="0"/>
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="F12">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G12">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>-6</v>
       </c>
       <c r="H12">
         <f t="shared" si="0"/>
@@ -4494,15 +4510,15 @@
       </c>
       <c r="I12">
         <f t="shared" si="0"/>
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="J12">
         <f t="shared" si="0"/>
-        <v>-2</v>
+        <v>0</v>
       </c>
       <c r="K12">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>-6</v>
       </c>
       <c r="L12">
         <f t="shared" si="0"/>
@@ -4510,7 +4526,7 @@
       </c>
       <c r="M12">
         <f t="shared" si="0"/>
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="N12">
         <f t="shared" si="0"/>
@@ -4522,47 +4538,47 @@
         <v>103</v>
       </c>
       <c r="B13" s="1">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C13">
         <f t="shared" si="1"/>
-        <v>6</v>
+        <v>-6</v>
       </c>
       <c r="D13">
         <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F13">
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="E13">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F13">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
       <c r="G13">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>-6</v>
       </c>
       <c r="H13">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I13">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="J13">
         <f t="shared" si="0"/>
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="K13">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>-6</v>
       </c>
       <c r="L13">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M13">
         <f t="shared" si="0"/>
@@ -4570,7 +4586,7 @@
       </c>
       <c r="N13">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:14">
@@ -4578,11 +4594,11 @@
         <v>17</v>
       </c>
       <c r="B14" s="1">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C14">
         <f t="shared" si="1"/>
-        <v>5</v>
+        <v>-6</v>
       </c>
       <c r="D14">
         <f t="shared" si="0"/>
@@ -4590,15 +4606,15 @@
       </c>
       <c r="E14">
         <f t="shared" si="0"/>
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="F14">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G14">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>-6</v>
       </c>
       <c r="H14">
         <f t="shared" si="0"/>
@@ -4606,15 +4622,15 @@
       </c>
       <c r="I14">
         <f t="shared" si="0"/>
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="J14">
         <f t="shared" si="0"/>
-        <v>-2</v>
+        <v>0</v>
       </c>
       <c r="K14">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>-6</v>
       </c>
       <c r="L14">
         <f t="shared" si="0"/>
@@ -4622,7 +4638,7 @@
       </c>
       <c r="M14">
         <f t="shared" si="0"/>
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="N14">
         <f t="shared" si="0"/>
@@ -4716,7 +4732,7 @@
       </c>
       <c r="M17">
         <f>M3*Shared_Lines!L2</f>
-        <v>-6</v>
+        <v>6</v>
       </c>
       <c r="N17">
         <f>N3*Shared_Lines!M2</f>
@@ -4879,7 +4895,7 @@
       </c>
       <c r="N20">
         <f>N6*Shared_Lines!M5</f>
-        <v>0</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="21" spans="2:14">
@@ -5998,7 +6014,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="P34" sqref="P34"/>
     </sheetView>
   </sheetViews>
@@ -8125,8 +8141,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N42"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="J45" sqref="J45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -8175,16 +8191,16 @@
         <v>106</v>
       </c>
       <c r="C2" s="1">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="D2" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E2" s="1">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="F2" s="1">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="G2" s="1">
         <v>8</v>
@@ -8196,19 +8212,19 @@
         <v>5</v>
       </c>
       <c r="J2" s="1">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="K2" s="1">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="L2" s="1">
         <v>10</v>
       </c>
       <c r="M2" s="1">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="N2" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:14">
@@ -8216,7 +8232,7 @@
         <v>22</v>
       </c>
       <c r="B3" s="1">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C3">
         <f>$B3-C$2</f>
@@ -8224,47 +8240,47 @@
       </c>
       <c r="D3">
         <f t="shared" ref="D3:N14" si="0">$B3-D$2</f>
+        <v>9</v>
+      </c>
+      <c r="E3">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="F3">
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="E3">
+      <c r="G3">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="H3">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="I3">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="J3">
         <f t="shared" si="0"/>
         <v>-1</v>
       </c>
-      <c r="F3">
-        <f t="shared" si="0"/>
-        <v>-1</v>
-      </c>
-      <c r="G3">
-        <f t="shared" si="0"/>
-        <v>-1</v>
-      </c>
-      <c r="H3">
-        <f t="shared" si="0"/>
-        <v>7</v>
-      </c>
-      <c r="I3">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="J3">
-        <f t="shared" si="0"/>
-        <v>7</v>
-      </c>
       <c r="K3">
         <f t="shared" si="0"/>
-        <v>-4</v>
+        <v>0</v>
       </c>
       <c r="L3">
         <f t="shared" si="0"/>
-        <v>-3</v>
+        <v>0</v>
       </c>
       <c r="M3">
         <f t="shared" si="0"/>
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="N3">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:14">
@@ -8272,11 +8288,11 @@
         <v>16</v>
       </c>
       <c r="B4" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C4">
         <f t="shared" ref="C4:C14" si="1">$B4-C$2</f>
-        <v>-5</v>
+        <v>-9</v>
       </c>
       <c r="D4">
         <f t="shared" si="0"/>
@@ -8284,43 +8300,43 @@
       </c>
       <c r="E4">
         <f t="shared" si="0"/>
-        <v>-6</v>
+        <v>0</v>
       </c>
       <c r="F4">
         <f t="shared" si="0"/>
-        <v>-6</v>
+        <v>-4</v>
       </c>
       <c r="G4">
         <f t="shared" si="0"/>
-        <v>-6</v>
+        <v>-7</v>
       </c>
       <c r="H4">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I4">
         <f t="shared" si="0"/>
+        <v>-4</v>
+      </c>
+      <c r="J4">
+        <f t="shared" si="0"/>
+        <v>-10</v>
+      </c>
+      <c r="K4">
+        <f t="shared" si="0"/>
+        <v>-9</v>
+      </c>
+      <c r="L4">
+        <f t="shared" si="0"/>
+        <v>-9</v>
+      </c>
+      <c r="M4">
+        <f t="shared" si="0"/>
+        <v>-9</v>
+      </c>
+      <c r="N4">
+        <f t="shared" si="0"/>
         <v>-3</v>
-      </c>
-      <c r="J4">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="K4">
-        <f t="shared" si="0"/>
-        <v>-9</v>
-      </c>
-      <c r="L4">
-        <f t="shared" si="0"/>
-        <v>-8</v>
-      </c>
-      <c r="M4">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="N4">
-        <f t="shared" si="0"/>
-        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:14">
@@ -8328,55 +8344,55 @@
         <v>95</v>
       </c>
       <c r="B5" s="1">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="C5">
         <f t="shared" si="1"/>
+        <v>-9</v>
+      </c>
+      <c r="D5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <f t="shared" si="0"/>
+        <v>-4</v>
+      </c>
+      <c r="G5">
+        <f t="shared" si="0"/>
+        <v>-7</v>
+      </c>
+      <c r="H5">
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="D5">
-        <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="E5">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F5">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G5">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H5">
-        <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
       <c r="I5">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>-4</v>
       </c>
       <c r="J5">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>-10</v>
       </c>
       <c r="K5">
         <f t="shared" si="0"/>
+        <v>-9</v>
+      </c>
+      <c r="L5">
+        <f t="shared" si="0"/>
+        <v>-9</v>
+      </c>
+      <c r="M5">
+        <f t="shared" si="0"/>
+        <v>-9</v>
+      </c>
+      <c r="N5">
+        <f t="shared" si="0"/>
         <v>-3</v>
-      </c>
-      <c r="L5">
-        <f t="shared" si="0"/>
-        <v>-2</v>
-      </c>
-      <c r="M5">
-        <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="N5">
-        <f t="shared" si="0"/>
-        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:14">
@@ -8384,55 +8400,55 @@
         <v>96</v>
       </c>
       <c r="B6" s="1">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C6">
         <f t="shared" si="1"/>
+        <v>-5</v>
+      </c>
+      <c r="D6">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="F6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <f t="shared" si="0"/>
+        <v>-3</v>
+      </c>
+      <c r="H6">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="I6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J6">
+        <f t="shared" si="0"/>
+        <v>-6</v>
+      </c>
+      <c r="K6">
+        <f t="shared" si="0"/>
+        <v>-5</v>
+      </c>
+      <c r="L6">
+        <f t="shared" si="0"/>
+        <v>-5</v>
+      </c>
+      <c r="M6">
+        <f t="shared" si="0"/>
+        <v>-5</v>
+      </c>
+      <c r="N6">
+        <f t="shared" si="0"/>
         <v>1</v>
-      </c>
-      <c r="D6">
-        <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="E6">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F6">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G6">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H6">
-        <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="I6">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="J6">
-        <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="K6">
-        <f t="shared" si="0"/>
-        <v>-3</v>
-      </c>
-      <c r="L6">
-        <f t="shared" si="0"/>
-        <v>-2</v>
-      </c>
-      <c r="M6">
-        <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="N6">
-        <f t="shared" si="0"/>
-        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:14">
@@ -8444,19 +8460,19 @@
       </c>
       <c r="C7">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>-2</v>
       </c>
       <c r="D7">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="F7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G7">
         <f t="shared" si="0"/>
@@ -8472,11 +8488,11 @@
       </c>
       <c r="J7">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>-3</v>
       </c>
       <c r="K7">
         <f t="shared" si="0"/>
-        <v>-3</v>
+        <v>-2</v>
       </c>
       <c r="L7">
         <f t="shared" si="0"/>
@@ -8484,11 +8500,11 @@
       </c>
       <c r="M7">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>-2</v>
       </c>
       <c r="N7">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:14">
@@ -8500,24 +8516,24 @@
       </c>
       <c r="C8">
         <f t="shared" si="1"/>
-        <v>-7</v>
+        <v>-10</v>
       </c>
       <c r="D8">
         <f t="shared" si="0"/>
-        <v>-2</v>
+        <v>-1</v>
       </c>
       <c r="E8">
         <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+      <c r="F8">
+        <f t="shared" si="0"/>
+        <v>-5</v>
+      </c>
+      <c r="G8">
+        <f t="shared" si="0"/>
         <v>-8</v>
       </c>
-      <c r="F8">
-        <f t="shared" si="0"/>
-        <v>-8</v>
-      </c>
-      <c r="G8">
-        <f t="shared" si="0"/>
-        <v>-8</v>
-      </c>
       <c r="H8">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -8528,11 +8544,11 @@
       </c>
       <c r="J8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>-11</v>
       </c>
       <c r="K8">
         <f t="shared" si="0"/>
-        <v>-11</v>
+        <v>-10</v>
       </c>
       <c r="L8">
         <f t="shared" si="0"/>
@@ -8540,11 +8556,11 @@
       </c>
       <c r="M8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>-10</v>
       </c>
       <c r="N8">
         <f t="shared" si="0"/>
-        <v>-2</v>
+        <v>-4</v>
       </c>
     </row>
     <row r="9" spans="1:14">
@@ -8556,24 +8572,24 @@
       </c>
       <c r="C9">
         <f t="shared" si="1"/>
-        <v>-2</v>
+        <v>-5</v>
       </c>
       <c r="D9">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E9">
         <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="F9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G9">
+        <f t="shared" si="0"/>
         <v>-3</v>
       </c>
-      <c r="F9">
-        <f t="shared" si="0"/>
-        <v>-3</v>
-      </c>
-      <c r="G9">
-        <f t="shared" si="0"/>
-        <v>-3</v>
-      </c>
       <c r="H9">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -8584,11 +8600,11 @@
       </c>
       <c r="J9">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>-6</v>
       </c>
       <c r="K9">
         <f t="shared" si="0"/>
-        <v>-6</v>
+        <v>-5</v>
       </c>
       <c r="L9">
         <f t="shared" si="0"/>
@@ -8596,11 +8612,11 @@
       </c>
       <c r="M9">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>-5</v>
       </c>
       <c r="N9">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:14">
@@ -8608,35 +8624,35 @@
         <v>100</v>
       </c>
       <c r="B10" s="1">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="C10">
         <f t="shared" si="1"/>
-        <v>-7</v>
+        <v>1</v>
       </c>
       <c r="D10">
         <f t="shared" si="0"/>
-        <v>-2</v>
+        <v>10</v>
       </c>
       <c r="E10">
         <f t="shared" si="0"/>
-        <v>-8</v>
+        <v>10</v>
       </c>
       <c r="F10">
         <f t="shared" si="0"/>
-        <v>-8</v>
+        <v>6</v>
       </c>
       <c r="G10">
         <f t="shared" si="0"/>
-        <v>-8</v>
+        <v>3</v>
       </c>
       <c r="H10">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="I10">
         <f t="shared" si="0"/>
-        <v>-5</v>
+        <v>6</v>
       </c>
       <c r="J10">
         <f t="shared" si="0"/>
@@ -8644,19 +8660,19 @@
       </c>
       <c r="K10">
         <f t="shared" si="0"/>
-        <v>-11</v>
+        <v>1</v>
       </c>
       <c r="L10">
         <f t="shared" si="0"/>
-        <v>-10</v>
+        <v>1</v>
       </c>
       <c r="M10">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N10">
         <f t="shared" si="0"/>
-        <v>-2</v>
+        <v>7</v>
       </c>
     </row>
     <row r="11" spans="1:14">
@@ -8664,11 +8680,11 @@
         <v>101</v>
       </c>
       <c r="B11" s="1">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C11">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D11">
         <f t="shared" si="0"/>
@@ -8676,43 +8692,43 @@
       </c>
       <c r="E11">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="F11">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="G11">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H11">
         <f t="shared" si="0"/>
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="I11">
         <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="J11">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+      <c r="K11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N11">
+        <f t="shared" si="0"/>
         <v>6</v>
-      </c>
-      <c r="J11">
-        <f t="shared" si="0"/>
-        <v>11</v>
-      </c>
-      <c r="K11">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="L11">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="M11">
-        <f t="shared" si="0"/>
-        <v>11</v>
-      </c>
-      <c r="N11">
-        <f t="shared" si="0"/>
-        <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:14">
@@ -8724,24 +8740,24 @@
       </c>
       <c r="C12">
         <f t="shared" si="1"/>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D12">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E12">
         <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="F12">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="G12">
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="F12">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="G12">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
       <c r="H12">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -8752,11 +8768,11 @@
       </c>
       <c r="J12">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>-1</v>
       </c>
       <c r="K12">
         <f t="shared" si="0"/>
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="L12">
         <f t="shared" si="0"/>
@@ -8764,11 +8780,11 @@
       </c>
       <c r="M12">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="N12">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="13" spans="1:14">
@@ -8776,47 +8792,47 @@
         <v>103</v>
       </c>
       <c r="B13" s="1">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="C13">
         <f t="shared" si="1"/>
-        <v>-7</v>
+        <v>0</v>
       </c>
       <c r="D13">
         <f t="shared" si="0"/>
-        <v>-2</v>
+        <v>9</v>
       </c>
       <c r="E13">
         <f t="shared" si="0"/>
-        <v>-8</v>
+        <v>9</v>
       </c>
       <c r="F13">
         <f t="shared" si="0"/>
-        <v>-8</v>
+        <v>5</v>
       </c>
       <c r="G13">
         <f t="shared" si="0"/>
-        <v>-8</v>
+        <v>2</v>
       </c>
       <c r="H13">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="I13">
         <f t="shared" si="0"/>
-        <v>-5</v>
+        <v>5</v>
       </c>
       <c r="J13">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="K13">
         <f t="shared" si="0"/>
-        <v>-11</v>
+        <v>0</v>
       </c>
       <c r="L13">
         <f t="shared" si="0"/>
-        <v>-10</v>
+        <v>0</v>
       </c>
       <c r="M13">
         <f t="shared" si="0"/>
@@ -8824,7 +8840,7 @@
       </c>
       <c r="N13">
         <f t="shared" si="0"/>
-        <v>-2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="14" spans="1:14">
@@ -8832,51 +8848,51 @@
         <v>17</v>
       </c>
       <c r="B14" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C14">
         <f t="shared" si="1"/>
-        <v>-5</v>
+        <v>-6</v>
       </c>
       <c r="D14">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E14">
         <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="F14">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+      <c r="G14">
+        <f t="shared" si="0"/>
+        <v>-4</v>
+      </c>
+      <c r="H14">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="I14">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+      <c r="J14">
+        <f t="shared" si="0"/>
+        <v>-7</v>
+      </c>
+      <c r="K14">
+        <f t="shared" si="0"/>
         <v>-6</v>
       </c>
-      <c r="F14">
+      <c r="L14">
         <f t="shared" si="0"/>
         <v>-6</v>
       </c>
-      <c r="G14">
+      <c r="M14">
         <f t="shared" si="0"/>
         <v>-6</v>
-      </c>
-      <c r="H14">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="I14">
-        <f t="shared" si="0"/>
-        <v>-3</v>
-      </c>
-      <c r="J14">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="K14">
-        <f t="shared" si="0"/>
-        <v>-9</v>
-      </c>
-      <c r="L14">
-        <f t="shared" si="0"/>
-        <v>-8</v>
-      </c>
-      <c r="M14">
-        <f t="shared" si="0"/>
-        <v>2</v>
       </c>
       <c r="N14">
         <f t="shared" si="0"/>
@@ -8946,7 +8962,7 @@
       </c>
       <c r="G17">
         <f>G3*Shared_Lines!F2</f>
-        <v>-1</v>
+        <v>2</v>
       </c>
       <c r="H17">
         <f>H3*Shared_Lines!G2</f>
@@ -8962,7 +8978,7 @@
       </c>
       <c r="K17">
         <f>K3*Shared_Lines!J2</f>
-        <v>-4</v>
+        <v>0</v>
       </c>
       <c r="L17">
         <f>L3*Shared_Lines!K2</f>
@@ -8970,7 +8986,7 @@
       </c>
       <c r="M17">
         <f>M3*Shared_Lines!L2</f>
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="N17">
         <f>N3*Shared_Lines!M2</f>
@@ -9003,7 +9019,7 @@
       </c>
       <c r="H18">
         <f>H4*Shared_Lines!G3</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I18">
         <f>I4*Shared_Lines!H3</f>
@@ -9019,7 +9035,7 @@
       </c>
       <c r="L18">
         <f>L4*Shared_Lines!K3</f>
-        <v>-8</v>
+        <v>-9</v>
       </c>
       <c r="M18">
         <f>M4*Shared_Lines!L3</f>
@@ -9027,7 +9043,7 @@
       </c>
       <c r="N18">
         <f>N4*Shared_Lines!M3</f>
-        <v>0</v>
+        <v>-3</v>
       </c>
     </row>
     <row r="19" spans="2:14">
@@ -9076,7 +9092,7 @@
       </c>
       <c r="M19">
         <f>M5*Shared_Lines!L4</f>
-        <v>8</v>
+        <v>-9</v>
       </c>
       <c r="N19">
         <f>N5*Shared_Lines!M4</f>
@@ -9133,7 +9149,7 @@
       </c>
       <c r="N20">
         <f>N6*Shared_Lines!M5</f>
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="2:14">
@@ -9174,7 +9190,7 @@
       </c>
       <c r="K21">
         <f>K7*Shared_Lines!J6</f>
-        <v>-3</v>
+        <v>-2</v>
       </c>
       <c r="L21">
         <f>L7*Shared_Lines!K6</f>
@@ -10252,8 +10268,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N67"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="D49" sqref="D49"/>
+    <sheetView topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="J58" sqref="J58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -11620,7 +11636,7 @@
         <v>0</v>
       </c>
       <c r="J46">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="K46">
         <v>37</v>
@@ -11938,7 +11954,8 @@
         <v>0</v>
       </c>
       <c r="J53">
-        <v>36</v>
+        <f>J38</f>
+        <v>38</v>
       </c>
       <c r="K53">
         <v>35</v>
@@ -12091,7 +12108,7 @@
       </c>
       <c r="J58">
         <f t="shared" si="1"/>
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="K58">
         <f t="shared" si="1"/>
@@ -12118,9 +12135,9 @@
         <f t="shared" si="2"/>
         <v>36</v>
       </c>
-      <c r="D59" t="str">
-        <f t="shared" si="2"/>
-        <v>-</v>
+      <c r="D59">
+        <f>I4-J59</f>
+        <v>13</v>
       </c>
       <c r="E59" t="str">
         <f t="shared" si="2"/>
@@ -12460,8 +12477,8 @@
         <v>-</v>
       </c>
       <c r="J65">
-        <f t="shared" si="8"/>
-        <v>36</v>
+        <f>J53+I41</f>
+        <v>38</v>
       </c>
       <c r="K65">
         <f t="shared" si="8"/>
@@ -12497,7 +12514,7 @@
   <dimension ref="A1:M10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -12613,7 +12630,7 @@
         <v>0</v>
       </c>
       <c r="J3">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="K3">
         <v>37</v>
@@ -12635,8 +12652,8 @@
       <c r="C4">
         <v>36</v>
       </c>
-      <c r="D4" t="s">
-        <v>0</v>
+      <c r="D4">
+        <v>13</v>
       </c>
       <c r="E4" t="s">
         <v>0</v>
@@ -12900,7 +12917,7 @@
         <v>0</v>
       </c>
       <c r="J10">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="K10">
         <v>35</v>
@@ -12928,7 +12945,7 @@
   <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F33" sqref="F33"/>
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -13039,8 +13056,8 @@
       <c r="C4">
         <v>3</v>
       </c>
-      <c r="D4" t="s">
-        <v>0</v>
+      <c r="D4">
+        <v>13</v>
       </c>
       <c r="E4">
         <v>22</v>
@@ -13229,7 +13246,7 @@
         <v>0</v>
       </c>
       <c r="C10">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="D10">
         <v>40</v>
@@ -13250,7 +13267,7 @@
         <v>0</v>
       </c>
       <c r="J10">
-        <v>36</v>
+        <v>38</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -13365,7 +13382,7 @@
   <dimension ref="A1:M23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D13" sqref="D13:H23"/>
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -13481,7 +13498,7 @@
         <v>0</v>
       </c>
       <c r="J3">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="K3">
         <v>37</v>
@@ -13503,8 +13520,8 @@
       <c r="C4">
         <v>36</v>
       </c>
-      <c r="D4" t="s">
-        <v>0</v>
+      <c r="D4">
+        <v>13</v>
       </c>
       <c r="E4" t="s">
         <v>0</v>
@@ -13768,7 +13785,7 @@
         <v>0</v>
       </c>
       <c r="J10">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="K10">
         <v>35</v>
@@ -13972,11 +13989,11 @@
         <v>35</v>
       </c>
       <c r="G19">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="H19">
         <f t="shared" si="2"/>
-        <v>-1</v>
+        <v>-3</v>
       </c>
     </row>
     <row r="20" spans="1:8">
@@ -14638,7 +14655,7 @@
   <dimension ref="A1:M13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L4" sqref="L4"/>
+      <selection activeCell="M4" sqref="M4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -14763,7 +14780,7 @@
         <v>0</v>
       </c>
       <c r="M3">
-        <v>-1</v>
+        <v>-3</v>
       </c>
     </row>
     <row r="4" spans="1:13">

</xml_diff>